<commit_message>
Syncing to Pull from Master, then Journey's branch
</commit_message>
<xml_diff>
--- a/SetupSheets.xlsx
+++ b/SetupSheets.xlsx
@@ -1442,10 +1442,10 @@
   <dimension ref="A1:CU50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="N6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="T6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="AA7" sqref="AA7"/>
+      <selection pane="bottomRight" activeCell="AA9" sqref="AA9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2842,7 +2842,7 @@
         <v>-2.9000000000000001E-2</v>
       </c>
       <c r="CE6" s="49">
-        <v>2015</v>
+        <v>2592</v>
       </c>
       <c r="CF6" s="49">
         <v>2.3289999999999999E-3</v>
@@ -3125,7 +3125,7 @@
         <v>-0.45</v>
       </c>
       <c r="CE7" s="49">
-        <v>2015</v>
+        <v>2592</v>
       </c>
       <c r="CF7" s="49">
         <v>2.3289999999999999E-3</v>
@@ -3408,7 +3408,7 @@
         <v>-0.89</v>
       </c>
       <c r="CE8" s="49">
-        <v>2015</v>
+        <v>2592</v>
       </c>
       <c r="CF8" s="49">
         <v>2.3289999999999999E-3</v>
@@ -7029,19 +7029,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="11267" r:id="rId4" name="SetDateTimeMain">
+        <control shapeId="11265" r:id="rId4" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>12700</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -7049,7 +7049,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="11267" r:id="rId4" name="SetDateTimeMain"/>
+        <control shapeId="11265" r:id="rId4" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -7079,19 +7079,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="11265" r:id="rId8" name="SetDateTimeRef">
+        <control shapeId="11267" r:id="rId8" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>12700</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -7099,7 +7099,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="11265" r:id="rId8" name="SetDateTimeRef"/>
+        <control shapeId="11267" r:id="rId8" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -10974,19 +10974,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain">
+        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>12700</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -10994,7 +10994,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain"/>
+        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11024,19 +11024,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef">
+        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>12700</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -11044,7 +11044,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef"/>
+        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
2015 Fuel map uploaded
</commit_message>
<xml_diff>
--- a/SetupSheets.xlsx
+++ b/SetupSheets.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Code\LapSimCombined\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Journey\Documents\GitHub\LapSimCombined\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1815" yWindow="540" windowWidth="9705" windowHeight="3240" activeTab="1"/>
+    <workbookView xWindow="1820" yWindow="540" windowWidth="9710" windowHeight="3240"/>
   </bookViews>
   <sheets>
     <sheet name="Combustion" sheetId="11" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="119">
   <si>
     <t>Date</t>
   </si>
@@ -368,6 +368,15 @@
   </si>
   <si>
     <t>Wf</t>
+  </si>
+  <si>
+    <t>[kwh] or L</t>
+  </si>
+  <si>
+    <t>L/s</t>
+  </si>
+  <si>
+    <t>num2str(CalPolySLO)</t>
   </si>
 </sst>
 </file>
@@ -520,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -701,6 +710,10 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -751,11 +764,11 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -810,7 +823,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -861,11 +874,11 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -971,11 +984,11 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -1030,7 +1043,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -1081,11 +1094,11 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -1436,39 +1449,39 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:CU50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="BT6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="BA6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="CU6" sqref="CU6"/>
+      <selection pane="bottomRight" activeCell="BC6" sqref="BC6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" style="23" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="33" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="34" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="24" customWidth="1"/>
-    <col min="5" max="25" width="6.85546875" style="23" customWidth="1"/>
-    <col min="26" max="26" width="6.85546875" style="24" customWidth="1"/>
-    <col min="27" max="48" width="6.85546875" style="23" customWidth="1"/>
-    <col min="49" max="49" width="6.85546875" style="24" customWidth="1"/>
-    <col min="50" max="54" width="6.85546875" style="23" customWidth="1"/>
-    <col min="55" max="55" width="10.85546875" style="23" customWidth="1"/>
-    <col min="56" max="56" width="6.85546875" style="24" customWidth="1"/>
-    <col min="57" max="69" width="6.85546875" style="23" customWidth="1"/>
-    <col min="70" max="70" width="6.85546875" style="24" customWidth="1"/>
-    <col min="71" max="76" width="6.85546875" style="23" customWidth="1"/>
-    <col min="77" max="77" width="6.85546875" style="24" customWidth="1"/>
-    <col min="78" max="87" width="6.85546875" style="23" customWidth="1"/>
-    <col min="88" max="88" width="6.85546875" style="24" customWidth="1"/>
-    <col min="89" max="95" width="6.85546875" style="23" customWidth="1"/>
-    <col min="96" max="96" width="6.85546875" style="24" customWidth="1"/>
-    <col min="97" max="99" width="6.85546875" style="23" customWidth="1"/>
-    <col min="100" max="16384" width="9.140625" style="23"/>
+    <col min="2" max="2" width="12.26953125" style="33" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" style="34" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" style="24" customWidth="1"/>
+    <col min="5" max="25" width="6.81640625" style="23" customWidth="1"/>
+    <col min="26" max="26" width="6.81640625" style="24" customWidth="1"/>
+    <col min="27" max="48" width="6.81640625" style="23" customWidth="1"/>
+    <col min="49" max="49" width="6.81640625" style="24" customWidth="1"/>
+    <col min="50" max="54" width="6.81640625" style="23" customWidth="1"/>
+    <col min="55" max="55" width="10.81640625" style="23" customWidth="1"/>
+    <col min="56" max="56" width="6.81640625" style="24" customWidth="1"/>
+    <col min="57" max="69" width="6.81640625" style="23" customWidth="1"/>
+    <col min="70" max="70" width="6.81640625" style="24" customWidth="1"/>
+    <col min="71" max="76" width="6.81640625" style="23" customWidth="1"/>
+    <col min="77" max="77" width="6.81640625" style="24" customWidth="1"/>
+    <col min="78" max="87" width="6.81640625" style="23" customWidth="1"/>
+    <col min="88" max="88" width="6.81640625" style="24" customWidth="1"/>
+    <col min="89" max="95" width="6.81640625" style="23" customWidth="1"/>
+    <col min="96" max="96" width="6.81640625" style="24" customWidth="1"/>
+    <col min="97" max="99" width="6.81640625" style="23" customWidth="1"/>
+    <col min="100" max="16384" width="9.1796875" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" s="25" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:99" s="25" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>35</v>
       </c>
@@ -1763,7 +1776,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:99" s="28" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:99" s="28" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="36"/>
       <c r="B2" s="26" t="s">
         <v>0</v>
@@ -2013,22 +2026,22 @@
       </c>
       <c r="CJ2" s="9"/>
       <c r="CK2" s="11" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="CL2" s="11" t="s">
         <v>38</v>
       </c>
       <c r="CM2" s="42" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="CN2" s="42" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="CO2" s="42" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="CP2" s="42" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="CQ2" s="42" t="s">
         <v>79</v>
@@ -2044,7 +2057,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:99" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:99" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37"/>
       <c r="B3" s="29"/>
       <c r="C3" s="30"/>
@@ -2145,7 +2158,7 @@
       <c r="CT3" s="15"/>
       <c r="CU3" s="15"/>
     </row>
-    <row r="4" spans="1:99" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:99" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="37"/>
       <c r="B4" s="29"/>
       <c r="C4" s="30"/>
@@ -2246,7 +2259,7 @@
       <c r="CT4" s="15"/>
       <c r="CU4" s="15"/>
     </row>
-    <row r="5" spans="1:99" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:99" s="22" customFormat="1" ht="13" x14ac:dyDescent="0.25">
       <c r="A5" s="51" t="s">
         <v>115</v>
       </c>
@@ -2254,248 +2267,248 @@
       <c r="C5" s="30"/>
       <c r="D5" s="21"/>
       <c r="E5" s="43">
-        <f>E3-E4</f>
+        <f t="shared" ref="E5:AE5" si="0">E3-E4</f>
         <v>0</v>
       </c>
       <c r="F5" s="43">
-        <f>F3-F4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G5" s="43">
-        <f>G3-G4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H5" s="43">
-        <f>H3-H4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I5" s="43">
-        <f>I3-I4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J5" s="43">
-        <f>J3-J4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K5" s="43">
-        <f>K3-K4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L5" s="43">
-        <f>L3-L4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M5" s="43">
-        <f>M3-M4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N5" s="43">
-        <f>N3-N4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O5" s="43">
-        <f>O3-O4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P5" s="43">
-        <f>P3-P4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q5" s="43">
-        <f>Q3-Q4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R5" s="43">
-        <f>R3-R4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S5" s="43">
-        <f>S3-S4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T5" s="43">
-        <f>T3-T4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U5" s="43">
-        <f>U3-U4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="V5" s="43">
-        <f>V3-V4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W5" s="43">
-        <f>W3-W4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X5" s="43">
-        <f>X3-X4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Y5" s="43">
-        <f>Y3-Y4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Z5" s="21">
-        <f>Z3-Z4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AA5" s="43">
-        <f>AA3-AA4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB5" s="43">
-        <f>AB3-AB4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AC5" s="43">
-        <f>AC3-AC4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD5" s="43">
-        <f>AD3-AD4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AE5" s="43">
-        <f>AE3-AE4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AF5" s="43"/>
       <c r="AG5" s="43">
-        <f>AG3-AG4</f>
+        <f t="shared" ref="AG5:BN5" si="1">AG3-AG4</f>
         <v>0</v>
       </c>
       <c r="AH5" s="43">
-        <f>AH3-AH4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI5" s="43">
-        <f>AI3-AI4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AJ5" s="43">
-        <f>AJ3-AJ4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AK5" s="43">
-        <f>AK3-AK4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AL5" s="43">
-        <f>AL3-AL4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AM5" s="43">
-        <f>AM3-AM4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AN5" s="43">
-        <f>AN3-AN4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AO5" s="43">
-        <f>AO3-AO4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AP5" s="43">
-        <f>AP3-AP4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AQ5" s="43">
-        <f>AQ3-AQ4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AR5" s="43">
-        <f>AR3-AR4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AS5" s="43">
-        <f>AS3-AS4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AT5" s="43">
-        <f>AT3-AT4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU5" s="43">
-        <f>AU3-AU4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AV5" s="43">
-        <f>AV3-AV4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AW5" s="21">
-        <f>AW3-AW4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AX5" s="43">
-        <f>AX3-AX4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AY5" s="43">
-        <f>AY3-AY4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AZ5" s="43">
-        <f>AZ3-AZ4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BA5" s="43">
-        <f>BA3-BA4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BB5" s="43">
-        <f>BB3-BB4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BC5" s="43">
-        <f>BC3-BC4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BD5" s="21">
-        <f>BD3-BD4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BE5" s="43">
-        <f>BE3-BE4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BF5" s="43">
-        <f>BF3-BF4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BG5" s="43">
-        <f>BG3-BG4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BH5" s="43">
-        <f>BH3-BH4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BI5" s="43">
-        <f>BI3-BI4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BJ5" s="43">
-        <f>BJ3-BJ4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BK5" s="43">
-        <f>BK3-BK4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BL5" s="43">
-        <f>BL3-BL4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BM5" s="43">
-        <f>BM3-BM4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BN5" s="43">
-        <f>BN3-BN4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BO5" s="43"/>
@@ -2523,27 +2536,27 @@
       <c r="BV5" s="43"/>
       <c r="BW5" s="43"/>
       <c r="BX5" s="43">
-        <f>BX3-BX4</f>
+        <f t="shared" ref="BX5:CC5" si="2">BX3-BX4</f>
         <v>0</v>
       </c>
       <c r="BY5" s="21">
-        <f>BY3-BY4</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BZ5" s="43">
-        <f>BZ3-BZ4</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CA5" s="43">
-        <f>CA3-CA4</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CB5" s="43">
-        <f>CB3-CB4</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CC5" s="43">
-        <f>CC3-CC4</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CD5" s="43"/>
@@ -2556,31 +2569,31 @@
       <c r="CH5" s="43"/>
       <c r="CI5" s="43"/>
       <c r="CJ5" s="21">
-        <f>CJ3-CJ4</f>
+        <f t="shared" ref="CJ5:CP5" si="3">CJ3-CJ4</f>
         <v>0</v>
       </c>
       <c r="CK5" s="43">
-        <f>CK3-CK4</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CL5" s="43">
-        <f>CL3-CL4</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CM5" s="43">
-        <f>CM3-CM4</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CN5" s="43">
-        <f>CN3-CN4</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CO5" s="43">
-        <f>CO3-CO4</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CP5" s="43">
-        <f>CP3-CP4</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CQ5" s="43"/>
@@ -2601,7 +2614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:99" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:99" s="50" customFormat="1" ht="25" x14ac:dyDescent="0.25">
       <c r="A6" s="49">
         <v>0</v>
       </c>
@@ -2758,8 +2771,8 @@
       <c r="BB6" s="45">
         <v>70.396699999999996</v>
       </c>
-      <c r="BC6" s="45">
-        <v>0</v>
+      <c r="BC6" s="52" t="s">
+        <v>118</v>
       </c>
       <c r="BD6" s="45"/>
       <c r="BE6" s="45">
@@ -2853,604 +2866,240 @@
       </c>
       <c r="CJ6" s="45"/>
       <c r="CK6" s="45">
-        <v>0.7</v>
+        <v>3.984</v>
       </c>
       <c r="CL6" s="45">
-        <v>0</v>
+        <v>6.56</v>
       </c>
       <c r="CM6" s="45">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="CN6" s="45">
-        <v>0</v>
+        <v>8.9789999999999998E-4</v>
       </c>
       <c r="CO6" s="45">
-        <v>0</v>
+        <v>8.9789999999999998E-4</v>
       </c>
       <c r="CP6" s="45">
-        <v>0</v>
+        <v>8.9789999999999998E-4</v>
       </c>
       <c r="CQ6" s="45">
         <v>0</v>
       </c>
       <c r="CR6" s="45"/>
       <c r="CS6" s="45">
-        <v>280</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="CT6" s="45">
-        <v>9900</v>
+        <v>9000</v>
       </c>
       <c r="CU6" s="45">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:99" x14ac:dyDescent="0.2">
-      <c r="A7" s="49">
-        <v>1</v>
-      </c>
-      <c r="B7" s="48">
-        <v>1</v>
-      </c>
-      <c r="C7" s="47">
-        <v>4.1666666666666699E-2</v>
-      </c>
+    <row r="7" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="A7" s="49"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="47"/>
       <c r="D7" s="45"/>
-      <c r="E7" s="45">
-        <v>63</v>
-      </c>
-      <c r="F7" s="45">
-        <v>47</v>
-      </c>
-      <c r="G7" s="45">
-        <v>46</v>
-      </c>
-      <c r="H7" s="45">
-        <v>0</v>
-      </c>
-      <c r="I7" s="45">
-        <v>0</v>
-      </c>
-      <c r="J7" s="45">
-        <v>0</v>
-      </c>
-      <c r="K7" s="45">
-        <v>0</v>
-      </c>
-      <c r="L7" s="45">
-        <v>0</v>
-      </c>
-      <c r="M7" s="45">
-        <v>0</v>
-      </c>
-      <c r="N7" s="45">
-        <v>0</v>
-      </c>
-      <c r="O7" s="45">
-        <v>0</v>
-      </c>
-      <c r="P7" s="45">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="45">
-        <v>0</v>
-      </c>
-      <c r="R7" s="45">
-        <v>33.39</v>
-      </c>
-      <c r="S7" s="45">
-        <v>0</v>
-      </c>
-      <c r="T7" s="46">
-        <v>12</v>
-      </c>
-      <c r="U7" s="45">
-        <v>175</v>
-      </c>
-      <c r="V7" s="45">
-        <v>33.9</v>
-      </c>
-      <c r="W7" s="45">
-        <v>0</v>
-      </c>
-      <c r="X7" s="45">
-        <v>12</v>
-      </c>
-      <c r="Y7" s="45">
-        <v>404</v>
-      </c>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="45"/>
+      <c r="M7" s="45"/>
+      <c r="N7" s="45"/>
+      <c r="O7" s="45"/>
+      <c r="P7" s="45"/>
+      <c r="Q7" s="45"/>
+      <c r="R7" s="45"/>
+      <c r="S7" s="45"/>
+      <c r="T7" s="46"/>
+      <c r="U7" s="45"/>
+      <c r="V7" s="45"/>
+      <c r="W7" s="45"/>
+      <c r="X7" s="45"/>
+      <c r="Y7" s="45"/>
       <c r="Z7" s="45"/>
-      <c r="AA7" s="45">
-        <v>250</v>
-      </c>
-      <c r="AB7" s="45">
-        <v>200</v>
-      </c>
-      <c r="AC7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AD7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AF7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AG7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AH7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AI7" s="45">
-        <v>10.25</v>
-      </c>
-      <c r="AJ7" s="45">
-        <v>10.25</v>
-      </c>
-      <c r="AK7" s="45">
-        <v>-0.25</v>
-      </c>
-      <c r="AL7" s="45">
-        <v>1.9</v>
-      </c>
-      <c r="AM7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AN7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AO7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AP7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AQ7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AR7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AS7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AT7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AU7" s="45">
-        <v>10</v>
-      </c>
-      <c r="AV7" s="45">
-        <v>30</v>
-      </c>
+      <c r="AA7" s="45"/>
+      <c r="AB7" s="45"/>
+      <c r="AC7" s="45"/>
+      <c r="AD7" s="45"/>
+      <c r="AE7" s="45"/>
+      <c r="AF7" s="45"/>
+      <c r="AG7" s="45"/>
+      <c r="AH7" s="45"/>
+      <c r="AI7" s="45"/>
+      <c r="AJ7" s="45"/>
+      <c r="AK7" s="45"/>
+      <c r="AL7" s="45"/>
+      <c r="AM7" s="45"/>
+      <c r="AN7" s="45"/>
+      <c r="AO7" s="45"/>
+      <c r="AP7" s="45"/>
+      <c r="AQ7" s="45"/>
+      <c r="AR7" s="45"/>
+      <c r="AS7" s="45"/>
+      <c r="AT7" s="45"/>
+      <c r="AU7" s="45"/>
+      <c r="AV7" s="45"/>
       <c r="AW7" s="45"/>
-      <c r="AX7" s="45">
-        <v>900</v>
-      </c>
-      <c r="AY7" s="45">
-        <v>10.5</v>
-      </c>
-      <c r="AZ7" s="45">
-        <v>0.03</v>
-      </c>
-      <c r="BA7" s="45">
-        <v>120.628</v>
-      </c>
-      <c r="BB7" s="45">
-        <v>70.396699999999996</v>
-      </c>
-      <c r="BC7" s="45">
-        <v>0</v>
-      </c>
+      <c r="AX7" s="45"/>
+      <c r="AY7" s="45"/>
+      <c r="AZ7" s="45"/>
+      <c r="BA7" s="45"/>
+      <c r="BB7" s="45"/>
+      <c r="BC7" s="45"/>
       <c r="BD7" s="45"/>
-      <c r="BE7" s="45">
-        <v>1</v>
-      </c>
-      <c r="BF7" s="45">
-        <v>2.5</v>
-      </c>
-      <c r="BG7" s="45">
-        <v>2</v>
-      </c>
-      <c r="BH7" s="45">
-        <v>1.62</v>
-      </c>
-      <c r="BI7" s="45">
-        <v>1.333</v>
-      </c>
-      <c r="BJ7" s="45">
-        <v>1.095</v>
-      </c>
-      <c r="BK7" s="45">
-        <v>2.6520000000000001</v>
-      </c>
-      <c r="BL7" s="45">
-        <v>2.714</v>
-      </c>
-      <c r="BM7" s="45">
-        <v>0.9</v>
-      </c>
-      <c r="BN7" s="45">
-        <v>0</v>
-      </c>
-      <c r="BO7" s="45">
-        <v>0</v>
-      </c>
-      <c r="BP7" s="45">
-        <v>0</v>
-      </c>
-      <c r="BQ7" s="45">
-        <v>20</v>
-      </c>
+      <c r="BE7" s="45"/>
+      <c r="BF7" s="45"/>
+      <c r="BG7" s="45"/>
+      <c r="BH7" s="45"/>
+      <c r="BI7" s="45"/>
+      <c r="BJ7" s="45"/>
+      <c r="BK7" s="45"/>
+      <c r="BL7" s="45"/>
+      <c r="BM7" s="45"/>
+      <c r="BN7" s="45"/>
+      <c r="BO7" s="45"/>
+      <c r="BP7" s="45"/>
+      <c r="BQ7" s="45"/>
       <c r="BR7" s="45"/>
-      <c r="BS7" s="45">
-        <v>6762.75</v>
-      </c>
-      <c r="BT7" s="45">
-        <v>3238.5</v>
-      </c>
-      <c r="BU7" s="45">
-        <v>0</v>
-      </c>
-      <c r="BV7" s="45">
-        <v>0</v>
-      </c>
-      <c r="BW7" s="45">
-        <v>0</v>
-      </c>
-      <c r="BX7" s="45">
-        <v>0.96699999999999997</v>
-      </c>
+      <c r="BS7" s="45"/>
+      <c r="BT7" s="45"/>
+      <c r="BU7" s="45"/>
+      <c r="BV7" s="45"/>
+      <c r="BW7" s="45"/>
+      <c r="BX7" s="45"/>
       <c r="BY7" s="45"/>
-      <c r="BZ7" s="45">
-        <v>0</v>
-      </c>
-      <c r="CA7" s="45">
-        <v>0</v>
-      </c>
-      <c r="CB7" s="45">
-        <v>0</v>
-      </c>
-      <c r="CC7" s="45">
-        <v>0.35</v>
-      </c>
-      <c r="CD7" s="45">
-        <v>-0.45</v>
-      </c>
-      <c r="CE7" s="45">
-        <v>2015</v>
-      </c>
-      <c r="CF7" s="45">
-        <v>2.3289999999999999E-3</v>
-      </c>
-      <c r="CG7" s="45">
-        <v>34.25</v>
-      </c>
-      <c r="CH7" s="45">
-        <v>0</v>
-      </c>
-      <c r="CI7" s="45">
-        <v>10</v>
-      </c>
+      <c r="BZ7" s="45"/>
+      <c r="CA7" s="45"/>
+      <c r="CB7" s="45"/>
+      <c r="CC7" s="45"/>
+      <c r="CD7" s="45"/>
+      <c r="CE7" s="45"/>
+      <c r="CF7" s="45"/>
+      <c r="CG7" s="45"/>
+      <c r="CH7" s="45"/>
+      <c r="CI7" s="45"/>
       <c r="CJ7" s="45"/>
-      <c r="CK7" s="45">
-        <v>0.7</v>
-      </c>
-      <c r="CL7" s="45">
-        <v>0</v>
-      </c>
-      <c r="CM7" s="45">
-        <v>0</v>
-      </c>
-      <c r="CN7" s="45">
-        <v>0</v>
-      </c>
-      <c r="CO7" s="45">
-        <v>0</v>
-      </c>
-      <c r="CP7" s="45">
-        <v>0</v>
-      </c>
-      <c r="CQ7" s="45">
-        <v>0</v>
-      </c>
+      <c r="CK7" s="45"/>
+      <c r="CL7" s="45"/>
+      <c r="CM7" s="45"/>
+      <c r="CN7" s="45"/>
+      <c r="CO7" s="45"/>
+      <c r="CP7" s="45"/>
+      <c r="CQ7" s="45"/>
       <c r="CR7" s="45"/>
-      <c r="CS7" s="45">
-        <v>280</v>
-      </c>
-      <c r="CT7" s="45">
-        <v>9900</v>
-      </c>
-      <c r="CU7" s="45">
-        <v>0</v>
-      </c>
+      <c r="CS7" s="45"/>
+      <c r="CT7" s="45"/>
+      <c r="CU7" s="45"/>
     </row>
-    <row r="8" spans="1:99" x14ac:dyDescent="0.2">
-      <c r="A8" s="49">
-        <v>2</v>
-      </c>
-      <c r="B8" s="48">
-        <v>2</v>
-      </c>
-      <c r="C8" s="47">
-        <v>8.3333333333333301E-2</v>
-      </c>
+    <row r="8" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="A8" s="49"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="47"/>
       <c r="D8" s="45"/>
-      <c r="E8" s="45">
-        <v>63</v>
-      </c>
-      <c r="F8" s="45">
-        <v>47</v>
-      </c>
-      <c r="G8" s="45">
-        <v>46</v>
-      </c>
-      <c r="H8" s="45">
-        <v>0</v>
-      </c>
-      <c r="I8" s="45">
-        <v>0</v>
-      </c>
-      <c r="J8" s="45">
-        <v>0</v>
-      </c>
-      <c r="K8" s="45">
-        <v>0</v>
-      </c>
-      <c r="L8" s="45">
-        <v>0</v>
-      </c>
-      <c r="M8" s="45">
-        <v>0</v>
-      </c>
-      <c r="N8" s="45">
-        <v>0</v>
-      </c>
-      <c r="O8" s="45">
-        <v>0</v>
-      </c>
-      <c r="P8" s="45">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="45">
-        <v>0</v>
-      </c>
-      <c r="R8" s="45">
-        <v>33.39</v>
-      </c>
-      <c r="S8" s="45">
-        <v>0</v>
-      </c>
-      <c r="T8" s="46">
-        <v>12</v>
-      </c>
-      <c r="U8" s="45">
-        <v>175</v>
-      </c>
-      <c r="V8" s="45">
-        <v>33.9</v>
-      </c>
-      <c r="W8" s="45">
-        <v>0</v>
-      </c>
-      <c r="X8" s="45">
-        <v>12</v>
-      </c>
-      <c r="Y8" s="45">
-        <v>404</v>
-      </c>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
+      <c r="M8" s="45"/>
+      <c r="N8" s="45"/>
+      <c r="O8" s="45"/>
+      <c r="P8" s="45"/>
+      <c r="Q8" s="45"/>
+      <c r="R8" s="45"/>
+      <c r="S8" s="45"/>
+      <c r="T8" s="46"/>
+      <c r="U8" s="45"/>
+      <c r="V8" s="45"/>
+      <c r="W8" s="45"/>
+      <c r="X8" s="45"/>
+      <c r="Y8" s="45"/>
       <c r="Z8" s="45"/>
-      <c r="AA8" s="45">
-        <v>250</v>
-      </c>
-      <c r="AB8" s="45">
-        <v>200</v>
-      </c>
-      <c r="AC8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AE8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AF8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AG8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AH8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AI8" s="45">
-        <v>10.25</v>
-      </c>
-      <c r="AJ8" s="45">
-        <v>10.25</v>
-      </c>
-      <c r="AK8" s="45">
-        <v>-0.25</v>
-      </c>
-      <c r="AL8" s="45">
-        <v>1.9</v>
-      </c>
-      <c r="AM8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AN8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AO8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AP8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AQ8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AR8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AS8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AT8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AU8" s="45">
-        <v>10</v>
-      </c>
-      <c r="AV8" s="45">
-        <v>30</v>
-      </c>
+      <c r="AA8" s="45"/>
+      <c r="AB8" s="45"/>
+      <c r="AC8" s="45"/>
+      <c r="AD8" s="45"/>
+      <c r="AE8" s="45"/>
+      <c r="AF8" s="45"/>
+      <c r="AG8" s="45"/>
+      <c r="AH8" s="45"/>
+      <c r="AI8" s="45"/>
+      <c r="AJ8" s="45"/>
+      <c r="AK8" s="45"/>
+      <c r="AL8" s="45"/>
+      <c r="AM8" s="45"/>
+      <c r="AN8" s="45"/>
+      <c r="AO8" s="45"/>
+      <c r="AP8" s="45"/>
+      <c r="AQ8" s="45"/>
+      <c r="AR8" s="45"/>
+      <c r="AS8" s="45"/>
+      <c r="AT8" s="45"/>
+      <c r="AU8" s="45"/>
+      <c r="AV8" s="45"/>
       <c r="AW8" s="45"/>
-      <c r="AX8" s="45">
-        <v>900</v>
-      </c>
-      <c r="AY8" s="45">
-        <v>10.5</v>
-      </c>
-      <c r="AZ8" s="45">
-        <v>0.03</v>
-      </c>
-      <c r="BA8" s="45">
-        <v>120.628</v>
-      </c>
-      <c r="BB8" s="45">
-        <v>70.396699999999996</v>
-      </c>
-      <c r="BC8" s="45">
-        <v>0</v>
-      </c>
+      <c r="AX8" s="45"/>
+      <c r="AY8" s="45"/>
+      <c r="AZ8" s="45"/>
+      <c r="BA8" s="45"/>
+      <c r="BB8" s="45"/>
+      <c r="BC8" s="45"/>
       <c r="BD8" s="45"/>
-      <c r="BE8" s="45">
-        <v>1</v>
-      </c>
-      <c r="BF8" s="45">
-        <v>2.5</v>
-      </c>
-      <c r="BG8" s="45">
-        <v>2</v>
-      </c>
-      <c r="BH8" s="45">
-        <v>1.62</v>
-      </c>
-      <c r="BI8" s="45">
-        <v>1.333</v>
-      </c>
-      <c r="BJ8" s="45">
-        <v>1.095</v>
-      </c>
-      <c r="BK8" s="45">
-        <v>2.6520000000000001</v>
-      </c>
-      <c r="BL8" s="45">
-        <v>2.714</v>
-      </c>
-      <c r="BM8" s="45">
-        <v>0.9</v>
-      </c>
-      <c r="BN8" s="45">
-        <v>0</v>
-      </c>
-      <c r="BO8" s="45">
-        <v>0</v>
-      </c>
-      <c r="BP8" s="45">
-        <v>0</v>
-      </c>
-      <c r="BQ8" s="45">
-        <v>20</v>
-      </c>
+      <c r="BE8" s="45"/>
+      <c r="BF8" s="45"/>
+      <c r="BG8" s="45"/>
+      <c r="BH8" s="45"/>
+      <c r="BI8" s="45"/>
+      <c r="BJ8" s="45"/>
+      <c r="BK8" s="45"/>
+      <c r="BL8" s="45"/>
+      <c r="BM8" s="45"/>
+      <c r="BN8" s="45"/>
+      <c r="BO8" s="45"/>
+      <c r="BP8" s="45"/>
+      <c r="BQ8" s="45"/>
       <c r="BR8" s="45"/>
-      <c r="BS8" s="45">
-        <v>6762.75</v>
-      </c>
-      <c r="BT8" s="45">
-        <v>3238.5</v>
-      </c>
-      <c r="BU8" s="45">
-        <v>0</v>
-      </c>
-      <c r="BV8" s="45">
-        <v>0</v>
-      </c>
-      <c r="BW8" s="45">
-        <v>0</v>
-      </c>
-      <c r="BX8" s="45">
-        <v>0.96699999999999997</v>
-      </c>
+      <c r="BS8" s="45"/>
+      <c r="BT8" s="45"/>
+      <c r="BU8" s="45"/>
+      <c r="BV8" s="45"/>
+      <c r="BW8" s="45"/>
+      <c r="BX8" s="45"/>
       <c r="BY8" s="45"/>
-      <c r="BZ8" s="45">
-        <v>0</v>
-      </c>
-      <c r="CA8" s="45">
-        <v>0</v>
-      </c>
-      <c r="CB8" s="45">
-        <v>0</v>
-      </c>
-      <c r="CC8" s="45">
-        <v>0.45</v>
-      </c>
-      <c r="CD8" s="45">
-        <v>-0.89</v>
-      </c>
-      <c r="CE8" s="45">
-        <v>2015</v>
-      </c>
-      <c r="CF8" s="45">
-        <v>2.3289999999999999E-3</v>
-      </c>
-      <c r="CG8" s="45">
-        <v>34.25</v>
-      </c>
-      <c r="CH8" s="45">
-        <v>0</v>
-      </c>
-      <c r="CI8" s="45">
-        <v>10</v>
-      </c>
+      <c r="BZ8" s="45"/>
+      <c r="CA8" s="45"/>
+      <c r="CB8" s="45"/>
+      <c r="CC8" s="45"/>
+      <c r="CD8" s="45"/>
+      <c r="CE8" s="45"/>
+      <c r="CF8" s="45"/>
+      <c r="CG8" s="45"/>
+      <c r="CH8" s="45"/>
+      <c r="CI8" s="45"/>
       <c r="CJ8" s="45"/>
-      <c r="CK8" s="45">
-        <v>0.7</v>
-      </c>
-      <c r="CL8" s="45">
-        <v>0</v>
-      </c>
-      <c r="CM8" s="45">
-        <v>0</v>
-      </c>
-      <c r="CN8" s="45">
-        <v>0</v>
-      </c>
-      <c r="CO8" s="45">
-        <v>0</v>
-      </c>
-      <c r="CP8" s="45">
-        <v>0</v>
-      </c>
-      <c r="CQ8" s="45">
-        <v>0</v>
-      </c>
+      <c r="CK8" s="45"/>
+      <c r="CL8" s="45"/>
+      <c r="CM8" s="45"/>
+      <c r="CN8" s="45"/>
+      <c r="CO8" s="45"/>
+      <c r="CP8" s="45"/>
+      <c r="CQ8" s="45"/>
       <c r="CR8" s="45"/>
-      <c r="CS8" s="45">
-        <v>280</v>
-      </c>
-      <c r="CT8" s="45">
-        <v>9900</v>
-      </c>
-      <c r="CU8" s="45">
-        <v>0</v>
-      </c>
+      <c r="CS8" s="45"/>
+      <c r="CT8" s="45"/>
+      <c r="CU8" s="45"/>
     </row>
-    <row r="9" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A9" s="49"/>
       <c r="B9" s="48"/>
       <c r="C9" s="47"/>
@@ -3551,7 +3200,7 @@
       <c r="CT9" s="45"/>
       <c r="CU9" s="45"/>
     </row>
-    <row r="10" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A10" s="49"/>
       <c r="B10" s="48"/>
       <c r="C10" s="47"/>
@@ -3652,7 +3301,7 @@
       <c r="CT10" s="45"/>
       <c r="CU10" s="45"/>
     </row>
-    <row r="11" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A11" s="49"/>
       <c r="B11" s="48"/>
       <c r="C11" s="47"/>
@@ -3753,7 +3402,7 @@
       <c r="CT11" s="45"/>
       <c r="CU11" s="45"/>
     </row>
-    <row r="12" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A12" s="49"/>
       <c r="B12" s="48"/>
       <c r="C12" s="47"/>
@@ -3854,7 +3503,7 @@
       <c r="CT12" s="45"/>
       <c r="CU12" s="45"/>
     </row>
-    <row r="13" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A13" s="49"/>
       <c r="B13" s="48"/>
       <c r="C13" s="47"/>
@@ -3955,7 +3604,7 @@
       <c r="CT13" s="45"/>
       <c r="CU13" s="45"/>
     </row>
-    <row r="14" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A14" s="49"/>
       <c r="B14" s="48"/>
       <c r="C14" s="47"/>
@@ -4056,7 +3705,7 @@
       <c r="CT14" s="45"/>
       <c r="CU14" s="45"/>
     </row>
-    <row r="15" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A15" s="49"/>
       <c r="B15" s="48"/>
       <c r="C15" s="47"/>
@@ -4157,7 +3806,7 @@
       <c r="CT15" s="45"/>
       <c r="CU15" s="45"/>
     </row>
-    <row r="16" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A16" s="49"/>
       <c r="B16" s="48"/>
       <c r="C16" s="47"/>
@@ -4258,7 +3907,7 @@
       <c r="CT16" s="45"/>
       <c r="CU16" s="45"/>
     </row>
-    <row r="17" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A17" s="49"/>
       <c r="B17" s="48"/>
       <c r="C17" s="47"/>
@@ -4359,7 +4008,7 @@
       <c r="CT17" s="45"/>
       <c r="CU17" s="45"/>
     </row>
-    <row r="18" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A18" s="49"/>
       <c r="B18" s="48"/>
       <c r="C18" s="47"/>
@@ -4460,7 +4109,7 @@
       <c r="CT18" s="45"/>
       <c r="CU18" s="45"/>
     </row>
-    <row r="19" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A19" s="49"/>
       <c r="B19" s="48"/>
       <c r="C19" s="47"/>
@@ -4561,7 +4210,7 @@
       <c r="CT19" s="45"/>
       <c r="CU19" s="45"/>
     </row>
-    <row r="20" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A20" s="49"/>
       <c r="B20" s="48"/>
       <c r="C20" s="47"/>
@@ -4662,7 +4311,7 @@
       <c r="CT20" s="45"/>
       <c r="CU20" s="45"/>
     </row>
-    <row r="21" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A21" s="49"/>
       <c r="B21" s="48"/>
       <c r="C21" s="47"/>
@@ -4763,7 +4412,7 @@
       <c r="CT21" s="45"/>
       <c r="CU21" s="45"/>
     </row>
-    <row r="22" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A22" s="49"/>
       <c r="B22" s="48"/>
       <c r="C22" s="47"/>
@@ -4864,7 +4513,7 @@
       <c r="CT22" s="45"/>
       <c r="CU22" s="45"/>
     </row>
-    <row r="23" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A23" s="49"/>
       <c r="B23" s="48"/>
       <c r="C23" s="47"/>
@@ -4965,7 +4614,7 @@
       <c r="CT23" s="45"/>
       <c r="CU23" s="45"/>
     </row>
-    <row r="24" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A24" s="49"/>
       <c r="B24" s="48"/>
       <c r="C24" s="47"/>
@@ -5066,7 +4715,7 @@
       <c r="CT24" s="45"/>
       <c r="CU24" s="45"/>
     </row>
-    <row r="25" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A25" s="49"/>
       <c r="B25" s="48"/>
       <c r="C25" s="47"/>
@@ -5167,7 +4816,7 @@
       <c r="CT25" s="45"/>
       <c r="CU25" s="45"/>
     </row>
-    <row r="26" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A26" s="49"/>
       <c r="B26" s="48"/>
       <c r="C26" s="47"/>
@@ -5268,7 +4917,7 @@
       <c r="CT26" s="45"/>
       <c r="CU26" s="45"/>
     </row>
-    <row r="27" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A27" s="49"/>
       <c r="B27" s="48"/>
       <c r="C27" s="47"/>
@@ -5369,7 +5018,7 @@
       <c r="CT27" s="45"/>
       <c r="CU27" s="45"/>
     </row>
-    <row r="28" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A28" s="49"/>
       <c r="B28" s="48"/>
       <c r="C28" s="47"/>
@@ -5470,7 +5119,7 @@
       <c r="CT28" s="45"/>
       <c r="CU28" s="45"/>
     </row>
-    <row r="29" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A29" s="49"/>
       <c r="B29" s="48"/>
       <c r="C29" s="47"/>
@@ -5571,7 +5220,7 @@
       <c r="CT29" s="45"/>
       <c r="CU29" s="45"/>
     </row>
-    <row r="30" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A30" s="49"/>
       <c r="B30" s="48"/>
       <c r="C30" s="47"/>
@@ -5672,7 +5321,7 @@
       <c r="CT30" s="45"/>
       <c r="CU30" s="45"/>
     </row>
-    <row r="31" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A31" s="49"/>
       <c r="B31" s="48"/>
       <c r="C31" s="47"/>
@@ -5773,7 +5422,7 @@
       <c r="CT31" s="45"/>
       <c r="CU31" s="45"/>
     </row>
-    <row r="32" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A32" s="49"/>
       <c r="B32" s="48"/>
       <c r="C32" s="47"/>
@@ -5874,7 +5523,7 @@
       <c r="CT32" s="45"/>
       <c r="CU32" s="45"/>
     </row>
-    <row r="33" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A33" s="49"/>
       <c r="B33" s="48"/>
       <c r="C33" s="47"/>
@@ -5975,7 +5624,7 @@
       <c r="CT33" s="45"/>
       <c r="CU33" s="45"/>
     </row>
-    <row r="34" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A34" s="49"/>
       <c r="B34" s="48"/>
       <c r="C34" s="47"/>
@@ -6076,7 +5725,7 @@
       <c r="CT34" s="45"/>
       <c r="CU34" s="45"/>
     </row>
-    <row r="35" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A35" s="49"/>
       <c r="B35" s="48"/>
       <c r="C35" s="47"/>
@@ -6177,7 +5826,7 @@
       <c r="CT35" s="45"/>
       <c r="CU35" s="45"/>
     </row>
-    <row r="36" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A36" s="49"/>
       <c r="B36" s="48"/>
       <c r="C36" s="47"/>
@@ -6278,7 +5927,7 @@
       <c r="CT36" s="45"/>
       <c r="CU36" s="45"/>
     </row>
-    <row r="37" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A37" s="49"/>
       <c r="B37" s="48"/>
       <c r="C37" s="47"/>
@@ -6379,7 +6028,7 @@
       <c r="CT37" s="45"/>
       <c r="CU37" s="45"/>
     </row>
-    <row r="38" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A38" s="49"/>
       <c r="B38" s="48"/>
       <c r="C38" s="47"/>
@@ -6480,7 +6129,7 @@
       <c r="CT38" s="45"/>
       <c r="CU38" s="45"/>
     </row>
-    <row r="39" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A39" s="49"/>
       <c r="B39" s="48"/>
       <c r="C39" s="47"/>
@@ -6581,7 +6230,7 @@
       <c r="CT39" s="45"/>
       <c r="CU39" s="45"/>
     </row>
-    <row r="40" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A40" s="49"/>
       <c r="B40" s="48"/>
       <c r="C40" s="47"/>
@@ -6682,7 +6331,7 @@
       <c r="CT40" s="45"/>
       <c r="CU40" s="45"/>
     </row>
-    <row r="41" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A41" s="49"/>
       <c r="B41" s="48"/>
       <c r="C41" s="47"/>
@@ -6783,7 +6432,7 @@
       <c r="CT41" s="45"/>
       <c r="CU41" s="45"/>
     </row>
-    <row r="42" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A42" s="49"/>
       <c r="B42" s="48"/>
       <c r="C42" s="47"/>
@@ -6884,7 +6533,7 @@
       <c r="CT42" s="45"/>
       <c r="CU42" s="45"/>
     </row>
-    <row r="43" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A43" s="49"/>
       <c r="B43" s="48"/>
       <c r="C43" s="47"/>
@@ -6985,31 +6634,31 @@
       <c r="CT43" s="45"/>
       <c r="CU43" s="45"/>
     </row>
-    <row r="44" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B44" s="31"/>
       <c r="C44" s="32"/>
     </row>
-    <row r="45" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B45" s="31"/>
       <c r="C45" s="32"/>
     </row>
-    <row r="46" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B46" s="31"/>
       <c r="C46" s="32"/>
     </row>
-    <row r="47" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B47" s="31"/>
       <c r="C47" s="32"/>
     </row>
-    <row r="48" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B48" s="31"/>
       <c r="C48" s="32"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="31"/>
       <c r="C49" s="32"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="31"/>
       <c r="C50" s="32"/>
     </row>
@@ -7024,19 +6673,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="11267" r:id="rId4" name="SetDateTimeMain">
+        <control shapeId="11265" r:id="rId4" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>12700</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:colOff>12700</xdr:colOff>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -7044,7 +6693,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="11267" r:id="rId4" name="SetDateTimeMain"/>
+        <control shapeId="11265" r:id="rId4" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -7060,7 +6709,7 @@
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:colOff>12700</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
@@ -7074,19 +6723,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="11265" r:id="rId8" name="SetDateTimeRef">
+        <control shapeId="11267" r:id="rId8" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" autoPict="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>12700</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:colOff>12700</xdr:colOff>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -7094,7 +6743,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="11265" r:id="rId8" name="SetDateTimeRef"/>
+        <control shapeId="11267" r:id="rId8" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -7106,39 +6755,39 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:CU50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="5" topLeftCell="CD6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="CU6" sqref="CU6"/>
+      <selection pane="bottomRight" activeCell="CE9" sqref="CE9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" style="23" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="33" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="34" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="24" customWidth="1"/>
-    <col min="5" max="25" width="6.85546875" style="23" customWidth="1"/>
-    <col min="26" max="26" width="6.85546875" style="24" customWidth="1"/>
-    <col min="27" max="48" width="6.85546875" style="23" customWidth="1"/>
-    <col min="49" max="49" width="6.85546875" style="24" customWidth="1"/>
-    <col min="50" max="54" width="6.85546875" style="23" customWidth="1"/>
-    <col min="55" max="55" width="10.85546875" style="23" customWidth="1"/>
-    <col min="56" max="56" width="6.85546875" style="24" customWidth="1"/>
-    <col min="57" max="69" width="6.85546875" style="23" customWidth="1"/>
-    <col min="70" max="70" width="6.85546875" style="24" customWidth="1"/>
-    <col min="71" max="76" width="6.85546875" style="23" customWidth="1"/>
-    <col min="77" max="77" width="6.85546875" style="24" customWidth="1"/>
-    <col min="78" max="87" width="6.85546875" style="23" customWidth="1"/>
-    <col min="88" max="88" width="6.85546875" style="24" customWidth="1"/>
-    <col min="89" max="95" width="6.85546875" style="23" customWidth="1"/>
-    <col min="96" max="96" width="6.85546875" style="24" customWidth="1"/>
-    <col min="97" max="99" width="6.85546875" style="23" customWidth="1"/>
-    <col min="100" max="16384" width="9.140625" style="23"/>
+    <col min="2" max="2" width="12.26953125" style="33" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" style="34" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" style="24" customWidth="1"/>
+    <col min="5" max="25" width="6.81640625" style="23" customWidth="1"/>
+    <col min="26" max="26" width="6.81640625" style="24" customWidth="1"/>
+    <col min="27" max="48" width="6.81640625" style="23" customWidth="1"/>
+    <col min="49" max="49" width="6.81640625" style="24" customWidth="1"/>
+    <col min="50" max="54" width="6.81640625" style="23" customWidth="1"/>
+    <col min="55" max="55" width="10.81640625" style="23" customWidth="1"/>
+    <col min="56" max="56" width="6.81640625" style="24" customWidth="1"/>
+    <col min="57" max="69" width="6.81640625" style="23" customWidth="1"/>
+    <col min="70" max="70" width="6.81640625" style="24" customWidth="1"/>
+    <col min="71" max="76" width="6.81640625" style="23" customWidth="1"/>
+    <col min="77" max="77" width="6.81640625" style="24" customWidth="1"/>
+    <col min="78" max="87" width="6.81640625" style="23" customWidth="1"/>
+    <col min="88" max="88" width="6.81640625" style="24" customWidth="1"/>
+    <col min="89" max="95" width="6.81640625" style="23" customWidth="1"/>
+    <col min="96" max="96" width="6.81640625" style="24" customWidth="1"/>
+    <col min="97" max="99" width="6.81640625" style="23" customWidth="1"/>
+    <col min="100" max="16384" width="9.1796875" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" s="25" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:99" s="25" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>35</v>
       </c>
@@ -7433,7 +7082,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:99" s="28" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:99" s="28" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="36"/>
       <c r="B2" s="26" t="s">
         <v>0</v>
@@ -7714,7 +7363,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:99" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:99" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37"/>
       <c r="B3" s="29"/>
       <c r="C3" s="30"/>
@@ -7815,7 +7464,7 @@
       <c r="CT3" s="15"/>
       <c r="CU3" s="15"/>
     </row>
-    <row r="4" spans="1:99" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:99" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="37"/>
       <c r="B4" s="29"/>
       <c r="C4" s="30"/>
@@ -7916,7 +7565,7 @@
       <c r="CT4" s="15"/>
       <c r="CU4" s="15"/>
     </row>
-    <row r="5" spans="1:99" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:99" s="22" customFormat="1" ht="13" x14ac:dyDescent="0.25">
       <c r="A5" s="37" t="s">
         <v>36</v>
       </c>
@@ -8271,7 +7920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:99" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:99" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="1">
         <v>35065</v>
@@ -8554,7 +8203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:99" ht="13" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="1"/>
       <c r="C7" s="8"/>
@@ -8655,7 +8304,7 @@
       <c r="CT7" s="18"/>
       <c r="CU7" s="18"/>
     </row>
-    <row r="8" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
       <c r="B8" s="1"/>
       <c r="C8" s="8"/>
@@ -8755,7 +8404,7 @@
       <c r="CT8" s="18"/>
       <c r="CU8" s="18"/>
     </row>
-    <row r="9" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="B9" s="1"/>
       <c r="C9" s="8"/>
@@ -8856,7 +8505,7 @@
       <c r="CT9" s="18"/>
       <c r="CU9" s="18"/>
     </row>
-    <row r="10" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
       <c r="B10" s="1"/>
       <c r="C10" s="8"/>
@@ -8957,7 +8606,7 @@
       <c r="CT10" s="18"/>
       <c r="CU10" s="18"/>
     </row>
-    <row r="11" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A11" s="19"/>
       <c r="B11" s="1"/>
       <c r="C11" s="8"/>
@@ -9058,7 +8707,7 @@
       <c r="CT11" s="18"/>
       <c r="CU11" s="18"/>
     </row>
-    <row r="12" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A12" s="19"/>
       <c r="B12" s="1"/>
       <c r="C12" s="8"/>
@@ -9159,7 +8808,7 @@
       <c r="CT12" s="18"/>
       <c r="CU12" s="18"/>
     </row>
-    <row r="13" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
       <c r="B13" s="1"/>
       <c r="C13" s="8"/>
@@ -9260,7 +8909,7 @@
       <c r="CT13" s="18"/>
       <c r="CU13" s="18"/>
     </row>
-    <row r="14" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A14" s="19"/>
       <c r="B14" s="1"/>
       <c r="C14" s="8"/>
@@ -9361,7 +9010,7 @@
       <c r="CT14" s="18"/>
       <c r="CU14" s="18"/>
     </row>
-    <row r="15" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
       <c r="B15" s="1"/>
       <c r="C15" s="8"/>
@@ -9462,7 +9111,7 @@
       <c r="CT15" s="18"/>
       <c r="CU15" s="18"/>
     </row>
-    <row r="16" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
       <c r="B16" s="1"/>
       <c r="C16" s="8"/>
@@ -9563,7 +9212,7 @@
       <c r="CT16" s="18"/>
       <c r="CU16" s="18"/>
     </row>
-    <row r="17" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
       <c r="B17" s="1"/>
       <c r="C17" s="8"/>
@@ -9664,7 +9313,7 @@
       <c r="CT17" s="18"/>
       <c r="CU17" s="18"/>
     </row>
-    <row r="18" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18" s="1"/>
       <c r="C18" s="8"/>
@@ -9765,7 +9414,7 @@
       <c r="CT18" s="18"/>
       <c r="CU18" s="18"/>
     </row>
-    <row r="19" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
       <c r="B19" s="1"/>
       <c r="C19" s="8"/>
@@ -9866,7 +9515,7 @@
       <c r="CT19" s="18"/>
       <c r="CU19" s="18"/>
     </row>
-    <row r="20" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
       <c r="B20" s="1"/>
       <c r="C20" s="8"/>
@@ -9967,7 +9616,7 @@
       <c r="CT20" s="18"/>
       <c r="CU20" s="18"/>
     </row>
-    <row r="21" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
       <c r="B21" s="1"/>
       <c r="C21" s="8"/>
@@ -10068,7 +9717,7 @@
       <c r="CT21" s="18"/>
       <c r="CU21" s="18"/>
     </row>
-    <row r="22" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
       <c r="B22" s="1"/>
       <c r="C22" s="8"/>
@@ -10169,7 +9818,7 @@
       <c r="CT22" s="18"/>
       <c r="CU22" s="18"/>
     </row>
-    <row r="23" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
       <c r="B23" s="1"/>
       <c r="C23" s="8"/>
@@ -10270,7 +9919,7 @@
       <c r="CT23" s="18"/>
       <c r="CU23" s="18"/>
     </row>
-    <row r="24" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24" s="1"/>
       <c r="C24" s="8"/>
@@ -10371,7 +10020,7 @@
       <c r="CT24" s="18"/>
       <c r="CU24" s="18"/>
     </row>
-    <row r="25" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
       <c r="B25" s="1"/>
       <c r="C25" s="8"/>
@@ -10472,7 +10121,7 @@
       <c r="CT25" s="18"/>
       <c r="CU25" s="18"/>
     </row>
-    <row r="26" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="B26" s="1"/>
       <c r="C26" s="8"/>
@@ -10573,7 +10222,7 @@
       <c r="CT26" s="18"/>
       <c r="CU26" s="18"/>
     </row>
-    <row r="27" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
       <c r="B27" s="1"/>
       <c r="C27" s="8"/>
@@ -10674,7 +10323,7 @@
       <c r="CT27" s="18"/>
       <c r="CU27" s="18"/>
     </row>
-    <row r="28" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
       <c r="B28" s="1"/>
       <c r="C28" s="8"/>
@@ -10775,7 +10424,7 @@
       <c r="CT28" s="18"/>
       <c r="CU28" s="18"/>
     </row>
-    <row r="29" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
       <c r="B29" s="1"/>
       <c r="C29" s="8"/>
@@ -10876,87 +10525,87 @@
       <c r="CT29" s="18"/>
       <c r="CU29" s="18"/>
     </row>
-    <row r="30" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B30" s="31"/>
       <c r="C30" s="32"/>
     </row>
-    <row r="31" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B31" s="31"/>
       <c r="C31" s="32"/>
     </row>
-    <row r="32" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B32" s="31"/>
       <c r="C32" s="32"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="31"/>
       <c r="C33" s="32"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="31"/>
       <c r="C34" s="32"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="31"/>
       <c r="C35" s="32"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="31"/>
       <c r="C36" s="32"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="31"/>
       <c r="C37" s="32"/>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="31"/>
       <c r="C38" s="32"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="31"/>
       <c r="C39" s="32"/>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="31"/>
       <c r="C40" s="32"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="31"/>
       <c r="C41" s="32"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="31"/>
       <c r="C42" s="32"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" s="31"/>
       <c r="C43" s="32"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" s="31"/>
       <c r="C44" s="32"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" s="31"/>
       <c r="C45" s="32"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" s="31"/>
       <c r="C46" s="32"/>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" s="31"/>
       <c r="C47" s="32"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" s="31"/>
       <c r="C48" s="32"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="31"/>
       <c r="C49" s="32"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="31"/>
       <c r="C50" s="32"/>
     </row>
@@ -10971,19 +10620,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain">
+        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>12700</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:colOff>12700</xdr:colOff>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -10991,7 +10640,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain"/>
+        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11007,7 +10656,7 @@
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:colOff>12700</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
@@ -11021,19 +10670,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef">
+        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>12700</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:colOff>12700</xdr:colOff>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -11041,7 +10690,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef"/>
+        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Can now choose Engine choice by text in Setup Sheet
</commit_message>
<xml_diff>
--- a/SetupSheets.xlsx
+++ b/SetupSheets.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="121">
   <si>
     <t>Date</t>
   </si>
@@ -376,7 +376,13 @@
     <t>L/s</t>
   </si>
   <si>
-    <t>num2str(CalPolySLO)</t>
+    <t>Powertrain Choice</t>
+  </si>
+  <si>
+    <t>CalPolySLO</t>
+  </si>
+  <si>
+    <t>Delft</t>
   </si>
 </sst>
 </file>
@@ -529,7 +535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -693,14 +699,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -713,6 +711,17 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1447,13 +1456,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:CU50"/>
+  <dimension ref="A1:CV50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="BA6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="CP6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="BC6" sqref="BC6"/>
+      <selection pane="bottomRight" activeCell="CS10" sqref="CS10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1478,10 +1487,11 @@
     <col min="89" max="95" width="6.81640625" style="23" customWidth="1"/>
     <col min="96" max="96" width="6.81640625" style="24" customWidth="1"/>
     <col min="97" max="99" width="6.81640625" style="23" customWidth="1"/>
-    <col min="100" max="16384" width="9.1796875" style="23"/>
+    <col min="100" max="100" width="13.36328125" style="23" customWidth="1"/>
+    <col min="101" max="16384" width="9.1796875" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" s="25" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:100" s="25" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>35</v>
       </c>
@@ -1775,8 +1785,11 @@
       <c r="CU1" s="6" t="s">
         <v>98</v>
       </c>
+      <c r="CV1" s="6" t="s">
+        <v>118</v>
+      </c>
     </row>
-    <row r="2" spans="1:99" s="28" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:100" s="28" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="36"/>
       <c r="B2" s="26" t="s">
         <v>0</v>
@@ -2056,8 +2069,11 @@
       <c r="CU2" s="11" t="s">
         <v>86</v>
       </c>
+      <c r="CV2" s="11" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="3" spans="1:99" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:100" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37"/>
       <c r="B3" s="29"/>
       <c r="C3" s="30"/>
@@ -2157,8 +2173,9 @@
       <c r="CS3" s="15"/>
       <c r="CT3" s="15"/>
       <c r="CU3" s="15"/>
+      <c r="CV3" s="15"/>
     </row>
-    <row r="4" spans="1:99" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:100" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="37"/>
       <c r="B4" s="29"/>
       <c r="C4" s="30"/>
@@ -2258,9 +2275,10 @@
       <c r="CS4" s="15"/>
       <c r="CT4" s="15"/>
       <c r="CU4" s="15"/>
+      <c r="CV4" s="15"/>
     </row>
-    <row r="5" spans="1:99" s="22" customFormat="1" ht="13" x14ac:dyDescent="0.25">
-      <c r="A5" s="51" t="s">
+    <row r="5" spans="1:100" s="22" customFormat="1" ht="13" x14ac:dyDescent="0.25">
+      <c r="A5" s="49" t="s">
         <v>115</v>
       </c>
       <c r="B5" s="29"/>
@@ -2613,18 +2631,22 @@
         <f>CU3-CU4</f>
         <v>0</v>
       </c>
+      <c r="CV5" s="43">
+        <f>CV3-CV4</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:99" s="50" customFormat="1" ht="25" x14ac:dyDescent="0.25">
-      <c r="A6" s="49">
-        <v>0</v>
-      </c>
-      <c r="B6" s="48">
-        <v>0</v>
-      </c>
-      <c r="C6" s="47">
-        <v>0</v>
-      </c>
-      <c r="D6" s="45"/>
+    <row r="6" spans="1:100" s="48" customFormat="1" ht="13" x14ac:dyDescent="0.25">
+      <c r="A6" s="47">
+        <v>0</v>
+      </c>
+      <c r="B6" s="52">
+        <v>0</v>
+      </c>
+      <c r="C6" s="52">
+        <v>0</v>
+      </c>
+      <c r="D6" s="24"/>
       <c r="E6" s="45">
         <v>63</v>
       </c>
@@ -2688,7 +2710,7 @@
       <c r="Y6" s="45">
         <v>404</v>
       </c>
-      <c r="Z6" s="45"/>
+      <c r="Z6" s="14"/>
       <c r="AA6" s="45">
         <v>250</v>
       </c>
@@ -2755,7 +2777,7 @@
       <c r="AV6" s="45">
         <v>30</v>
       </c>
-      <c r="AW6" s="45"/>
+      <c r="AW6" s="14"/>
       <c r="AX6" s="45">
         <v>900</v>
       </c>
@@ -2771,10 +2793,10 @@
       <c r="BB6" s="45">
         <v>70.396699999999996</v>
       </c>
-      <c r="BC6" s="52" t="s">
-        <v>118</v>
-      </c>
-      <c r="BD6" s="45"/>
+      <c r="BC6" s="50">
+        <v>0</v>
+      </c>
+      <c r="BD6" s="14"/>
       <c r="BE6" s="45">
         <v>1</v>
       </c>
@@ -2814,7 +2836,7 @@
       <c r="BQ6" s="45">
         <v>20</v>
       </c>
-      <c r="BR6" s="45"/>
+      <c r="BR6" s="14"/>
       <c r="BS6" s="45">
         <v>6762.75</v>
       </c>
@@ -2833,7 +2855,7 @@
       <c r="BX6" s="45">
         <v>0.96699999999999997</v>
       </c>
-      <c r="BY6" s="45"/>
+      <c r="BY6" s="14"/>
       <c r="BZ6" s="45">
         <v>0</v>
       </c>
@@ -2864,7 +2886,7 @@
       <c r="CI6" s="45">
         <v>10</v>
       </c>
-      <c r="CJ6" s="45"/>
+      <c r="CJ6" s="14"/>
       <c r="CK6" s="45">
         <v>3.984</v>
       </c>
@@ -2886,7 +2908,7 @@
       <c r="CQ6" s="45">
         <v>0</v>
       </c>
-      <c r="CR6" s="45"/>
+      <c r="CR6" s="14"/>
       <c r="CS6" s="45">
         <v>0.28000000000000003</v>
       </c>
@@ -2896,113 +2918,299 @@
       <c r="CU6" s="45">
         <v>0</v>
       </c>
+      <c r="CV6" s="51" t="s">
+        <v>119</v>
+      </c>
     </row>
-    <row r="7" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A7" s="49"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="45"/>
-      <c r="O7" s="45"/>
-      <c r="P7" s="45"/>
-      <c r="Q7" s="45"/>
-      <c r="R7" s="45"/>
-      <c r="S7" s="45"/>
-      <c r="T7" s="46"/>
-      <c r="U7" s="45"/>
-      <c r="V7" s="45"/>
-      <c r="W7" s="45"/>
-      <c r="X7" s="45"/>
-      <c r="Y7" s="45"/>
-      <c r="Z7" s="45"/>
-      <c r="AA7" s="45"/>
-      <c r="AB7" s="45"/>
-      <c r="AC7" s="45"/>
-      <c r="AD7" s="45"/>
-      <c r="AE7" s="45"/>
-      <c r="AF7" s="45"/>
-      <c r="AG7" s="45"/>
-      <c r="AH7" s="45"/>
-      <c r="AI7" s="45"/>
-      <c r="AJ7" s="45"/>
-      <c r="AK7" s="45"/>
-      <c r="AL7" s="45"/>
-      <c r="AM7" s="45"/>
-      <c r="AN7" s="45"/>
-      <c r="AO7" s="45"/>
-      <c r="AP7" s="45"/>
-      <c r="AQ7" s="45"/>
-      <c r="AR7" s="45"/>
-      <c r="AS7" s="45"/>
-      <c r="AT7" s="45"/>
-      <c r="AU7" s="45"/>
-      <c r="AV7" s="45"/>
-      <c r="AW7" s="45"/>
-      <c r="AX7" s="45"/>
-      <c r="AY7" s="45"/>
-      <c r="AZ7" s="45"/>
-      <c r="BA7" s="45"/>
-      <c r="BB7" s="45"/>
-      <c r="BC7" s="45"/>
-      <c r="BD7" s="45"/>
-      <c r="BE7" s="45"/>
-      <c r="BF7" s="45"/>
-      <c r="BG7" s="45"/>
-      <c r="BH7" s="45"/>
-      <c r="BI7" s="45"/>
-      <c r="BJ7" s="45"/>
-      <c r="BK7" s="45"/>
-      <c r="BL7" s="45"/>
-      <c r="BM7" s="45"/>
-      <c r="BN7" s="45"/>
-      <c r="BO7" s="45"/>
-      <c r="BP7" s="45"/>
-      <c r="BQ7" s="45"/>
-      <c r="BR7" s="45"/>
-      <c r="BS7" s="45"/>
-      <c r="BT7" s="45"/>
-      <c r="BU7" s="45"/>
-      <c r="BV7" s="45"/>
-      <c r="BW7" s="45"/>
-      <c r="BX7" s="45"/>
-      <c r="BY7" s="45"/>
-      <c r="BZ7" s="45"/>
-      <c r="CA7" s="45"/>
-      <c r="CB7" s="45"/>
-      <c r="CC7" s="45"/>
-      <c r="CD7" s="45"/>
-      <c r="CE7" s="45"/>
-      <c r="CF7" s="45"/>
-      <c r="CG7" s="45"/>
-      <c r="CH7" s="45"/>
-      <c r="CI7" s="45"/>
-      <c r="CJ7" s="45"/>
-      <c r="CK7" s="45"/>
-      <c r="CL7" s="45"/>
-      <c r="CM7" s="45"/>
-      <c r="CN7" s="45"/>
-      <c r="CO7" s="45"/>
-      <c r="CP7" s="45"/>
-      <c r="CQ7" s="45"/>
-      <c r="CR7" s="45"/>
-      <c r="CS7" s="45"/>
-      <c r="CT7" s="45"/>
-      <c r="CU7" s="45"/>
+    <row r="7" spans="1:100" ht="13" x14ac:dyDescent="0.25">
+      <c r="A7" s="47">
+        <v>0</v>
+      </c>
+      <c r="B7" s="52">
+        <v>0</v>
+      </c>
+      <c r="C7" s="52">
+        <v>0</v>
+      </c>
+      <c r="E7" s="45">
+        <v>63</v>
+      </c>
+      <c r="F7" s="45">
+        <v>47</v>
+      </c>
+      <c r="G7" s="45">
+        <v>46</v>
+      </c>
+      <c r="H7" s="45">
+        <v>0</v>
+      </c>
+      <c r="I7" s="45">
+        <v>0</v>
+      </c>
+      <c r="J7" s="45">
+        <v>0</v>
+      </c>
+      <c r="K7" s="45">
+        <v>0</v>
+      </c>
+      <c r="L7" s="45">
+        <v>0</v>
+      </c>
+      <c r="M7" s="45">
+        <v>0</v>
+      </c>
+      <c r="N7" s="45">
+        <v>0</v>
+      </c>
+      <c r="O7" s="45">
+        <v>0</v>
+      </c>
+      <c r="P7" s="45">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="45">
+        <v>0</v>
+      </c>
+      <c r="R7" s="45">
+        <v>33.39</v>
+      </c>
+      <c r="S7" s="45">
+        <v>0</v>
+      </c>
+      <c r="T7" s="46">
+        <v>12</v>
+      </c>
+      <c r="U7" s="45">
+        <v>175</v>
+      </c>
+      <c r="V7" s="45">
+        <v>33.9</v>
+      </c>
+      <c r="W7" s="45">
+        <v>0</v>
+      </c>
+      <c r="X7" s="45">
+        <v>12</v>
+      </c>
+      <c r="Y7" s="45">
+        <v>404</v>
+      </c>
+      <c r="Z7" s="14"/>
+      <c r="AA7" s="45">
+        <v>250</v>
+      </c>
+      <c r="AB7" s="45">
+        <v>200</v>
+      </c>
+      <c r="AC7" s="45">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="45">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="45">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="45">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="45">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="45">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="45">
+        <v>10.25</v>
+      </c>
+      <c r="AJ7" s="45">
+        <v>10.25</v>
+      </c>
+      <c r="AK7" s="45">
+        <v>-0.25</v>
+      </c>
+      <c r="AL7" s="45">
+        <v>1.9</v>
+      </c>
+      <c r="AM7" s="45">
+        <v>0</v>
+      </c>
+      <c r="AN7" s="45">
+        <v>0</v>
+      </c>
+      <c r="AO7" s="45">
+        <v>0</v>
+      </c>
+      <c r="AP7" s="45">
+        <v>0</v>
+      </c>
+      <c r="AQ7" s="45">
+        <v>0</v>
+      </c>
+      <c r="AR7" s="45">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="45">
+        <v>0</v>
+      </c>
+      <c r="AT7" s="45">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="45">
+        <v>10</v>
+      </c>
+      <c r="AV7" s="45">
+        <v>30</v>
+      </c>
+      <c r="AW7" s="14"/>
+      <c r="AX7" s="45">
+        <v>900</v>
+      </c>
+      <c r="AY7" s="45">
+        <v>10.5</v>
+      </c>
+      <c r="AZ7" s="45">
+        <v>0.03</v>
+      </c>
+      <c r="BA7" s="45">
+        <v>120.628</v>
+      </c>
+      <c r="BB7" s="45">
+        <v>70.396699999999996</v>
+      </c>
+      <c r="BC7" s="50">
+        <v>0</v>
+      </c>
+      <c r="BD7" s="14"/>
+      <c r="BE7" s="45">
+        <v>1</v>
+      </c>
+      <c r="BF7" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="BG7" s="45">
+        <v>2</v>
+      </c>
+      <c r="BH7" s="45">
+        <v>1.62</v>
+      </c>
+      <c r="BI7" s="45">
+        <v>1.333</v>
+      </c>
+      <c r="BJ7" s="45">
+        <v>1.095</v>
+      </c>
+      <c r="BK7" s="45">
+        <v>2.6520000000000001</v>
+      </c>
+      <c r="BL7" s="45">
+        <v>2.714</v>
+      </c>
+      <c r="BM7" s="45">
+        <v>0.9</v>
+      </c>
+      <c r="BN7" s="45">
+        <v>0</v>
+      </c>
+      <c r="BO7" s="45">
+        <v>0</v>
+      </c>
+      <c r="BP7" s="45">
+        <v>0</v>
+      </c>
+      <c r="BQ7" s="45">
+        <v>20</v>
+      </c>
+      <c r="BR7" s="14"/>
+      <c r="BS7" s="45">
+        <v>6762.75</v>
+      </c>
+      <c r="BT7" s="45">
+        <v>3238.5</v>
+      </c>
+      <c r="BU7" s="45">
+        <v>0</v>
+      </c>
+      <c r="BV7" s="45">
+        <v>0</v>
+      </c>
+      <c r="BW7" s="45">
+        <v>0</v>
+      </c>
+      <c r="BX7" s="45">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="BY7" s="14"/>
+      <c r="BZ7" s="45">
+        <v>0</v>
+      </c>
+      <c r="CA7" s="45">
+        <v>0</v>
+      </c>
+      <c r="CB7" s="45">
+        <v>0</v>
+      </c>
+      <c r="CC7" s="45">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="CD7" s="45">
+        <v>-2.9000000000000001E-2</v>
+      </c>
+      <c r="CE7" s="45">
+        <v>2015</v>
+      </c>
+      <c r="CF7" s="45">
+        <v>2.3289999999999999E-3</v>
+      </c>
+      <c r="CG7" s="45">
+        <v>34.25</v>
+      </c>
+      <c r="CH7" s="45">
+        <v>0</v>
+      </c>
+      <c r="CI7" s="45">
+        <v>10</v>
+      </c>
+      <c r="CJ7" s="14"/>
+      <c r="CK7" s="45">
+        <v>3.984</v>
+      </c>
+      <c r="CL7" s="45">
+        <v>6.56</v>
+      </c>
+      <c r="CM7" s="45">
+        <v>250</v>
+      </c>
+      <c r="CN7" s="45">
+        <v>8.9789999999999998E-4</v>
+      </c>
+      <c r="CO7" s="45">
+        <v>8.9789999999999998E-4</v>
+      </c>
+      <c r="CP7" s="45">
+        <v>8.9789999999999998E-4</v>
+      </c>
+      <c r="CQ7" s="45">
+        <v>0</v>
+      </c>
+      <c r="CR7" s="14"/>
+      <c r="CS7" s="45">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="CT7" s="45">
+        <v>9000</v>
+      </c>
+      <c r="CU7" s="45">
+        <v>0</v>
+      </c>
+      <c r="CV7" s="51" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="8" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A8" s="49"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="45"/>
+    <row r="8" spans="1:100" ht="13" x14ac:dyDescent="0.25">
+      <c r="A8" s="47"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
       <c r="E8" s="45"/>
       <c r="F8" s="45"/>
       <c r="G8" s="45"/>
@@ -3024,7 +3232,7 @@
       <c r="W8" s="45"/>
       <c r="X8" s="45"/>
       <c r="Y8" s="45"/>
-      <c r="Z8" s="45"/>
+      <c r="Z8" s="14"/>
       <c r="AA8" s="45"/>
       <c r="AB8" s="45"/>
       <c r="AC8" s="45"/>
@@ -3047,14 +3255,14 @@
       <c r="AT8" s="45"/>
       <c r="AU8" s="45"/>
       <c r="AV8" s="45"/>
-      <c r="AW8" s="45"/>
+      <c r="AW8" s="14"/>
       <c r="AX8" s="45"/>
       <c r="AY8" s="45"/>
       <c r="AZ8" s="45"/>
       <c r="BA8" s="45"/>
       <c r="BB8" s="45"/>
-      <c r="BC8" s="45"/>
-      <c r="BD8" s="45"/>
+      <c r="BC8" s="50"/>
+      <c r="BD8" s="14"/>
       <c r="BE8" s="45"/>
       <c r="BF8" s="45"/>
       <c r="BG8" s="45"/>
@@ -3068,14 +3276,14 @@
       <c r="BO8" s="45"/>
       <c r="BP8" s="45"/>
       <c r="BQ8" s="45"/>
-      <c r="BR8" s="45"/>
+      <c r="BR8" s="14"/>
       <c r="BS8" s="45"/>
       <c r="BT8" s="45"/>
       <c r="BU8" s="45"/>
       <c r="BV8" s="45"/>
       <c r="BW8" s="45"/>
       <c r="BX8" s="45"/>
-      <c r="BY8" s="45"/>
+      <c r="BY8" s="14"/>
       <c r="BZ8" s="45"/>
       <c r="CA8" s="45"/>
       <c r="CB8" s="45"/>
@@ -3086,7 +3294,7 @@
       <c r="CG8" s="45"/>
       <c r="CH8" s="45"/>
       <c r="CI8" s="45"/>
-      <c r="CJ8" s="45"/>
+      <c r="CJ8" s="14"/>
       <c r="CK8" s="45"/>
       <c r="CL8" s="45"/>
       <c r="CM8" s="45"/>
@@ -3094,16 +3302,16 @@
       <c r="CO8" s="45"/>
       <c r="CP8" s="45"/>
       <c r="CQ8" s="45"/>
-      <c r="CR8" s="45"/>
+      <c r="CR8" s="14"/>
       <c r="CS8" s="45"/>
       <c r="CT8" s="45"/>
       <c r="CU8" s="45"/>
+      <c r="CV8" s="51"/>
     </row>
-    <row r="9" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A9" s="49"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="45"/>
+    <row r="9" spans="1:100" ht="13" x14ac:dyDescent="0.25">
+      <c r="A9" s="47"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="52"/>
       <c r="E9" s="45"/>
       <c r="F9" s="45"/>
       <c r="G9" s="45"/>
@@ -3125,7 +3333,7 @@
       <c r="W9" s="45"/>
       <c r="X9" s="45"/>
       <c r="Y9" s="45"/>
-      <c r="Z9" s="45"/>
+      <c r="Z9" s="14"/>
       <c r="AA9" s="45"/>
       <c r="AB9" s="45"/>
       <c r="AC9" s="45"/>
@@ -3148,14 +3356,14 @@
       <c r="AT9" s="45"/>
       <c r="AU9" s="45"/>
       <c r="AV9" s="45"/>
-      <c r="AW9" s="45"/>
+      <c r="AW9" s="14"/>
       <c r="AX9" s="45"/>
       <c r="AY9" s="45"/>
       <c r="AZ9" s="45"/>
       <c r="BA9" s="45"/>
       <c r="BB9" s="45"/>
       <c r="BC9" s="45"/>
-      <c r="BD9" s="45"/>
+      <c r="BD9" s="14"/>
       <c r="BE9" s="45"/>
       <c r="BF9" s="45"/>
       <c r="BG9" s="45"/>
@@ -3169,14 +3377,14 @@
       <c r="BO9" s="45"/>
       <c r="BP9" s="45"/>
       <c r="BQ9" s="45"/>
-      <c r="BR9" s="45"/>
+      <c r="BR9" s="14"/>
       <c r="BS9" s="45"/>
       <c r="BT9" s="45"/>
       <c r="BU9" s="45"/>
       <c r="BV9" s="45"/>
       <c r="BW9" s="45"/>
       <c r="BX9" s="45"/>
-      <c r="BY9" s="45"/>
+      <c r="BY9" s="14"/>
       <c r="BZ9" s="45"/>
       <c r="CA9" s="45"/>
       <c r="CB9" s="45"/>
@@ -3187,7 +3395,7 @@
       <c r="CG9" s="45"/>
       <c r="CH9" s="45"/>
       <c r="CI9" s="45"/>
-      <c r="CJ9" s="45"/>
+      <c r="CJ9" s="14"/>
       <c r="CK9" s="45"/>
       <c r="CL9" s="45"/>
       <c r="CM9" s="45"/>
@@ -3195,16 +3403,15 @@
       <c r="CO9" s="45"/>
       <c r="CP9" s="45"/>
       <c r="CQ9" s="45"/>
-      <c r="CR9" s="45"/>
+      <c r="CR9" s="14"/>
       <c r="CS9" s="45"/>
       <c r="CT9" s="45"/>
       <c r="CU9" s="45"/>
     </row>
-    <row r="10" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A10" s="49"/>
-      <c r="B10" s="48"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="45"/>
+    <row r="10" spans="1:100" ht="13" x14ac:dyDescent="0.25">
+      <c r="A10" s="47"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
       <c r="E10" s="45"/>
       <c r="F10" s="45"/>
       <c r="G10" s="45"/>
@@ -3226,7 +3433,7 @@
       <c r="W10" s="45"/>
       <c r="X10" s="45"/>
       <c r="Y10" s="45"/>
-      <c r="Z10" s="45"/>
+      <c r="Z10" s="14"/>
       <c r="AA10" s="45"/>
       <c r="AB10" s="45"/>
       <c r="AC10" s="45"/>
@@ -3249,14 +3456,14 @@
       <c r="AT10" s="45"/>
       <c r="AU10" s="45"/>
       <c r="AV10" s="45"/>
-      <c r="AW10" s="45"/>
+      <c r="AW10" s="14"/>
       <c r="AX10" s="45"/>
       <c r="AY10" s="45"/>
       <c r="AZ10" s="45"/>
       <c r="BA10" s="45"/>
       <c r="BB10" s="45"/>
       <c r="BC10" s="45"/>
-      <c r="BD10" s="45"/>
+      <c r="BD10" s="14"/>
       <c r="BE10" s="45"/>
       <c r="BF10" s="45"/>
       <c r="BG10" s="45"/>
@@ -3270,14 +3477,14 @@
       <c r="BO10" s="45"/>
       <c r="BP10" s="45"/>
       <c r="BQ10" s="45"/>
-      <c r="BR10" s="45"/>
+      <c r="BR10" s="14"/>
       <c r="BS10" s="45"/>
       <c r="BT10" s="45"/>
       <c r="BU10" s="45"/>
       <c r="BV10" s="45"/>
       <c r="BW10" s="45"/>
       <c r="BX10" s="45"/>
-      <c r="BY10" s="45"/>
+      <c r="BY10" s="14"/>
       <c r="BZ10" s="45"/>
       <c r="CA10" s="45"/>
       <c r="CB10" s="45"/>
@@ -3288,7 +3495,7 @@
       <c r="CG10" s="45"/>
       <c r="CH10" s="45"/>
       <c r="CI10" s="45"/>
-      <c r="CJ10" s="45"/>
+      <c r="CJ10" s="14"/>
       <c r="CK10" s="45"/>
       <c r="CL10" s="45"/>
       <c r="CM10" s="45"/>
@@ -3296,16 +3503,15 @@
       <c r="CO10" s="45"/>
       <c r="CP10" s="45"/>
       <c r="CQ10" s="45"/>
-      <c r="CR10" s="45"/>
+      <c r="CR10" s="14"/>
       <c r="CS10" s="45"/>
       <c r="CT10" s="45"/>
       <c r="CU10" s="45"/>
     </row>
-    <row r="11" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="45"/>
+    <row r="11" spans="1:100" ht="13" x14ac:dyDescent="0.25">
+      <c r="A11" s="47"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
       <c r="E11" s="45"/>
       <c r="F11" s="45"/>
       <c r="G11" s="45"/>
@@ -3327,7 +3533,7 @@
       <c r="W11" s="45"/>
       <c r="X11" s="45"/>
       <c r="Y11" s="45"/>
-      <c r="Z11" s="45"/>
+      <c r="Z11" s="14"/>
       <c r="AA11" s="45"/>
       <c r="AB11" s="45"/>
       <c r="AC11" s="45"/>
@@ -3350,14 +3556,14 @@
       <c r="AT11" s="45"/>
       <c r="AU11" s="45"/>
       <c r="AV11" s="45"/>
-      <c r="AW11" s="45"/>
+      <c r="AW11" s="14"/>
       <c r="AX11" s="45"/>
       <c r="AY11" s="45"/>
       <c r="AZ11" s="45"/>
       <c r="BA11" s="45"/>
       <c r="BB11" s="45"/>
       <c r="BC11" s="45"/>
-      <c r="BD11" s="45"/>
+      <c r="BD11" s="14"/>
       <c r="BE11" s="45"/>
       <c r="BF11" s="45"/>
       <c r="BG11" s="45"/>
@@ -3371,14 +3577,14 @@
       <c r="BO11" s="45"/>
       <c r="BP11" s="45"/>
       <c r="BQ11" s="45"/>
-      <c r="BR11" s="45"/>
+      <c r="BR11" s="14"/>
       <c r="BS11" s="45"/>
       <c r="BT11" s="45"/>
       <c r="BU11" s="45"/>
       <c r="BV11" s="45"/>
       <c r="BW11" s="45"/>
       <c r="BX11" s="45"/>
-      <c r="BY11" s="45"/>
+      <c r="BY11" s="14"/>
       <c r="BZ11" s="45"/>
       <c r="CA11" s="45"/>
       <c r="CB11" s="45"/>
@@ -3389,7 +3595,7 @@
       <c r="CG11" s="45"/>
       <c r="CH11" s="45"/>
       <c r="CI11" s="45"/>
-      <c r="CJ11" s="45"/>
+      <c r="CJ11" s="14"/>
       <c r="CK11" s="45"/>
       <c r="CL11" s="45"/>
       <c r="CM11" s="45"/>
@@ -3397,16 +3603,15 @@
       <c r="CO11" s="45"/>
       <c r="CP11" s="45"/>
       <c r="CQ11" s="45"/>
-      <c r="CR11" s="45"/>
+      <c r="CR11" s="14"/>
       <c r="CS11" s="45"/>
       <c r="CT11" s="45"/>
       <c r="CU11" s="45"/>
     </row>
-    <row r="12" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A12" s="49"/>
-      <c r="B12" s="48"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="45"/>
+    <row r="12" spans="1:100" ht="13" x14ac:dyDescent="0.25">
+      <c r="A12" s="47"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="52"/>
       <c r="E12" s="45"/>
       <c r="F12" s="45"/>
       <c r="G12" s="45"/>
@@ -3428,7 +3633,7 @@
       <c r="W12" s="45"/>
       <c r="X12" s="45"/>
       <c r="Y12" s="45"/>
-      <c r="Z12" s="45"/>
+      <c r="Z12" s="14"/>
       <c r="AA12" s="45"/>
       <c r="AB12" s="45"/>
       <c r="AC12" s="45"/>
@@ -3451,14 +3656,14 @@
       <c r="AT12" s="45"/>
       <c r="AU12" s="45"/>
       <c r="AV12" s="45"/>
-      <c r="AW12" s="45"/>
+      <c r="AW12" s="14"/>
       <c r="AX12" s="45"/>
       <c r="AY12" s="45"/>
       <c r="AZ12" s="45"/>
       <c r="BA12" s="45"/>
       <c r="BB12" s="45"/>
       <c r="BC12" s="45"/>
-      <c r="BD12" s="45"/>
+      <c r="BD12" s="14"/>
       <c r="BE12" s="45"/>
       <c r="BF12" s="45"/>
       <c r="BG12" s="45"/>
@@ -3472,14 +3677,14 @@
       <c r="BO12" s="45"/>
       <c r="BP12" s="45"/>
       <c r="BQ12" s="45"/>
-      <c r="BR12" s="45"/>
+      <c r="BR12" s="14"/>
       <c r="BS12" s="45"/>
       <c r="BT12" s="45"/>
       <c r="BU12" s="45"/>
       <c r="BV12" s="45"/>
       <c r="BW12" s="45"/>
       <c r="BX12" s="45"/>
-      <c r="BY12" s="45"/>
+      <c r="BY12" s="14"/>
       <c r="BZ12" s="45"/>
       <c r="CA12" s="45"/>
       <c r="CB12" s="45"/>
@@ -3490,7 +3695,7 @@
       <c r="CG12" s="45"/>
       <c r="CH12" s="45"/>
       <c r="CI12" s="45"/>
-      <c r="CJ12" s="45"/>
+      <c r="CJ12" s="14"/>
       <c r="CK12" s="45"/>
       <c r="CL12" s="45"/>
       <c r="CM12" s="45"/>
@@ -3498,16 +3703,15 @@
       <c r="CO12" s="45"/>
       <c r="CP12" s="45"/>
       <c r="CQ12" s="45"/>
-      <c r="CR12" s="45"/>
+      <c r="CR12" s="14"/>
       <c r="CS12" s="45"/>
       <c r="CT12" s="45"/>
       <c r="CU12" s="45"/>
     </row>
-    <row r="13" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A13" s="49"/>
-      <c r="B13" s="48"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="45"/>
+    <row r="13" spans="1:100" ht="13" x14ac:dyDescent="0.25">
+      <c r="A13" s="47"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="52"/>
       <c r="E13" s="45"/>
       <c r="F13" s="45"/>
       <c r="G13" s="45"/>
@@ -3529,7 +3733,7 @@
       <c r="W13" s="45"/>
       <c r="X13" s="45"/>
       <c r="Y13" s="45"/>
-      <c r="Z13" s="45"/>
+      <c r="Z13" s="14"/>
       <c r="AA13" s="45"/>
       <c r="AB13" s="45"/>
       <c r="AC13" s="45"/>
@@ -3552,14 +3756,14 @@
       <c r="AT13" s="45"/>
       <c r="AU13" s="45"/>
       <c r="AV13" s="45"/>
-      <c r="AW13" s="45"/>
+      <c r="AW13" s="14"/>
       <c r="AX13" s="45"/>
       <c r="AY13" s="45"/>
       <c r="AZ13" s="45"/>
       <c r="BA13" s="45"/>
       <c r="BB13" s="45"/>
       <c r="BC13" s="45"/>
-      <c r="BD13" s="45"/>
+      <c r="BD13" s="14"/>
       <c r="BE13" s="45"/>
       <c r="BF13" s="45"/>
       <c r="BG13" s="45"/>
@@ -3573,14 +3777,14 @@
       <c r="BO13" s="45"/>
       <c r="BP13" s="45"/>
       <c r="BQ13" s="45"/>
-      <c r="BR13" s="45"/>
+      <c r="BR13" s="14"/>
       <c r="BS13" s="45"/>
       <c r="BT13" s="45"/>
       <c r="BU13" s="45"/>
       <c r="BV13" s="45"/>
       <c r="BW13" s="45"/>
       <c r="BX13" s="45"/>
-      <c r="BY13" s="45"/>
+      <c r="BY13" s="14"/>
       <c r="BZ13" s="45"/>
       <c r="CA13" s="45"/>
       <c r="CB13" s="45"/>
@@ -3591,7 +3795,7 @@
       <c r="CG13" s="45"/>
       <c r="CH13" s="45"/>
       <c r="CI13" s="45"/>
-      <c r="CJ13" s="45"/>
+      <c r="CJ13" s="14"/>
       <c r="CK13" s="45"/>
       <c r="CL13" s="45"/>
       <c r="CM13" s="45"/>
@@ -3599,16 +3803,15 @@
       <c r="CO13" s="45"/>
       <c r="CP13" s="45"/>
       <c r="CQ13" s="45"/>
-      <c r="CR13" s="45"/>
+      <c r="CR13" s="14"/>
       <c r="CS13" s="45"/>
       <c r="CT13" s="45"/>
       <c r="CU13" s="45"/>
     </row>
-    <row r="14" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A14" s="49"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="45"/>
+    <row r="14" spans="1:100" ht="13" x14ac:dyDescent="0.25">
+      <c r="A14" s="47"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
       <c r="E14" s="45"/>
       <c r="F14" s="45"/>
       <c r="G14" s="45"/>
@@ -3630,7 +3833,7 @@
       <c r="W14" s="45"/>
       <c r="X14" s="45"/>
       <c r="Y14" s="45"/>
-      <c r="Z14" s="45"/>
+      <c r="Z14" s="14"/>
       <c r="AA14" s="45"/>
       <c r="AB14" s="45"/>
       <c r="AC14" s="45"/>
@@ -3653,14 +3856,14 @@
       <c r="AT14" s="45"/>
       <c r="AU14" s="45"/>
       <c r="AV14" s="45"/>
-      <c r="AW14" s="45"/>
+      <c r="AW14" s="14"/>
       <c r="AX14" s="45"/>
       <c r="AY14" s="45"/>
       <c r="AZ14" s="45"/>
       <c r="BA14" s="45"/>
       <c r="BB14" s="45"/>
       <c r="BC14" s="45"/>
-      <c r="BD14" s="45"/>
+      <c r="BD14" s="14"/>
       <c r="BE14" s="45"/>
       <c r="BF14" s="45"/>
       <c r="BG14" s="45"/>
@@ -3674,14 +3877,14 @@
       <c r="BO14" s="45"/>
       <c r="BP14" s="45"/>
       <c r="BQ14" s="45"/>
-      <c r="BR14" s="45"/>
+      <c r="BR14" s="14"/>
       <c r="BS14" s="45"/>
       <c r="BT14" s="45"/>
       <c r="BU14" s="45"/>
       <c r="BV14" s="45"/>
       <c r="BW14" s="45"/>
       <c r="BX14" s="45"/>
-      <c r="BY14" s="45"/>
+      <c r="BY14" s="14"/>
       <c r="BZ14" s="45"/>
       <c r="CA14" s="45"/>
       <c r="CB14" s="45"/>
@@ -3692,7 +3895,7 @@
       <c r="CG14" s="45"/>
       <c r="CH14" s="45"/>
       <c r="CI14" s="45"/>
-      <c r="CJ14" s="45"/>
+      <c r="CJ14" s="14"/>
       <c r="CK14" s="45"/>
       <c r="CL14" s="45"/>
       <c r="CM14" s="45"/>
@@ -3700,16 +3903,15 @@
       <c r="CO14" s="45"/>
       <c r="CP14" s="45"/>
       <c r="CQ14" s="45"/>
-      <c r="CR14" s="45"/>
+      <c r="CR14" s="14"/>
       <c r="CS14" s="45"/>
       <c r="CT14" s="45"/>
       <c r="CU14" s="45"/>
     </row>
-    <row r="15" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A15" s="49"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="45"/>
+    <row r="15" spans="1:100" ht="13" x14ac:dyDescent="0.25">
+      <c r="A15" s="47"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
       <c r="E15" s="45"/>
       <c r="F15" s="45"/>
       <c r="G15" s="45"/>
@@ -3731,7 +3933,7 @@
       <c r="W15" s="45"/>
       <c r="X15" s="45"/>
       <c r="Y15" s="45"/>
-      <c r="Z15" s="45"/>
+      <c r="Z15" s="14"/>
       <c r="AA15" s="45"/>
       <c r="AB15" s="45"/>
       <c r="AC15" s="45"/>
@@ -3754,14 +3956,14 @@
       <c r="AT15" s="45"/>
       <c r="AU15" s="45"/>
       <c r="AV15" s="45"/>
-      <c r="AW15" s="45"/>
+      <c r="AW15" s="14"/>
       <c r="AX15" s="45"/>
       <c r="AY15" s="45"/>
       <c r="AZ15" s="45"/>
       <c r="BA15" s="45"/>
       <c r="BB15" s="45"/>
       <c r="BC15" s="45"/>
-      <c r="BD15" s="45"/>
+      <c r="BD15" s="14"/>
       <c r="BE15" s="45"/>
       <c r="BF15" s="45"/>
       <c r="BG15" s="45"/>
@@ -3775,14 +3977,14 @@
       <c r="BO15" s="45"/>
       <c r="BP15" s="45"/>
       <c r="BQ15" s="45"/>
-      <c r="BR15" s="45"/>
+      <c r="BR15" s="14"/>
       <c r="BS15" s="45"/>
       <c r="BT15" s="45"/>
       <c r="BU15" s="45"/>
       <c r="BV15" s="45"/>
       <c r="BW15" s="45"/>
       <c r="BX15" s="45"/>
-      <c r="BY15" s="45"/>
+      <c r="BY15" s="14"/>
       <c r="BZ15" s="45"/>
       <c r="CA15" s="45"/>
       <c r="CB15" s="45"/>
@@ -3793,7 +3995,7 @@
       <c r="CG15" s="45"/>
       <c r="CH15" s="45"/>
       <c r="CI15" s="45"/>
-      <c r="CJ15" s="45"/>
+      <c r="CJ15" s="14"/>
       <c r="CK15" s="45"/>
       <c r="CL15" s="45"/>
       <c r="CM15" s="45"/>
@@ -3801,16 +4003,15 @@
       <c r="CO15" s="45"/>
       <c r="CP15" s="45"/>
       <c r="CQ15" s="45"/>
-      <c r="CR15" s="45"/>
+      <c r="CR15" s="14"/>
       <c r="CS15" s="45"/>
       <c r="CT15" s="45"/>
       <c r="CU15" s="45"/>
     </row>
-    <row r="16" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A16" s="49"/>
-      <c r="B16" s="48"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="45"/>
+    <row r="16" spans="1:100" ht="13" x14ac:dyDescent="0.25">
+      <c r="A16" s="47"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="52"/>
       <c r="E16" s="45"/>
       <c r="F16" s="45"/>
       <c r="G16" s="45"/>
@@ -3832,7 +4033,7 @@
       <c r="W16" s="45"/>
       <c r="X16" s="45"/>
       <c r="Y16" s="45"/>
-      <c r="Z16" s="45"/>
+      <c r="Z16" s="14"/>
       <c r="AA16" s="45"/>
       <c r="AB16" s="45"/>
       <c r="AC16" s="45"/>
@@ -3855,14 +4056,14 @@
       <c r="AT16" s="45"/>
       <c r="AU16" s="45"/>
       <c r="AV16" s="45"/>
-      <c r="AW16" s="45"/>
+      <c r="AW16" s="14"/>
       <c r="AX16" s="45"/>
       <c r="AY16" s="45"/>
       <c r="AZ16" s="45"/>
       <c r="BA16" s="45"/>
       <c r="BB16" s="45"/>
       <c r="BC16" s="45"/>
-      <c r="BD16" s="45"/>
+      <c r="BD16" s="14"/>
       <c r="BE16" s="45"/>
       <c r="BF16" s="45"/>
       <c r="BG16" s="45"/>
@@ -3876,14 +4077,14 @@
       <c r="BO16" s="45"/>
       <c r="BP16" s="45"/>
       <c r="BQ16" s="45"/>
-      <c r="BR16" s="45"/>
+      <c r="BR16" s="14"/>
       <c r="BS16" s="45"/>
       <c r="BT16" s="45"/>
       <c r="BU16" s="45"/>
       <c r="BV16" s="45"/>
       <c r="BW16" s="45"/>
       <c r="BX16" s="45"/>
-      <c r="BY16" s="45"/>
+      <c r="BY16" s="14"/>
       <c r="BZ16" s="45"/>
       <c r="CA16" s="45"/>
       <c r="CB16" s="45"/>
@@ -3894,7 +4095,7 @@
       <c r="CG16" s="45"/>
       <c r="CH16" s="45"/>
       <c r="CI16" s="45"/>
-      <c r="CJ16" s="45"/>
+      <c r="CJ16" s="14"/>
       <c r="CK16" s="45"/>
       <c r="CL16" s="45"/>
       <c r="CM16" s="45"/>
@@ -3902,16 +4103,15 @@
       <c r="CO16" s="45"/>
       <c r="CP16" s="45"/>
       <c r="CQ16" s="45"/>
-      <c r="CR16" s="45"/>
+      <c r="CR16" s="14"/>
       <c r="CS16" s="45"/>
       <c r="CT16" s="45"/>
       <c r="CU16" s="45"/>
     </row>
-    <row r="17" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A17" s="49"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="45"/>
+    <row r="17" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="A17" s="47"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="52"/>
       <c r="E17" s="45"/>
       <c r="F17" s="45"/>
       <c r="G17" s="45"/>
@@ -3933,7 +4133,7 @@
       <c r="W17" s="45"/>
       <c r="X17" s="45"/>
       <c r="Y17" s="45"/>
-      <c r="Z17" s="45"/>
+      <c r="Z17" s="14"/>
       <c r="AA17" s="45"/>
       <c r="AB17" s="45"/>
       <c r="AC17" s="45"/>
@@ -3956,14 +4156,14 @@
       <c r="AT17" s="45"/>
       <c r="AU17" s="45"/>
       <c r="AV17" s="45"/>
-      <c r="AW17" s="45"/>
+      <c r="AW17" s="14"/>
       <c r="AX17" s="45"/>
       <c r="AY17" s="45"/>
       <c r="AZ17" s="45"/>
       <c r="BA17" s="45"/>
       <c r="BB17" s="45"/>
       <c r="BC17" s="45"/>
-      <c r="BD17" s="45"/>
+      <c r="BD17" s="14"/>
       <c r="BE17" s="45"/>
       <c r="BF17" s="45"/>
       <c r="BG17" s="45"/>
@@ -3977,14 +4177,14 @@
       <c r="BO17" s="45"/>
       <c r="BP17" s="45"/>
       <c r="BQ17" s="45"/>
-      <c r="BR17" s="45"/>
+      <c r="BR17" s="14"/>
       <c r="BS17" s="45"/>
       <c r="BT17" s="45"/>
       <c r="BU17" s="45"/>
       <c r="BV17" s="45"/>
       <c r="BW17" s="45"/>
       <c r="BX17" s="45"/>
-      <c r="BY17" s="45"/>
+      <c r="BY17" s="14"/>
       <c r="BZ17" s="45"/>
       <c r="CA17" s="45"/>
       <c r="CB17" s="45"/>
@@ -3995,7 +4195,7 @@
       <c r="CG17" s="45"/>
       <c r="CH17" s="45"/>
       <c r="CI17" s="45"/>
-      <c r="CJ17" s="45"/>
+      <c r="CJ17" s="14"/>
       <c r="CK17" s="45"/>
       <c r="CL17" s="45"/>
       <c r="CM17" s="45"/>
@@ -4003,16 +4203,15 @@
       <c r="CO17" s="45"/>
       <c r="CP17" s="45"/>
       <c r="CQ17" s="45"/>
-      <c r="CR17" s="45"/>
+      <c r="CR17" s="14"/>
       <c r="CS17" s="45"/>
       <c r="CT17" s="45"/>
       <c r="CU17" s="45"/>
     </row>
-    <row r="18" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A18" s="49"/>
-      <c r="B18" s="48"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="45"/>
+    <row r="18" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="A18" s="47"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="52"/>
       <c r="E18" s="45"/>
       <c r="F18" s="45"/>
       <c r="G18" s="45"/>
@@ -4034,7 +4233,7 @@
       <c r="W18" s="45"/>
       <c r="X18" s="45"/>
       <c r="Y18" s="45"/>
-      <c r="Z18" s="45"/>
+      <c r="Z18" s="14"/>
       <c r="AA18" s="45"/>
       <c r="AB18" s="45"/>
       <c r="AC18" s="45"/>
@@ -4057,14 +4256,14 @@
       <c r="AT18" s="45"/>
       <c r="AU18" s="45"/>
       <c r="AV18" s="45"/>
-      <c r="AW18" s="45"/>
+      <c r="AW18" s="14"/>
       <c r="AX18" s="45"/>
       <c r="AY18" s="45"/>
       <c r="AZ18" s="45"/>
       <c r="BA18" s="45"/>
       <c r="BB18" s="45"/>
       <c r="BC18" s="45"/>
-      <c r="BD18" s="45"/>
+      <c r="BD18" s="14"/>
       <c r="BE18" s="45"/>
       <c r="BF18" s="45"/>
       <c r="BG18" s="45"/>
@@ -4078,14 +4277,14 @@
       <c r="BO18" s="45"/>
       <c r="BP18" s="45"/>
       <c r="BQ18" s="45"/>
-      <c r="BR18" s="45"/>
+      <c r="BR18" s="14"/>
       <c r="BS18" s="45"/>
       <c r="BT18" s="45"/>
       <c r="BU18" s="45"/>
       <c r="BV18" s="45"/>
       <c r="BW18" s="45"/>
       <c r="BX18" s="45"/>
-      <c r="BY18" s="45"/>
+      <c r="BY18" s="14"/>
       <c r="BZ18" s="45"/>
       <c r="CA18" s="45"/>
       <c r="CB18" s="45"/>
@@ -4096,7 +4295,7 @@
       <c r="CG18" s="45"/>
       <c r="CH18" s="45"/>
       <c r="CI18" s="45"/>
-      <c r="CJ18" s="45"/>
+      <c r="CJ18" s="14"/>
       <c r="CK18" s="45"/>
       <c r="CL18" s="45"/>
       <c r="CM18" s="45"/>
@@ -4104,16 +4303,15 @@
       <c r="CO18" s="45"/>
       <c r="CP18" s="45"/>
       <c r="CQ18" s="45"/>
-      <c r="CR18" s="45"/>
+      <c r="CR18" s="14"/>
       <c r="CS18" s="45"/>
       <c r="CT18" s="45"/>
       <c r="CU18" s="45"/>
     </row>
-    <row r="19" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A19" s="49"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="45"/>
+    <row r="19" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="A19" s="47"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="52"/>
       <c r="E19" s="45"/>
       <c r="F19" s="45"/>
       <c r="G19" s="45"/>
@@ -4135,7 +4333,7 @@
       <c r="W19" s="45"/>
       <c r="X19" s="45"/>
       <c r="Y19" s="45"/>
-      <c r="Z19" s="45"/>
+      <c r="Z19" s="14"/>
       <c r="AA19" s="45"/>
       <c r="AB19" s="45"/>
       <c r="AC19" s="45"/>
@@ -4158,14 +4356,14 @@
       <c r="AT19" s="45"/>
       <c r="AU19" s="45"/>
       <c r="AV19" s="45"/>
-      <c r="AW19" s="45"/>
+      <c r="AW19" s="14"/>
       <c r="AX19" s="45"/>
       <c r="AY19" s="45"/>
       <c r="AZ19" s="45"/>
       <c r="BA19" s="45"/>
       <c r="BB19" s="45"/>
       <c r="BC19" s="45"/>
-      <c r="BD19" s="45"/>
+      <c r="BD19" s="14"/>
       <c r="BE19" s="45"/>
       <c r="BF19" s="45"/>
       <c r="BG19" s="45"/>
@@ -4179,14 +4377,14 @@
       <c r="BO19" s="45"/>
       <c r="BP19" s="45"/>
       <c r="BQ19" s="45"/>
-      <c r="BR19" s="45"/>
+      <c r="BR19" s="14"/>
       <c r="BS19" s="45"/>
       <c r="BT19" s="45"/>
       <c r="BU19" s="45"/>
       <c r="BV19" s="45"/>
       <c r="BW19" s="45"/>
       <c r="BX19" s="45"/>
-      <c r="BY19" s="45"/>
+      <c r="BY19" s="14"/>
       <c r="BZ19" s="45"/>
       <c r="CA19" s="45"/>
       <c r="CB19" s="45"/>
@@ -4197,7 +4395,7 @@
       <c r="CG19" s="45"/>
       <c r="CH19" s="45"/>
       <c r="CI19" s="45"/>
-      <c r="CJ19" s="45"/>
+      <c r="CJ19" s="14"/>
       <c r="CK19" s="45"/>
       <c r="CL19" s="45"/>
       <c r="CM19" s="45"/>
@@ -4205,16 +4403,15 @@
       <c r="CO19" s="45"/>
       <c r="CP19" s="45"/>
       <c r="CQ19" s="45"/>
-      <c r="CR19" s="45"/>
+      <c r="CR19" s="14"/>
       <c r="CS19" s="45"/>
       <c r="CT19" s="45"/>
       <c r="CU19" s="45"/>
     </row>
-    <row r="20" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A20" s="49"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="45"/>
+    <row r="20" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="A20" s="47"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="52"/>
       <c r="E20" s="45"/>
       <c r="F20" s="45"/>
       <c r="G20" s="45"/>
@@ -4236,7 +4433,7 @@
       <c r="W20" s="45"/>
       <c r="X20" s="45"/>
       <c r="Y20" s="45"/>
-      <c r="Z20" s="45"/>
+      <c r="Z20" s="14"/>
       <c r="AA20" s="45"/>
       <c r="AB20" s="45"/>
       <c r="AC20" s="45"/>
@@ -4259,14 +4456,14 @@
       <c r="AT20" s="45"/>
       <c r="AU20" s="45"/>
       <c r="AV20" s="45"/>
-      <c r="AW20" s="45"/>
+      <c r="AW20" s="14"/>
       <c r="AX20" s="45"/>
       <c r="AY20" s="45"/>
       <c r="AZ20" s="45"/>
       <c r="BA20" s="45"/>
       <c r="BB20" s="45"/>
       <c r="BC20" s="45"/>
-      <c r="BD20" s="45"/>
+      <c r="BD20" s="14"/>
       <c r="BE20" s="45"/>
       <c r="BF20" s="45"/>
       <c r="BG20" s="45"/>
@@ -4280,14 +4477,14 @@
       <c r="BO20" s="45"/>
       <c r="BP20" s="45"/>
       <c r="BQ20" s="45"/>
-      <c r="BR20" s="45"/>
+      <c r="BR20" s="14"/>
       <c r="BS20" s="45"/>
       <c r="BT20" s="45"/>
       <c r="BU20" s="45"/>
       <c r="BV20" s="45"/>
       <c r="BW20" s="45"/>
       <c r="BX20" s="45"/>
-      <c r="BY20" s="45"/>
+      <c r="BY20" s="14"/>
       <c r="BZ20" s="45"/>
       <c r="CA20" s="45"/>
       <c r="CB20" s="45"/>
@@ -4298,7 +4495,7 @@
       <c r="CG20" s="45"/>
       <c r="CH20" s="45"/>
       <c r="CI20" s="45"/>
-      <c r="CJ20" s="45"/>
+      <c r="CJ20" s="14"/>
       <c r="CK20" s="45"/>
       <c r="CL20" s="45"/>
       <c r="CM20" s="45"/>
@@ -4306,16 +4503,15 @@
       <c r="CO20" s="45"/>
       <c r="CP20" s="45"/>
       <c r="CQ20" s="45"/>
-      <c r="CR20" s="45"/>
+      <c r="CR20" s="14"/>
       <c r="CS20" s="45"/>
       <c r="CT20" s="45"/>
       <c r="CU20" s="45"/>
     </row>
-    <row r="21" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A21" s="49"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="45"/>
+    <row r="21" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="A21" s="47"/>
+      <c r="B21" s="52"/>
+      <c r="C21" s="52"/>
       <c r="E21" s="45"/>
       <c r="F21" s="45"/>
       <c r="G21" s="45"/>
@@ -4337,7 +4533,7 @@
       <c r="W21" s="45"/>
       <c r="X21" s="45"/>
       <c r="Y21" s="45"/>
-      <c r="Z21" s="45"/>
+      <c r="Z21" s="14"/>
       <c r="AA21" s="45"/>
       <c r="AB21" s="45"/>
       <c r="AC21" s="45"/>
@@ -4360,14 +4556,14 @@
       <c r="AT21" s="45"/>
       <c r="AU21" s="45"/>
       <c r="AV21" s="45"/>
-      <c r="AW21" s="45"/>
+      <c r="AW21" s="14"/>
       <c r="AX21" s="45"/>
       <c r="AY21" s="45"/>
       <c r="AZ21" s="45"/>
       <c r="BA21" s="45"/>
       <c r="BB21" s="45"/>
       <c r="BC21" s="45"/>
-      <c r="BD21" s="45"/>
+      <c r="BD21" s="14"/>
       <c r="BE21" s="45"/>
       <c r="BF21" s="45"/>
       <c r="BG21" s="45"/>
@@ -4381,14 +4577,14 @@
       <c r="BO21" s="45"/>
       <c r="BP21" s="45"/>
       <c r="BQ21" s="45"/>
-      <c r="BR21" s="45"/>
+      <c r="BR21" s="14"/>
       <c r="BS21" s="45"/>
       <c r="BT21" s="45"/>
       <c r="BU21" s="45"/>
       <c r="BV21" s="45"/>
       <c r="BW21" s="45"/>
       <c r="BX21" s="45"/>
-      <c r="BY21" s="45"/>
+      <c r="BY21" s="14"/>
       <c r="BZ21" s="45"/>
       <c r="CA21" s="45"/>
       <c r="CB21" s="45"/>
@@ -4399,7 +4595,7 @@
       <c r="CG21" s="45"/>
       <c r="CH21" s="45"/>
       <c r="CI21" s="45"/>
-      <c r="CJ21" s="45"/>
+      <c r="CJ21" s="14"/>
       <c r="CK21" s="45"/>
       <c r="CL21" s="45"/>
       <c r="CM21" s="45"/>
@@ -4407,16 +4603,15 @@
       <c r="CO21" s="45"/>
       <c r="CP21" s="45"/>
       <c r="CQ21" s="45"/>
-      <c r="CR21" s="45"/>
+      <c r="CR21" s="14"/>
       <c r="CS21" s="45"/>
       <c r="CT21" s="45"/>
       <c r="CU21" s="45"/>
     </row>
-    <row r="22" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A22" s="49"/>
-      <c r="B22" s="48"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="45"/>
+    <row r="22" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="A22" s="47"/>
+      <c r="B22" s="52"/>
+      <c r="C22" s="52"/>
       <c r="E22" s="45"/>
       <c r="F22" s="45"/>
       <c r="G22" s="45"/>
@@ -4438,7 +4633,7 @@
       <c r="W22" s="45"/>
       <c r="X22" s="45"/>
       <c r="Y22" s="45"/>
-      <c r="Z22" s="45"/>
+      <c r="Z22" s="14"/>
       <c r="AA22" s="45"/>
       <c r="AB22" s="45"/>
       <c r="AC22" s="45"/>
@@ -4461,14 +4656,14 @@
       <c r="AT22" s="45"/>
       <c r="AU22" s="45"/>
       <c r="AV22" s="45"/>
-      <c r="AW22" s="45"/>
+      <c r="AW22" s="14"/>
       <c r="AX22" s="45"/>
       <c r="AY22" s="45"/>
       <c r="AZ22" s="45"/>
       <c r="BA22" s="45"/>
       <c r="BB22" s="45"/>
       <c r="BC22" s="45"/>
-      <c r="BD22" s="45"/>
+      <c r="BD22" s="14"/>
       <c r="BE22" s="45"/>
       <c r="BF22" s="45"/>
       <c r="BG22" s="45"/>
@@ -4482,14 +4677,14 @@
       <c r="BO22" s="45"/>
       <c r="BP22" s="45"/>
       <c r="BQ22" s="45"/>
-      <c r="BR22" s="45"/>
+      <c r="BR22" s="14"/>
       <c r="BS22" s="45"/>
       <c r="BT22" s="45"/>
       <c r="BU22" s="45"/>
       <c r="BV22" s="45"/>
       <c r="BW22" s="45"/>
       <c r="BX22" s="45"/>
-      <c r="BY22" s="45"/>
+      <c r="BY22" s="14"/>
       <c r="BZ22" s="45"/>
       <c r="CA22" s="45"/>
       <c r="CB22" s="45"/>
@@ -4500,7 +4695,7 @@
       <c r="CG22" s="45"/>
       <c r="CH22" s="45"/>
       <c r="CI22" s="45"/>
-      <c r="CJ22" s="45"/>
+      <c r="CJ22" s="14"/>
       <c r="CK22" s="45"/>
       <c r="CL22" s="45"/>
       <c r="CM22" s="45"/>
@@ -4508,16 +4703,15 @@
       <c r="CO22" s="45"/>
       <c r="CP22" s="45"/>
       <c r="CQ22" s="45"/>
-      <c r="CR22" s="45"/>
+      <c r="CR22" s="14"/>
       <c r="CS22" s="45"/>
       <c r="CT22" s="45"/>
       <c r="CU22" s="45"/>
     </row>
-    <row r="23" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A23" s="49"/>
-      <c r="B23" s="48"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="45"/>
+    <row r="23" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="A23" s="47"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="52"/>
       <c r="E23" s="45"/>
       <c r="F23" s="45"/>
       <c r="G23" s="45"/>
@@ -4539,7 +4733,7 @@
       <c r="W23" s="45"/>
       <c r="X23" s="45"/>
       <c r="Y23" s="45"/>
-      <c r="Z23" s="45"/>
+      <c r="Z23" s="14"/>
       <c r="AA23" s="45"/>
       <c r="AB23" s="45"/>
       <c r="AC23" s="45"/>
@@ -4562,14 +4756,14 @@
       <c r="AT23" s="45"/>
       <c r="AU23" s="45"/>
       <c r="AV23" s="45"/>
-      <c r="AW23" s="45"/>
+      <c r="AW23" s="14"/>
       <c r="AX23" s="45"/>
       <c r="AY23" s="45"/>
       <c r="AZ23" s="45"/>
       <c r="BA23" s="45"/>
       <c r="BB23" s="45"/>
       <c r="BC23" s="45"/>
-      <c r="BD23" s="45"/>
+      <c r="BD23" s="14"/>
       <c r="BE23" s="45"/>
       <c r="BF23" s="45"/>
       <c r="BG23" s="45"/>
@@ -4583,14 +4777,14 @@
       <c r="BO23" s="45"/>
       <c r="BP23" s="45"/>
       <c r="BQ23" s="45"/>
-      <c r="BR23" s="45"/>
+      <c r="BR23" s="14"/>
       <c r="BS23" s="45"/>
       <c r="BT23" s="45"/>
       <c r="BU23" s="45"/>
       <c r="BV23" s="45"/>
       <c r="BW23" s="45"/>
       <c r="BX23" s="45"/>
-      <c r="BY23" s="45"/>
+      <c r="BY23" s="14"/>
       <c r="BZ23" s="45"/>
       <c r="CA23" s="45"/>
       <c r="CB23" s="45"/>
@@ -4601,7 +4795,7 @@
       <c r="CG23" s="45"/>
       <c r="CH23" s="45"/>
       <c r="CI23" s="45"/>
-      <c r="CJ23" s="45"/>
+      <c r="CJ23" s="14"/>
       <c r="CK23" s="45"/>
       <c r="CL23" s="45"/>
       <c r="CM23" s="45"/>
@@ -4609,16 +4803,15 @@
       <c r="CO23" s="45"/>
       <c r="CP23" s="45"/>
       <c r="CQ23" s="45"/>
-      <c r="CR23" s="45"/>
+      <c r="CR23" s="14"/>
       <c r="CS23" s="45"/>
       <c r="CT23" s="45"/>
       <c r="CU23" s="45"/>
     </row>
-    <row r="24" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A24" s="49"/>
-      <c r="B24" s="48"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="45"/>
+    <row r="24" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="A24" s="47"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="52"/>
       <c r="E24" s="45"/>
       <c r="F24" s="45"/>
       <c r="G24" s="45"/>
@@ -4640,7 +4833,7 @@
       <c r="W24" s="45"/>
       <c r="X24" s="45"/>
       <c r="Y24" s="45"/>
-      <c r="Z24" s="45"/>
+      <c r="Z24" s="14"/>
       <c r="AA24" s="45"/>
       <c r="AB24" s="45"/>
       <c r="AC24" s="45"/>
@@ -4663,14 +4856,14 @@
       <c r="AT24" s="45"/>
       <c r="AU24" s="45"/>
       <c r="AV24" s="45"/>
-      <c r="AW24" s="45"/>
+      <c r="AW24" s="14"/>
       <c r="AX24" s="45"/>
       <c r="AY24" s="45"/>
       <c r="AZ24" s="45"/>
       <c r="BA24" s="45"/>
       <c r="BB24" s="45"/>
       <c r="BC24" s="45"/>
-      <c r="BD24" s="45"/>
+      <c r="BD24" s="14"/>
       <c r="BE24" s="45"/>
       <c r="BF24" s="45"/>
       <c r="BG24" s="45"/>
@@ -4684,14 +4877,14 @@
       <c r="BO24" s="45"/>
       <c r="BP24" s="45"/>
       <c r="BQ24" s="45"/>
-      <c r="BR24" s="45"/>
+      <c r="BR24" s="14"/>
       <c r="BS24" s="45"/>
       <c r="BT24" s="45"/>
       <c r="BU24" s="45"/>
       <c r="BV24" s="45"/>
       <c r="BW24" s="45"/>
       <c r="BX24" s="45"/>
-      <c r="BY24" s="45"/>
+      <c r="BY24" s="14"/>
       <c r="BZ24" s="45"/>
       <c r="CA24" s="45"/>
       <c r="CB24" s="45"/>
@@ -4702,7 +4895,7 @@
       <c r="CG24" s="45"/>
       <c r="CH24" s="45"/>
       <c r="CI24" s="45"/>
-      <c r="CJ24" s="45"/>
+      <c r="CJ24" s="14"/>
       <c r="CK24" s="45"/>
       <c r="CL24" s="45"/>
       <c r="CM24" s="45"/>
@@ -4710,16 +4903,15 @@
       <c r="CO24" s="45"/>
       <c r="CP24" s="45"/>
       <c r="CQ24" s="45"/>
-      <c r="CR24" s="45"/>
+      <c r="CR24" s="14"/>
       <c r="CS24" s="45"/>
       <c r="CT24" s="45"/>
       <c r="CU24" s="45"/>
     </row>
-    <row r="25" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A25" s="49"/>
-      <c r="B25" s="48"/>
-      <c r="C25" s="47"/>
-      <c r="D25" s="45"/>
+    <row r="25" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="A25" s="47"/>
+      <c r="B25" s="52"/>
+      <c r="C25" s="52"/>
       <c r="E25" s="45"/>
       <c r="F25" s="45"/>
       <c r="G25" s="45"/>
@@ -4741,7 +4933,7 @@
       <c r="W25" s="45"/>
       <c r="X25" s="45"/>
       <c r="Y25" s="45"/>
-      <c r="Z25" s="45"/>
+      <c r="Z25" s="14"/>
       <c r="AA25" s="45"/>
       <c r="AB25" s="45"/>
       <c r="AC25" s="45"/>
@@ -4764,14 +4956,14 @@
       <c r="AT25" s="45"/>
       <c r="AU25" s="45"/>
       <c r="AV25" s="45"/>
-      <c r="AW25" s="45"/>
+      <c r="AW25" s="14"/>
       <c r="AX25" s="45"/>
       <c r="AY25" s="45"/>
       <c r="AZ25" s="45"/>
       <c r="BA25" s="45"/>
       <c r="BB25" s="45"/>
       <c r="BC25" s="45"/>
-      <c r="BD25" s="45"/>
+      <c r="BD25" s="14"/>
       <c r="BE25" s="45"/>
       <c r="BF25" s="45"/>
       <c r="BG25" s="45"/>
@@ -4785,14 +4977,14 @@
       <c r="BO25" s="45"/>
       <c r="BP25" s="45"/>
       <c r="BQ25" s="45"/>
-      <c r="BR25" s="45"/>
+      <c r="BR25" s="14"/>
       <c r="BS25" s="45"/>
       <c r="BT25" s="45"/>
       <c r="BU25" s="45"/>
       <c r="BV25" s="45"/>
       <c r="BW25" s="45"/>
       <c r="BX25" s="45"/>
-      <c r="BY25" s="45"/>
+      <c r="BY25" s="14"/>
       <c r="BZ25" s="45"/>
       <c r="CA25" s="45"/>
       <c r="CB25" s="45"/>
@@ -4803,7 +4995,7 @@
       <c r="CG25" s="45"/>
       <c r="CH25" s="45"/>
       <c r="CI25" s="45"/>
-      <c r="CJ25" s="45"/>
+      <c r="CJ25" s="14"/>
       <c r="CK25" s="45"/>
       <c r="CL25" s="45"/>
       <c r="CM25" s="45"/>
@@ -4811,16 +5003,15 @@
       <c r="CO25" s="45"/>
       <c r="CP25" s="45"/>
       <c r="CQ25" s="45"/>
-      <c r="CR25" s="45"/>
+      <c r="CR25" s="14"/>
       <c r="CS25" s="45"/>
       <c r="CT25" s="45"/>
       <c r="CU25" s="45"/>
     </row>
-    <row r="26" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A26" s="49"/>
-      <c r="B26" s="48"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="45"/>
+    <row r="26" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="A26" s="47"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="52"/>
       <c r="E26" s="45"/>
       <c r="F26" s="45"/>
       <c r="G26" s="45"/>
@@ -4842,7 +5033,7 @@
       <c r="W26" s="45"/>
       <c r="X26" s="45"/>
       <c r="Y26" s="45"/>
-      <c r="Z26" s="45"/>
+      <c r="Z26" s="14"/>
       <c r="AA26" s="45"/>
       <c r="AB26" s="45"/>
       <c r="AC26" s="45"/>
@@ -4865,14 +5056,14 @@
       <c r="AT26" s="45"/>
       <c r="AU26" s="45"/>
       <c r="AV26" s="45"/>
-      <c r="AW26" s="45"/>
+      <c r="AW26" s="14"/>
       <c r="AX26" s="45"/>
       <c r="AY26" s="45"/>
       <c r="AZ26" s="45"/>
       <c r="BA26" s="45"/>
       <c r="BB26" s="45"/>
       <c r="BC26" s="45"/>
-      <c r="BD26" s="45"/>
+      <c r="BD26" s="14"/>
       <c r="BE26" s="45"/>
       <c r="BF26" s="45"/>
       <c r="BG26" s="45"/>
@@ -4886,14 +5077,14 @@
       <c r="BO26" s="45"/>
       <c r="BP26" s="45"/>
       <c r="BQ26" s="45"/>
-      <c r="BR26" s="45"/>
+      <c r="BR26" s="14"/>
       <c r="BS26" s="45"/>
       <c r="BT26" s="45"/>
       <c r="BU26" s="45"/>
       <c r="BV26" s="45"/>
       <c r="BW26" s="45"/>
       <c r="BX26" s="45"/>
-      <c r="BY26" s="45"/>
+      <c r="BY26" s="14"/>
       <c r="BZ26" s="45"/>
       <c r="CA26" s="45"/>
       <c r="CB26" s="45"/>
@@ -4904,7 +5095,7 @@
       <c r="CG26" s="45"/>
       <c r="CH26" s="45"/>
       <c r="CI26" s="45"/>
-      <c r="CJ26" s="45"/>
+      <c r="CJ26" s="14"/>
       <c r="CK26" s="45"/>
       <c r="CL26" s="45"/>
       <c r="CM26" s="45"/>
@@ -4912,16 +5103,15 @@
       <c r="CO26" s="45"/>
       <c r="CP26" s="45"/>
       <c r="CQ26" s="45"/>
-      <c r="CR26" s="45"/>
+      <c r="CR26" s="14"/>
       <c r="CS26" s="45"/>
       <c r="CT26" s="45"/>
       <c r="CU26" s="45"/>
     </row>
-    <row r="27" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A27" s="49"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="45"/>
+    <row r="27" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="A27" s="47"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="52"/>
       <c r="E27" s="45"/>
       <c r="F27" s="45"/>
       <c r="G27" s="45"/>
@@ -4943,7 +5133,7 @@
       <c r="W27" s="45"/>
       <c r="X27" s="45"/>
       <c r="Y27" s="45"/>
-      <c r="Z27" s="45"/>
+      <c r="Z27" s="14"/>
       <c r="AA27" s="45"/>
       <c r="AB27" s="45"/>
       <c r="AC27" s="45"/>
@@ -4966,14 +5156,14 @@
       <c r="AT27" s="45"/>
       <c r="AU27" s="45"/>
       <c r="AV27" s="45"/>
-      <c r="AW27" s="45"/>
+      <c r="AW27" s="14"/>
       <c r="AX27" s="45"/>
       <c r="AY27" s="45"/>
       <c r="AZ27" s="45"/>
       <c r="BA27" s="45"/>
       <c r="BB27" s="45"/>
       <c r="BC27" s="45"/>
-      <c r="BD27" s="45"/>
+      <c r="BD27" s="14"/>
       <c r="BE27" s="45"/>
       <c r="BF27" s="45"/>
       <c r="BG27" s="45"/>
@@ -4987,14 +5177,14 @@
       <c r="BO27" s="45"/>
       <c r="BP27" s="45"/>
       <c r="BQ27" s="45"/>
-      <c r="BR27" s="45"/>
+      <c r="BR27" s="14"/>
       <c r="BS27" s="45"/>
       <c r="BT27" s="45"/>
       <c r="BU27" s="45"/>
       <c r="BV27" s="45"/>
       <c r="BW27" s="45"/>
       <c r="BX27" s="45"/>
-      <c r="BY27" s="45"/>
+      <c r="BY27" s="14"/>
       <c r="BZ27" s="45"/>
       <c r="CA27" s="45"/>
       <c r="CB27" s="45"/>
@@ -5005,7 +5195,7 @@
       <c r="CG27" s="45"/>
       <c r="CH27" s="45"/>
       <c r="CI27" s="45"/>
-      <c r="CJ27" s="45"/>
+      <c r="CJ27" s="14"/>
       <c r="CK27" s="45"/>
       <c r="CL27" s="45"/>
       <c r="CM27" s="45"/>
@@ -5013,16 +5203,15 @@
       <c r="CO27" s="45"/>
       <c r="CP27" s="45"/>
       <c r="CQ27" s="45"/>
-      <c r="CR27" s="45"/>
+      <c r="CR27" s="14"/>
       <c r="CS27" s="45"/>
       <c r="CT27" s="45"/>
       <c r="CU27" s="45"/>
     </row>
-    <row r="28" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A28" s="49"/>
-      <c r="B28" s="48"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="45"/>
+    <row r="28" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="A28" s="47"/>
+      <c r="B28" s="52"/>
+      <c r="C28" s="52"/>
       <c r="E28" s="45"/>
       <c r="F28" s="45"/>
       <c r="G28" s="45"/>
@@ -5044,7 +5233,7 @@
       <c r="W28" s="45"/>
       <c r="X28" s="45"/>
       <c r="Y28" s="45"/>
-      <c r="Z28" s="45"/>
+      <c r="Z28" s="14"/>
       <c r="AA28" s="45"/>
       <c r="AB28" s="45"/>
       <c r="AC28" s="45"/>
@@ -5067,14 +5256,14 @@
       <c r="AT28" s="45"/>
       <c r="AU28" s="45"/>
       <c r="AV28" s="45"/>
-      <c r="AW28" s="45"/>
+      <c r="AW28" s="14"/>
       <c r="AX28" s="45"/>
       <c r="AY28" s="45"/>
       <c r="AZ28" s="45"/>
       <c r="BA28" s="45"/>
       <c r="BB28" s="45"/>
       <c r="BC28" s="45"/>
-      <c r="BD28" s="45"/>
+      <c r="BD28" s="14"/>
       <c r="BE28" s="45"/>
       <c r="BF28" s="45"/>
       <c r="BG28" s="45"/>
@@ -5088,14 +5277,14 @@
       <c r="BO28" s="45"/>
       <c r="BP28" s="45"/>
       <c r="BQ28" s="45"/>
-      <c r="BR28" s="45"/>
+      <c r="BR28" s="14"/>
       <c r="BS28" s="45"/>
       <c r="BT28" s="45"/>
       <c r="BU28" s="45"/>
       <c r="BV28" s="45"/>
       <c r="BW28" s="45"/>
       <c r="BX28" s="45"/>
-      <c r="BY28" s="45"/>
+      <c r="BY28" s="14"/>
       <c r="BZ28" s="45"/>
       <c r="CA28" s="45"/>
       <c r="CB28" s="45"/>
@@ -5106,7 +5295,7 @@
       <c r="CG28" s="45"/>
       <c r="CH28" s="45"/>
       <c r="CI28" s="45"/>
-      <c r="CJ28" s="45"/>
+      <c r="CJ28" s="14"/>
       <c r="CK28" s="45"/>
       <c r="CL28" s="45"/>
       <c r="CM28" s="45"/>
@@ -5114,16 +5303,15 @@
       <c r="CO28" s="45"/>
       <c r="CP28" s="45"/>
       <c r="CQ28" s="45"/>
-      <c r="CR28" s="45"/>
+      <c r="CR28" s="14"/>
       <c r="CS28" s="45"/>
       <c r="CT28" s="45"/>
       <c r="CU28" s="45"/>
     </row>
-    <row r="29" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A29" s="49"/>
-      <c r="B29" s="48"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="45"/>
+    <row r="29" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="A29" s="47"/>
+      <c r="B29" s="52"/>
+      <c r="C29" s="52"/>
       <c r="E29" s="45"/>
       <c r="F29" s="45"/>
       <c r="G29" s="45"/>
@@ -5145,7 +5333,7 @@
       <c r="W29" s="45"/>
       <c r="X29" s="45"/>
       <c r="Y29" s="45"/>
-      <c r="Z29" s="45"/>
+      <c r="Z29" s="14"/>
       <c r="AA29" s="45"/>
       <c r="AB29" s="45"/>
       <c r="AC29" s="45"/>
@@ -5168,14 +5356,14 @@
       <c r="AT29" s="45"/>
       <c r="AU29" s="45"/>
       <c r="AV29" s="45"/>
-      <c r="AW29" s="45"/>
+      <c r="AW29" s="14"/>
       <c r="AX29" s="45"/>
       <c r="AY29" s="45"/>
       <c r="AZ29" s="45"/>
       <c r="BA29" s="45"/>
       <c r="BB29" s="45"/>
       <c r="BC29" s="45"/>
-      <c r="BD29" s="45"/>
+      <c r="BD29" s="14"/>
       <c r="BE29" s="45"/>
       <c r="BF29" s="45"/>
       <c r="BG29" s="45"/>
@@ -5189,14 +5377,14 @@
       <c r="BO29" s="45"/>
       <c r="BP29" s="45"/>
       <c r="BQ29" s="45"/>
-      <c r="BR29" s="45"/>
+      <c r="BR29" s="14"/>
       <c r="BS29" s="45"/>
       <c r="BT29" s="45"/>
       <c r="BU29" s="45"/>
       <c r="BV29" s="45"/>
       <c r="BW29" s="45"/>
       <c r="BX29" s="45"/>
-      <c r="BY29" s="45"/>
+      <c r="BY29" s="14"/>
       <c r="BZ29" s="45"/>
       <c r="CA29" s="45"/>
       <c r="CB29" s="45"/>
@@ -5207,7 +5395,7 @@
       <c r="CG29" s="45"/>
       <c r="CH29" s="45"/>
       <c r="CI29" s="45"/>
-      <c r="CJ29" s="45"/>
+      <c r="CJ29" s="14"/>
       <c r="CK29" s="45"/>
       <c r="CL29" s="45"/>
       <c r="CM29" s="45"/>
@@ -5215,16 +5403,15 @@
       <c r="CO29" s="45"/>
       <c r="CP29" s="45"/>
       <c r="CQ29" s="45"/>
-      <c r="CR29" s="45"/>
+      <c r="CR29" s="14"/>
       <c r="CS29" s="45"/>
       <c r="CT29" s="45"/>
       <c r="CU29" s="45"/>
     </row>
-    <row r="30" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A30" s="49"/>
-      <c r="B30" s="48"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="45"/>
+    <row r="30" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="A30" s="47"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="52"/>
       <c r="E30" s="45"/>
       <c r="F30" s="45"/>
       <c r="G30" s="45"/>
@@ -5246,7 +5433,7 @@
       <c r="W30" s="45"/>
       <c r="X30" s="45"/>
       <c r="Y30" s="45"/>
-      <c r="Z30" s="45"/>
+      <c r="Z30" s="14"/>
       <c r="AA30" s="45"/>
       <c r="AB30" s="45"/>
       <c r="AC30" s="45"/>
@@ -5269,14 +5456,14 @@
       <c r="AT30" s="45"/>
       <c r="AU30" s="45"/>
       <c r="AV30" s="45"/>
-      <c r="AW30" s="45"/>
+      <c r="AW30" s="14"/>
       <c r="AX30" s="45"/>
       <c r="AY30" s="45"/>
       <c r="AZ30" s="45"/>
       <c r="BA30" s="45"/>
       <c r="BB30" s="45"/>
       <c r="BC30" s="45"/>
-      <c r="BD30" s="45"/>
+      <c r="BD30" s="14"/>
       <c r="BE30" s="45"/>
       <c r="BF30" s="45"/>
       <c r="BG30" s="45"/>
@@ -5290,14 +5477,14 @@
       <c r="BO30" s="45"/>
       <c r="BP30" s="45"/>
       <c r="BQ30" s="45"/>
-      <c r="BR30" s="45"/>
+      <c r="BR30" s="14"/>
       <c r="BS30" s="45"/>
       <c r="BT30" s="45"/>
       <c r="BU30" s="45"/>
       <c r="BV30" s="45"/>
       <c r="BW30" s="45"/>
       <c r="BX30" s="45"/>
-      <c r="BY30" s="45"/>
+      <c r="BY30" s="14"/>
       <c r="BZ30" s="45"/>
       <c r="CA30" s="45"/>
       <c r="CB30" s="45"/>
@@ -5308,7 +5495,7 @@
       <c r="CG30" s="45"/>
       <c r="CH30" s="45"/>
       <c r="CI30" s="45"/>
-      <c r="CJ30" s="45"/>
+      <c r="CJ30" s="14"/>
       <c r="CK30" s="45"/>
       <c r="CL30" s="45"/>
       <c r="CM30" s="45"/>
@@ -5316,16 +5503,15 @@
       <c r="CO30" s="45"/>
       <c r="CP30" s="45"/>
       <c r="CQ30" s="45"/>
-      <c r="CR30" s="45"/>
+      <c r="CR30" s="14"/>
       <c r="CS30" s="45"/>
       <c r="CT30" s="45"/>
       <c r="CU30" s="45"/>
     </row>
-    <row r="31" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A31" s="49"/>
-      <c r="B31" s="48"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="45"/>
+    <row r="31" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="A31" s="47"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="52"/>
       <c r="E31" s="45"/>
       <c r="F31" s="45"/>
       <c r="G31" s="45"/>
@@ -5347,7 +5533,7 @@
       <c r="W31" s="45"/>
       <c r="X31" s="45"/>
       <c r="Y31" s="45"/>
-      <c r="Z31" s="45"/>
+      <c r="Z31" s="14"/>
       <c r="AA31" s="45"/>
       <c r="AB31" s="45"/>
       <c r="AC31" s="45"/>
@@ -5370,14 +5556,14 @@
       <c r="AT31" s="45"/>
       <c r="AU31" s="45"/>
       <c r="AV31" s="45"/>
-      <c r="AW31" s="45"/>
+      <c r="AW31" s="14"/>
       <c r="AX31" s="45"/>
       <c r="AY31" s="45"/>
       <c r="AZ31" s="45"/>
       <c r="BA31" s="45"/>
       <c r="BB31" s="45"/>
       <c r="BC31" s="45"/>
-      <c r="BD31" s="45"/>
+      <c r="BD31" s="14"/>
       <c r="BE31" s="45"/>
       <c r="BF31" s="45"/>
       <c r="BG31" s="45"/>
@@ -5391,14 +5577,14 @@
       <c r="BO31" s="45"/>
       <c r="BP31" s="45"/>
       <c r="BQ31" s="45"/>
-      <c r="BR31" s="45"/>
+      <c r="BR31" s="14"/>
       <c r="BS31" s="45"/>
       <c r="BT31" s="45"/>
       <c r="BU31" s="45"/>
       <c r="BV31" s="45"/>
       <c r="BW31" s="45"/>
       <c r="BX31" s="45"/>
-      <c r="BY31" s="45"/>
+      <c r="BY31" s="14"/>
       <c r="BZ31" s="45"/>
       <c r="CA31" s="45"/>
       <c r="CB31" s="45"/>
@@ -5409,7 +5595,7 @@
       <c r="CG31" s="45"/>
       <c r="CH31" s="45"/>
       <c r="CI31" s="45"/>
-      <c r="CJ31" s="45"/>
+      <c r="CJ31" s="14"/>
       <c r="CK31" s="45"/>
       <c r="CL31" s="45"/>
       <c r="CM31" s="45"/>
@@ -5417,16 +5603,15 @@
       <c r="CO31" s="45"/>
       <c r="CP31" s="45"/>
       <c r="CQ31" s="45"/>
-      <c r="CR31" s="45"/>
+      <c r="CR31" s="14"/>
       <c r="CS31" s="45"/>
       <c r="CT31" s="45"/>
       <c r="CU31" s="45"/>
     </row>
-    <row r="32" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A32" s="49"/>
-      <c r="B32" s="48"/>
-      <c r="C32" s="47"/>
-      <c r="D32" s="45"/>
+    <row r="32" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="A32" s="47"/>
+      <c r="B32" s="52"/>
+      <c r="C32" s="52"/>
       <c r="E32" s="45"/>
       <c r="F32" s="45"/>
       <c r="G32" s="45"/>
@@ -5448,7 +5633,7 @@
       <c r="W32" s="45"/>
       <c r="X32" s="45"/>
       <c r="Y32" s="45"/>
-      <c r="Z32" s="45"/>
+      <c r="Z32" s="14"/>
       <c r="AA32" s="45"/>
       <c r="AB32" s="45"/>
       <c r="AC32" s="45"/>
@@ -5471,14 +5656,14 @@
       <c r="AT32" s="45"/>
       <c r="AU32" s="45"/>
       <c r="AV32" s="45"/>
-      <c r="AW32" s="45"/>
+      <c r="AW32" s="14"/>
       <c r="AX32" s="45"/>
       <c r="AY32" s="45"/>
       <c r="AZ32" s="45"/>
       <c r="BA32" s="45"/>
       <c r="BB32" s="45"/>
       <c r="BC32" s="45"/>
-      <c r="BD32" s="45"/>
+      <c r="BD32" s="14"/>
       <c r="BE32" s="45"/>
       <c r="BF32" s="45"/>
       <c r="BG32" s="45"/>
@@ -5492,14 +5677,14 @@
       <c r="BO32" s="45"/>
       <c r="BP32" s="45"/>
       <c r="BQ32" s="45"/>
-      <c r="BR32" s="45"/>
+      <c r="BR32" s="14"/>
       <c r="BS32" s="45"/>
       <c r="BT32" s="45"/>
       <c r="BU32" s="45"/>
       <c r="BV32" s="45"/>
       <c r="BW32" s="45"/>
       <c r="BX32" s="45"/>
-      <c r="BY32" s="45"/>
+      <c r="BY32" s="14"/>
       <c r="BZ32" s="45"/>
       <c r="CA32" s="45"/>
       <c r="CB32" s="45"/>
@@ -5510,7 +5695,7 @@
       <c r="CG32" s="45"/>
       <c r="CH32" s="45"/>
       <c r="CI32" s="45"/>
-      <c r="CJ32" s="45"/>
+      <c r="CJ32" s="14"/>
       <c r="CK32" s="45"/>
       <c r="CL32" s="45"/>
       <c r="CM32" s="45"/>
@@ -5518,16 +5703,15 @@
       <c r="CO32" s="45"/>
       <c r="CP32" s="45"/>
       <c r="CQ32" s="45"/>
-      <c r="CR32" s="45"/>
+      <c r="CR32" s="14"/>
       <c r="CS32" s="45"/>
       <c r="CT32" s="45"/>
       <c r="CU32" s="45"/>
     </row>
-    <row r="33" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A33" s="49"/>
-      <c r="B33" s="48"/>
-      <c r="C33" s="47"/>
-      <c r="D33" s="45"/>
+    <row r="33" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="A33" s="47"/>
+      <c r="B33" s="52"/>
+      <c r="C33" s="52"/>
       <c r="E33" s="45"/>
       <c r="F33" s="45"/>
       <c r="G33" s="45"/>
@@ -5549,7 +5733,7 @@
       <c r="W33" s="45"/>
       <c r="X33" s="45"/>
       <c r="Y33" s="45"/>
-      <c r="Z33" s="45"/>
+      <c r="Z33" s="14"/>
       <c r="AA33" s="45"/>
       <c r="AB33" s="45"/>
       <c r="AC33" s="45"/>
@@ -5572,14 +5756,14 @@
       <c r="AT33" s="45"/>
       <c r="AU33" s="45"/>
       <c r="AV33" s="45"/>
-      <c r="AW33" s="45"/>
+      <c r="AW33" s="14"/>
       <c r="AX33" s="45"/>
       <c r="AY33" s="45"/>
       <c r="AZ33" s="45"/>
       <c r="BA33" s="45"/>
       <c r="BB33" s="45"/>
       <c r="BC33" s="45"/>
-      <c r="BD33" s="45"/>
+      <c r="BD33" s="14"/>
       <c r="BE33" s="45"/>
       <c r="BF33" s="45"/>
       <c r="BG33" s="45"/>
@@ -5593,14 +5777,14 @@
       <c r="BO33" s="45"/>
       <c r="BP33" s="45"/>
       <c r="BQ33" s="45"/>
-      <c r="BR33" s="45"/>
+      <c r="BR33" s="14"/>
       <c r="BS33" s="45"/>
       <c r="BT33" s="45"/>
       <c r="BU33" s="45"/>
       <c r="BV33" s="45"/>
       <c r="BW33" s="45"/>
       <c r="BX33" s="45"/>
-      <c r="BY33" s="45"/>
+      <c r="BY33" s="14"/>
       <c r="BZ33" s="45"/>
       <c r="CA33" s="45"/>
       <c r="CB33" s="45"/>
@@ -5611,7 +5795,7 @@
       <c r="CG33" s="45"/>
       <c r="CH33" s="45"/>
       <c r="CI33" s="45"/>
-      <c r="CJ33" s="45"/>
+      <c r="CJ33" s="14"/>
       <c r="CK33" s="45"/>
       <c r="CL33" s="45"/>
       <c r="CM33" s="45"/>
@@ -5619,16 +5803,15 @@
       <c r="CO33" s="45"/>
       <c r="CP33" s="45"/>
       <c r="CQ33" s="45"/>
-      <c r="CR33" s="45"/>
+      <c r="CR33" s="14"/>
       <c r="CS33" s="45"/>
       <c r="CT33" s="45"/>
       <c r="CU33" s="45"/>
     </row>
-    <row r="34" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A34" s="49"/>
-      <c r="B34" s="48"/>
-      <c r="C34" s="47"/>
-      <c r="D34" s="45"/>
+    <row r="34" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="A34" s="47"/>
+      <c r="B34" s="52"/>
+      <c r="C34" s="52"/>
       <c r="E34" s="45"/>
       <c r="F34" s="45"/>
       <c r="G34" s="45"/>
@@ -5650,7 +5833,7 @@
       <c r="W34" s="45"/>
       <c r="X34" s="45"/>
       <c r="Y34" s="45"/>
-      <c r="Z34" s="45"/>
+      <c r="Z34" s="14"/>
       <c r="AA34" s="45"/>
       <c r="AB34" s="45"/>
       <c r="AC34" s="45"/>
@@ -5673,14 +5856,14 @@
       <c r="AT34" s="45"/>
       <c r="AU34" s="45"/>
       <c r="AV34" s="45"/>
-      <c r="AW34" s="45"/>
+      <c r="AW34" s="14"/>
       <c r="AX34" s="45"/>
       <c r="AY34" s="45"/>
       <c r="AZ34" s="45"/>
       <c r="BA34" s="45"/>
       <c r="BB34" s="45"/>
       <c r="BC34" s="45"/>
-      <c r="BD34" s="45"/>
+      <c r="BD34" s="14"/>
       <c r="BE34" s="45"/>
       <c r="BF34" s="45"/>
       <c r="BG34" s="45"/>
@@ -5694,14 +5877,14 @@
       <c r="BO34" s="45"/>
       <c r="BP34" s="45"/>
       <c r="BQ34" s="45"/>
-      <c r="BR34" s="45"/>
+      <c r="BR34" s="14"/>
       <c r="BS34" s="45"/>
       <c r="BT34" s="45"/>
       <c r="BU34" s="45"/>
       <c r="BV34" s="45"/>
       <c r="BW34" s="45"/>
       <c r="BX34" s="45"/>
-      <c r="BY34" s="45"/>
+      <c r="BY34" s="14"/>
       <c r="BZ34" s="45"/>
       <c r="CA34" s="45"/>
       <c r="CB34" s="45"/>
@@ -5712,7 +5895,7 @@
       <c r="CG34" s="45"/>
       <c r="CH34" s="45"/>
       <c r="CI34" s="45"/>
-      <c r="CJ34" s="45"/>
+      <c r="CJ34" s="14"/>
       <c r="CK34" s="45"/>
       <c r="CL34" s="45"/>
       <c r="CM34" s="45"/>
@@ -5720,16 +5903,15 @@
       <c r="CO34" s="45"/>
       <c r="CP34" s="45"/>
       <c r="CQ34" s="45"/>
-      <c r="CR34" s="45"/>
+      <c r="CR34" s="14"/>
       <c r="CS34" s="45"/>
       <c r="CT34" s="45"/>
       <c r="CU34" s="45"/>
     </row>
-    <row r="35" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A35" s="49"/>
-      <c r="B35" s="48"/>
-      <c r="C35" s="47"/>
-      <c r="D35" s="45"/>
+    <row r="35" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="A35" s="47"/>
+      <c r="B35" s="52"/>
+      <c r="C35" s="52"/>
       <c r="E35" s="45"/>
       <c r="F35" s="45"/>
       <c r="G35" s="45"/>
@@ -5751,7 +5933,7 @@
       <c r="W35" s="45"/>
       <c r="X35" s="45"/>
       <c r="Y35" s="45"/>
-      <c r="Z35" s="45"/>
+      <c r="Z35" s="14"/>
       <c r="AA35" s="45"/>
       <c r="AB35" s="45"/>
       <c r="AC35" s="45"/>
@@ -5774,14 +5956,14 @@
       <c r="AT35" s="45"/>
       <c r="AU35" s="45"/>
       <c r="AV35" s="45"/>
-      <c r="AW35" s="45"/>
+      <c r="AW35" s="14"/>
       <c r="AX35" s="45"/>
       <c r="AY35" s="45"/>
       <c r="AZ35" s="45"/>
       <c r="BA35" s="45"/>
       <c r="BB35" s="45"/>
       <c r="BC35" s="45"/>
-      <c r="BD35" s="45"/>
+      <c r="BD35" s="14"/>
       <c r="BE35" s="45"/>
       <c r="BF35" s="45"/>
       <c r="BG35" s="45"/>
@@ -5795,14 +5977,14 @@
       <c r="BO35" s="45"/>
       <c r="BP35" s="45"/>
       <c r="BQ35" s="45"/>
-      <c r="BR35" s="45"/>
+      <c r="BR35" s="14"/>
       <c r="BS35" s="45"/>
       <c r="BT35" s="45"/>
       <c r="BU35" s="45"/>
       <c r="BV35" s="45"/>
       <c r="BW35" s="45"/>
       <c r="BX35" s="45"/>
-      <c r="BY35" s="45"/>
+      <c r="BY35" s="14"/>
       <c r="BZ35" s="45"/>
       <c r="CA35" s="45"/>
       <c r="CB35" s="45"/>
@@ -5813,7 +5995,7 @@
       <c r="CG35" s="45"/>
       <c r="CH35" s="45"/>
       <c r="CI35" s="45"/>
-      <c r="CJ35" s="45"/>
+      <c r="CJ35" s="14"/>
       <c r="CK35" s="45"/>
       <c r="CL35" s="45"/>
       <c r="CM35" s="45"/>
@@ -5821,16 +6003,15 @@
       <c r="CO35" s="45"/>
       <c r="CP35" s="45"/>
       <c r="CQ35" s="45"/>
-      <c r="CR35" s="45"/>
+      <c r="CR35" s="14"/>
       <c r="CS35" s="45"/>
       <c r="CT35" s="45"/>
       <c r="CU35" s="45"/>
     </row>
-    <row r="36" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A36" s="49"/>
-      <c r="B36" s="48"/>
-      <c r="C36" s="47"/>
-      <c r="D36" s="45"/>
+    <row r="36" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="A36" s="47"/>
+      <c r="B36" s="52"/>
+      <c r="C36" s="52"/>
       <c r="E36" s="45"/>
       <c r="F36" s="45"/>
       <c r="G36" s="45"/>
@@ -5852,7 +6033,7 @@
       <c r="W36" s="45"/>
       <c r="X36" s="45"/>
       <c r="Y36" s="45"/>
-      <c r="Z36" s="45"/>
+      <c r="Z36" s="14"/>
       <c r="AA36" s="45"/>
       <c r="AB36" s="45"/>
       <c r="AC36" s="45"/>
@@ -5875,14 +6056,14 @@
       <c r="AT36" s="45"/>
       <c r="AU36" s="45"/>
       <c r="AV36" s="45"/>
-      <c r="AW36" s="45"/>
+      <c r="AW36" s="14"/>
       <c r="AX36" s="45"/>
       <c r="AY36" s="45"/>
       <c r="AZ36" s="45"/>
       <c r="BA36" s="45"/>
       <c r="BB36" s="45"/>
       <c r="BC36" s="45"/>
-      <c r="BD36" s="45"/>
+      <c r="BD36" s="14"/>
       <c r="BE36" s="45"/>
       <c r="BF36" s="45"/>
       <c r="BG36" s="45"/>
@@ -5896,14 +6077,14 @@
       <c r="BO36" s="45"/>
       <c r="BP36" s="45"/>
       <c r="BQ36" s="45"/>
-      <c r="BR36" s="45"/>
+      <c r="BR36" s="14"/>
       <c r="BS36" s="45"/>
       <c r="BT36" s="45"/>
       <c r="BU36" s="45"/>
       <c r="BV36" s="45"/>
       <c r="BW36" s="45"/>
       <c r="BX36" s="45"/>
-      <c r="BY36" s="45"/>
+      <c r="BY36" s="14"/>
       <c r="BZ36" s="45"/>
       <c r="CA36" s="45"/>
       <c r="CB36" s="45"/>
@@ -5914,7 +6095,7 @@
       <c r="CG36" s="45"/>
       <c r="CH36" s="45"/>
       <c r="CI36" s="45"/>
-      <c r="CJ36" s="45"/>
+      <c r="CJ36" s="14"/>
       <c r="CK36" s="45"/>
       <c r="CL36" s="45"/>
       <c r="CM36" s="45"/>
@@ -5922,16 +6103,15 @@
       <c r="CO36" s="45"/>
       <c r="CP36" s="45"/>
       <c r="CQ36" s="45"/>
-      <c r="CR36" s="45"/>
+      <c r="CR36" s="14"/>
       <c r="CS36" s="45"/>
       <c r="CT36" s="45"/>
       <c r="CU36" s="45"/>
     </row>
-    <row r="37" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A37" s="49"/>
-      <c r="B37" s="48"/>
-      <c r="C37" s="47"/>
-      <c r="D37" s="45"/>
+    <row r="37" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="A37" s="47"/>
+      <c r="B37" s="52"/>
+      <c r="C37" s="52"/>
       <c r="E37" s="45"/>
       <c r="F37" s="45"/>
       <c r="G37" s="45"/>
@@ -5953,7 +6133,7 @@
       <c r="W37" s="45"/>
       <c r="X37" s="45"/>
       <c r="Y37" s="45"/>
-      <c r="Z37" s="45"/>
+      <c r="Z37" s="14"/>
       <c r="AA37" s="45"/>
       <c r="AB37" s="45"/>
       <c r="AC37" s="45"/>
@@ -5976,14 +6156,14 @@
       <c r="AT37" s="45"/>
       <c r="AU37" s="45"/>
       <c r="AV37" s="45"/>
-      <c r="AW37" s="45"/>
+      <c r="AW37" s="14"/>
       <c r="AX37" s="45"/>
       <c r="AY37" s="45"/>
       <c r="AZ37" s="45"/>
       <c r="BA37" s="45"/>
       <c r="BB37" s="45"/>
       <c r="BC37" s="45"/>
-      <c r="BD37" s="45"/>
+      <c r="BD37" s="14"/>
       <c r="BE37" s="45"/>
       <c r="BF37" s="45"/>
       <c r="BG37" s="45"/>
@@ -5997,14 +6177,14 @@
       <c r="BO37" s="45"/>
       <c r="BP37" s="45"/>
       <c r="BQ37" s="45"/>
-      <c r="BR37" s="45"/>
+      <c r="BR37" s="14"/>
       <c r="BS37" s="45"/>
       <c r="BT37" s="45"/>
       <c r="BU37" s="45"/>
       <c r="BV37" s="45"/>
       <c r="BW37" s="45"/>
       <c r="BX37" s="45"/>
-      <c r="BY37" s="45"/>
+      <c r="BY37" s="14"/>
       <c r="BZ37" s="45"/>
       <c r="CA37" s="45"/>
       <c r="CB37" s="45"/>
@@ -6015,7 +6195,7 @@
       <c r="CG37" s="45"/>
       <c r="CH37" s="45"/>
       <c r="CI37" s="45"/>
-      <c r="CJ37" s="45"/>
+      <c r="CJ37" s="14"/>
       <c r="CK37" s="45"/>
       <c r="CL37" s="45"/>
       <c r="CM37" s="45"/>
@@ -6023,16 +6203,15 @@
       <c r="CO37" s="45"/>
       <c r="CP37" s="45"/>
       <c r="CQ37" s="45"/>
-      <c r="CR37" s="45"/>
+      <c r="CR37" s="14"/>
       <c r="CS37" s="45"/>
       <c r="CT37" s="45"/>
       <c r="CU37" s="45"/>
     </row>
-    <row r="38" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A38" s="49"/>
-      <c r="B38" s="48"/>
-      <c r="C38" s="47"/>
-      <c r="D38" s="45"/>
+    <row r="38" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="A38" s="47"/>
+      <c r="B38" s="52"/>
+      <c r="C38" s="52"/>
       <c r="E38" s="45"/>
       <c r="F38" s="45"/>
       <c r="G38" s="45"/>
@@ -6054,7 +6233,7 @@
       <c r="W38" s="45"/>
       <c r="X38" s="45"/>
       <c r="Y38" s="45"/>
-      <c r="Z38" s="45"/>
+      <c r="Z38" s="14"/>
       <c r="AA38" s="45"/>
       <c r="AB38" s="45"/>
       <c r="AC38" s="45"/>
@@ -6077,14 +6256,14 @@
       <c r="AT38" s="45"/>
       <c r="AU38" s="45"/>
       <c r="AV38" s="45"/>
-      <c r="AW38" s="45"/>
+      <c r="AW38" s="14"/>
       <c r="AX38" s="45"/>
       <c r="AY38" s="45"/>
       <c r="AZ38" s="45"/>
       <c r="BA38" s="45"/>
       <c r="BB38" s="45"/>
       <c r="BC38" s="45"/>
-      <c r="BD38" s="45"/>
+      <c r="BD38" s="14"/>
       <c r="BE38" s="45"/>
       <c r="BF38" s="45"/>
       <c r="BG38" s="45"/>
@@ -6098,14 +6277,14 @@
       <c r="BO38" s="45"/>
       <c r="BP38" s="45"/>
       <c r="BQ38" s="45"/>
-      <c r="BR38" s="45"/>
+      <c r="BR38" s="14"/>
       <c r="BS38" s="45"/>
       <c r="BT38" s="45"/>
       <c r="BU38" s="45"/>
       <c r="BV38" s="45"/>
       <c r="BW38" s="45"/>
       <c r="BX38" s="45"/>
-      <c r="BY38" s="45"/>
+      <c r="BY38" s="14"/>
       <c r="BZ38" s="45"/>
       <c r="CA38" s="45"/>
       <c r="CB38" s="45"/>
@@ -6116,7 +6295,7 @@
       <c r="CG38" s="45"/>
       <c r="CH38" s="45"/>
       <c r="CI38" s="45"/>
-      <c r="CJ38" s="45"/>
+      <c r="CJ38" s="14"/>
       <c r="CK38" s="45"/>
       <c r="CL38" s="45"/>
       <c r="CM38" s="45"/>
@@ -6124,16 +6303,15 @@
       <c r="CO38" s="45"/>
       <c r="CP38" s="45"/>
       <c r="CQ38" s="45"/>
-      <c r="CR38" s="45"/>
+      <c r="CR38" s="14"/>
       <c r="CS38" s="45"/>
       <c r="CT38" s="45"/>
       <c r="CU38" s="45"/>
     </row>
-    <row r="39" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A39" s="49"/>
-      <c r="B39" s="48"/>
-      <c r="C39" s="47"/>
-      <c r="D39" s="45"/>
+    <row r="39" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="A39" s="47"/>
+      <c r="B39" s="52"/>
+      <c r="C39" s="52"/>
       <c r="E39" s="45"/>
       <c r="F39" s="45"/>
       <c r="G39" s="45"/>
@@ -6155,7 +6333,7 @@
       <c r="W39" s="45"/>
       <c r="X39" s="45"/>
       <c r="Y39" s="45"/>
-      <c r="Z39" s="45"/>
+      <c r="Z39" s="14"/>
       <c r="AA39" s="45"/>
       <c r="AB39" s="45"/>
       <c r="AC39" s="45"/>
@@ -6178,14 +6356,14 @@
       <c r="AT39" s="45"/>
       <c r="AU39" s="45"/>
       <c r="AV39" s="45"/>
-      <c r="AW39" s="45"/>
+      <c r="AW39" s="14"/>
       <c r="AX39" s="45"/>
       <c r="AY39" s="45"/>
       <c r="AZ39" s="45"/>
       <c r="BA39" s="45"/>
       <c r="BB39" s="45"/>
       <c r="BC39" s="45"/>
-      <c r="BD39" s="45"/>
+      <c r="BD39" s="14"/>
       <c r="BE39" s="45"/>
       <c r="BF39" s="45"/>
       <c r="BG39" s="45"/>
@@ -6199,14 +6377,14 @@
       <c r="BO39" s="45"/>
       <c r="BP39" s="45"/>
       <c r="BQ39" s="45"/>
-      <c r="BR39" s="45"/>
+      <c r="BR39" s="14"/>
       <c r="BS39" s="45"/>
       <c r="BT39" s="45"/>
       <c r="BU39" s="45"/>
       <c r="BV39" s="45"/>
       <c r="BW39" s="45"/>
       <c r="BX39" s="45"/>
-      <c r="BY39" s="45"/>
+      <c r="BY39" s="14"/>
       <c r="BZ39" s="45"/>
       <c r="CA39" s="45"/>
       <c r="CB39" s="45"/>
@@ -6217,7 +6395,7 @@
       <c r="CG39" s="45"/>
       <c r="CH39" s="45"/>
       <c r="CI39" s="45"/>
-      <c r="CJ39" s="45"/>
+      <c r="CJ39" s="14"/>
       <c r="CK39" s="45"/>
       <c r="CL39" s="45"/>
       <c r="CM39" s="45"/>
@@ -6225,16 +6403,15 @@
       <c r="CO39" s="45"/>
       <c r="CP39" s="45"/>
       <c r="CQ39" s="45"/>
-      <c r="CR39" s="45"/>
+      <c r="CR39" s="14"/>
       <c r="CS39" s="45"/>
       <c r="CT39" s="45"/>
       <c r="CU39" s="45"/>
     </row>
-    <row r="40" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A40" s="49"/>
-      <c r="B40" s="48"/>
-      <c r="C40" s="47"/>
-      <c r="D40" s="45"/>
+    <row r="40" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="A40" s="47"/>
+      <c r="B40" s="52"/>
+      <c r="C40" s="52"/>
       <c r="E40" s="45"/>
       <c r="F40" s="45"/>
       <c r="G40" s="45"/>
@@ -6256,7 +6433,7 @@
       <c r="W40" s="45"/>
       <c r="X40" s="45"/>
       <c r="Y40" s="45"/>
-      <c r="Z40" s="45"/>
+      <c r="Z40" s="14"/>
       <c r="AA40" s="45"/>
       <c r="AB40" s="45"/>
       <c r="AC40" s="45"/>
@@ -6279,14 +6456,14 @@
       <c r="AT40" s="45"/>
       <c r="AU40" s="45"/>
       <c r="AV40" s="45"/>
-      <c r="AW40" s="45"/>
+      <c r="AW40" s="14"/>
       <c r="AX40" s="45"/>
       <c r="AY40" s="45"/>
       <c r="AZ40" s="45"/>
       <c r="BA40" s="45"/>
       <c r="BB40" s="45"/>
       <c r="BC40" s="45"/>
-      <c r="BD40" s="45"/>
+      <c r="BD40" s="14"/>
       <c r="BE40" s="45"/>
       <c r="BF40" s="45"/>
       <c r="BG40" s="45"/>
@@ -6300,14 +6477,14 @@
       <c r="BO40" s="45"/>
       <c r="BP40" s="45"/>
       <c r="BQ40" s="45"/>
-      <c r="BR40" s="45"/>
+      <c r="BR40" s="14"/>
       <c r="BS40" s="45"/>
       <c r="BT40" s="45"/>
       <c r="BU40" s="45"/>
       <c r="BV40" s="45"/>
       <c r="BW40" s="45"/>
       <c r="BX40" s="45"/>
-      <c r="BY40" s="45"/>
+      <c r="BY40" s="14"/>
       <c r="BZ40" s="45"/>
       <c r="CA40" s="45"/>
       <c r="CB40" s="45"/>
@@ -6318,7 +6495,7 @@
       <c r="CG40" s="45"/>
       <c r="CH40" s="45"/>
       <c r="CI40" s="45"/>
-      <c r="CJ40" s="45"/>
+      <c r="CJ40" s="14"/>
       <c r="CK40" s="45"/>
       <c r="CL40" s="45"/>
       <c r="CM40" s="45"/>
@@ -6326,16 +6503,15 @@
       <c r="CO40" s="45"/>
       <c r="CP40" s="45"/>
       <c r="CQ40" s="45"/>
-      <c r="CR40" s="45"/>
+      <c r="CR40" s="14"/>
       <c r="CS40" s="45"/>
       <c r="CT40" s="45"/>
       <c r="CU40" s="45"/>
     </row>
-    <row r="41" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A41" s="49"/>
-      <c r="B41" s="48"/>
-      <c r="C41" s="47"/>
-      <c r="D41" s="45"/>
+    <row r="41" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="A41" s="47"/>
+      <c r="B41" s="52"/>
+      <c r="C41" s="52"/>
       <c r="E41" s="45"/>
       <c r="F41" s="45"/>
       <c r="G41" s="45"/>
@@ -6357,7 +6533,7 @@
       <c r="W41" s="45"/>
       <c r="X41" s="45"/>
       <c r="Y41" s="45"/>
-      <c r="Z41" s="45"/>
+      <c r="Z41" s="14"/>
       <c r="AA41" s="45"/>
       <c r="AB41" s="45"/>
       <c r="AC41" s="45"/>
@@ -6380,14 +6556,14 @@
       <c r="AT41" s="45"/>
       <c r="AU41" s="45"/>
       <c r="AV41" s="45"/>
-      <c r="AW41" s="45"/>
+      <c r="AW41" s="14"/>
       <c r="AX41" s="45"/>
       <c r="AY41" s="45"/>
       <c r="AZ41" s="45"/>
       <c r="BA41" s="45"/>
       <c r="BB41" s="45"/>
       <c r="BC41" s="45"/>
-      <c r="BD41" s="45"/>
+      <c r="BD41" s="14"/>
       <c r="BE41" s="45"/>
       <c r="BF41" s="45"/>
       <c r="BG41" s="45"/>
@@ -6401,14 +6577,14 @@
       <c r="BO41" s="45"/>
       <c r="BP41" s="45"/>
       <c r="BQ41" s="45"/>
-      <c r="BR41" s="45"/>
+      <c r="BR41" s="14"/>
       <c r="BS41" s="45"/>
       <c r="BT41" s="45"/>
       <c r="BU41" s="45"/>
       <c r="BV41" s="45"/>
       <c r="BW41" s="45"/>
       <c r="BX41" s="45"/>
-      <c r="BY41" s="45"/>
+      <c r="BY41" s="14"/>
       <c r="BZ41" s="45"/>
       <c r="CA41" s="45"/>
       <c r="CB41" s="45"/>
@@ -6419,7 +6595,7 @@
       <c r="CG41" s="45"/>
       <c r="CH41" s="45"/>
       <c r="CI41" s="45"/>
-      <c r="CJ41" s="45"/>
+      <c r="CJ41" s="14"/>
       <c r="CK41" s="45"/>
       <c r="CL41" s="45"/>
       <c r="CM41" s="45"/>
@@ -6427,16 +6603,15 @@
       <c r="CO41" s="45"/>
       <c r="CP41" s="45"/>
       <c r="CQ41" s="45"/>
-      <c r="CR41" s="45"/>
+      <c r="CR41" s="14"/>
       <c r="CS41" s="45"/>
       <c r="CT41" s="45"/>
       <c r="CU41" s="45"/>
     </row>
-    <row r="42" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A42" s="49"/>
-      <c r="B42" s="48"/>
-      <c r="C42" s="47"/>
-      <c r="D42" s="45"/>
+    <row r="42" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="A42" s="47"/>
+      <c r="B42" s="52"/>
+      <c r="C42" s="52"/>
       <c r="E42" s="45"/>
       <c r="F42" s="45"/>
       <c r="G42" s="45"/>
@@ -6458,7 +6633,7 @@
       <c r="W42" s="45"/>
       <c r="X42" s="45"/>
       <c r="Y42" s="45"/>
-      <c r="Z42" s="45"/>
+      <c r="Z42" s="14"/>
       <c r="AA42" s="45"/>
       <c r="AB42" s="45"/>
       <c r="AC42" s="45"/>
@@ -6481,14 +6656,14 @@
       <c r="AT42" s="45"/>
       <c r="AU42" s="45"/>
       <c r="AV42" s="45"/>
-      <c r="AW42" s="45"/>
+      <c r="AW42" s="14"/>
       <c r="AX42" s="45"/>
       <c r="AY42" s="45"/>
       <c r="AZ42" s="45"/>
       <c r="BA42" s="45"/>
       <c r="BB42" s="45"/>
       <c r="BC42" s="45"/>
-      <c r="BD42" s="45"/>
+      <c r="BD42" s="14"/>
       <c r="BE42" s="45"/>
       <c r="BF42" s="45"/>
       <c r="BG42" s="45"/>
@@ -6502,14 +6677,14 @@
       <c r="BO42" s="45"/>
       <c r="BP42" s="45"/>
       <c r="BQ42" s="45"/>
-      <c r="BR42" s="45"/>
+      <c r="BR42" s="14"/>
       <c r="BS42" s="45"/>
       <c r="BT42" s="45"/>
       <c r="BU42" s="45"/>
       <c r="BV42" s="45"/>
       <c r="BW42" s="45"/>
       <c r="BX42" s="45"/>
-      <c r="BY42" s="45"/>
+      <c r="BY42" s="14"/>
       <c r="BZ42" s="45"/>
       <c r="CA42" s="45"/>
       <c r="CB42" s="45"/>
@@ -6520,7 +6695,7 @@
       <c r="CG42" s="45"/>
       <c r="CH42" s="45"/>
       <c r="CI42" s="45"/>
-      <c r="CJ42" s="45"/>
+      <c r="CJ42" s="14"/>
       <c r="CK42" s="45"/>
       <c r="CL42" s="45"/>
       <c r="CM42" s="45"/>
@@ -6528,16 +6703,15 @@
       <c r="CO42" s="45"/>
       <c r="CP42" s="45"/>
       <c r="CQ42" s="45"/>
-      <c r="CR42" s="45"/>
+      <c r="CR42" s="14"/>
       <c r="CS42" s="45"/>
       <c r="CT42" s="45"/>
       <c r="CU42" s="45"/>
     </row>
-    <row r="43" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A43" s="49"/>
-      <c r="B43" s="48"/>
-      <c r="C43" s="47"/>
-      <c r="D43" s="45"/>
+    <row r="43" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="A43" s="47"/>
+      <c r="B43" s="52"/>
+      <c r="C43" s="52"/>
       <c r="E43" s="45"/>
       <c r="F43" s="45"/>
       <c r="G43" s="45"/>
@@ -6559,7 +6733,7 @@
       <c r="W43" s="45"/>
       <c r="X43" s="45"/>
       <c r="Y43" s="45"/>
-      <c r="Z43" s="45"/>
+      <c r="Z43" s="14"/>
       <c r="AA43" s="45"/>
       <c r="AB43" s="45"/>
       <c r="AC43" s="45"/>
@@ -6582,14 +6756,14 @@
       <c r="AT43" s="45"/>
       <c r="AU43" s="45"/>
       <c r="AV43" s="45"/>
-      <c r="AW43" s="45"/>
+      <c r="AW43" s="14"/>
       <c r="AX43" s="45"/>
       <c r="AY43" s="45"/>
       <c r="AZ43" s="45"/>
       <c r="BA43" s="45"/>
       <c r="BB43" s="45"/>
       <c r="BC43" s="45"/>
-      <c r="BD43" s="45"/>
+      <c r="BD43" s="14"/>
       <c r="BE43" s="45"/>
       <c r="BF43" s="45"/>
       <c r="BG43" s="45"/>
@@ -6603,14 +6777,14 @@
       <c r="BO43" s="45"/>
       <c r="BP43" s="45"/>
       <c r="BQ43" s="45"/>
-      <c r="BR43" s="45"/>
+      <c r="BR43" s="14"/>
       <c r="BS43" s="45"/>
       <c r="BT43" s="45"/>
       <c r="BU43" s="45"/>
       <c r="BV43" s="45"/>
       <c r="BW43" s="45"/>
       <c r="BX43" s="45"/>
-      <c r="BY43" s="45"/>
+      <c r="BY43" s="14"/>
       <c r="BZ43" s="45"/>
       <c r="CA43" s="45"/>
       <c r="CB43" s="45"/>
@@ -6621,7 +6795,7 @@
       <c r="CG43" s="45"/>
       <c r="CH43" s="45"/>
       <c r="CI43" s="45"/>
-      <c r="CJ43" s="45"/>
+      <c r="CJ43" s="14"/>
       <c r="CK43" s="45"/>
       <c r="CL43" s="45"/>
       <c r="CM43" s="45"/>
@@ -6629,14 +6803,15 @@
       <c r="CO43" s="45"/>
       <c r="CP43" s="45"/>
       <c r="CQ43" s="45"/>
-      <c r="CR43" s="45"/>
+      <c r="CR43" s="14"/>
       <c r="CS43" s="45"/>
       <c r="CT43" s="45"/>
       <c r="CU43" s="45"/>
     </row>
-    <row r="44" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="B44" s="31"/>
-      <c r="C44" s="32"/>
+    <row r="44" spans="1:99" ht="13" x14ac:dyDescent="0.25">
+      <c r="B44" s="53"/>
+      <c r="C44" s="53"/>
+      <c r="BR44" s="14"/>
     </row>
     <row r="45" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B45" s="31"/>
@@ -6673,19 +6848,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="11265" r:id="rId4" name="SetDateTimeRef">
+        <control shapeId="11267" r:id="rId4" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>12700</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -6693,7 +6868,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="11265" r:id="rId4" name="SetDateTimeRef"/>
+        <control shapeId="11267" r:id="rId4" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -6723,19 +6898,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="11267" r:id="rId8" name="SetDateTimeMain">
+        <control shapeId="11265" r:id="rId8" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" autoPict="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>12700</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -6743,7 +6918,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="11267" r:id="rId8" name="SetDateTimeMain"/>
+        <control shapeId="11265" r:id="rId8" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -6756,10 +6931,10 @@
   <dimension ref="A1:CU50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="CD6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="CE6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="CE9" sqref="CE9"/>
+      <selection pane="bottomRight" activeCell="CE6" sqref="CE6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -10620,19 +10795,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef">
+        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>12700</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -10640,7 +10815,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef"/>
+        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10670,19 +10845,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain">
+        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>12700</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -10690,7 +10865,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain"/>
+        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Beginning Fuel consumption working in ExcelSweep
Modified CarBattery to include fuel consumption in corners vs straights.
Notcing Michigan2015 causes some parfor messages to throw up: In
parallel_function>make_general_channel/channel_general (line 914)
In remoteParallelFunction (line 38)
</commit_message>
<xml_diff>
--- a/SetupSheets.xlsx
+++ b/SetupSheets.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="122">
   <si>
     <t>Date</t>
   </si>
@@ -382,7 +382,10 @@
     <t>CalPolySLO</t>
   </si>
   <si>
-    <t>Delft</t>
+    <t>GFR</t>
+  </si>
+  <si>
+    <t>Racetech</t>
   </si>
 </sst>
 </file>
@@ -1459,10 +1462,10 @@
   <dimension ref="A1:CV50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="CP6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="BE6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="CS10" sqref="CS10"/>
+      <selection pane="bottomRight" activeCell="BF9" sqref="BF9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2993,7 +2996,7 @@
         <v>12</v>
       </c>
       <c r="Y7" s="45">
-        <v>404</v>
+        <v>454</v>
       </c>
       <c r="Z7" s="14"/>
       <c r="AA7" s="45">
@@ -3086,25 +3089,25 @@
         <v>1</v>
       </c>
       <c r="BF7" s="45">
-        <v>2.5</v>
+        <v>2.8460000000000001</v>
       </c>
       <c r="BG7" s="45">
-        <v>2</v>
+        <v>1.9470000000000001</v>
       </c>
       <c r="BH7" s="45">
-        <v>1.62</v>
+        <v>1.556</v>
       </c>
       <c r="BI7" s="45">
         <v>1.333</v>
       </c>
       <c r="BJ7" s="45">
-        <v>1.095</v>
+        <v>1.19</v>
       </c>
       <c r="BK7" s="45">
-        <v>2.6520000000000001</v>
+        <v>1.9550000000000001</v>
       </c>
       <c r="BL7" s="45">
-        <v>2.714</v>
+        <v>3</v>
       </c>
       <c r="BM7" s="45">
         <v>0.9</v>
@@ -3208,105 +3211,289 @@
       </c>
     </row>
     <row r="8" spans="1:100" ht="13" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="52"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="45"/>
-      <c r="N8" s="45"/>
-      <c r="O8" s="45"/>
-      <c r="P8" s="45"/>
-      <c r="Q8" s="45"/>
-      <c r="R8" s="45"/>
-      <c r="S8" s="45"/>
-      <c r="T8" s="46"/>
-      <c r="U8" s="45"/>
-      <c r="V8" s="45"/>
-      <c r="W8" s="45"/>
-      <c r="X8" s="45"/>
-      <c r="Y8" s="45"/>
+      <c r="A8" s="47">
+        <v>0</v>
+      </c>
+      <c r="B8" s="52">
+        <v>0</v>
+      </c>
+      <c r="C8" s="52">
+        <v>0</v>
+      </c>
+      <c r="E8" s="45">
+        <v>63</v>
+      </c>
+      <c r="F8" s="45">
+        <v>47</v>
+      </c>
+      <c r="G8" s="45">
+        <v>46</v>
+      </c>
+      <c r="H8" s="45">
+        <v>0</v>
+      </c>
+      <c r="I8" s="45">
+        <v>0</v>
+      </c>
+      <c r="J8" s="45">
+        <v>0</v>
+      </c>
+      <c r="K8" s="45">
+        <v>0</v>
+      </c>
+      <c r="L8" s="45">
+        <v>0</v>
+      </c>
+      <c r="M8" s="45">
+        <v>0</v>
+      </c>
+      <c r="N8" s="45">
+        <v>0</v>
+      </c>
+      <c r="O8" s="45">
+        <v>0</v>
+      </c>
+      <c r="P8" s="45">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="45">
+        <v>0</v>
+      </c>
+      <c r="R8" s="45">
+        <v>33.39</v>
+      </c>
+      <c r="S8" s="45">
+        <v>0</v>
+      </c>
+      <c r="T8" s="46">
+        <v>12</v>
+      </c>
+      <c r="U8" s="45">
+        <v>175</v>
+      </c>
+      <c r="V8" s="45">
+        <v>33.9</v>
+      </c>
+      <c r="W8" s="45">
+        <v>0</v>
+      </c>
+      <c r="X8" s="45">
+        <v>12</v>
+      </c>
+      <c r="Y8" s="45">
+        <v>454</v>
+      </c>
       <c r="Z8" s="14"/>
-      <c r="AA8" s="45"/>
-      <c r="AB8" s="45"/>
-      <c r="AC8" s="45"/>
-      <c r="AD8" s="45"/>
-      <c r="AE8" s="45"/>
-      <c r="AF8" s="45"/>
-      <c r="AG8" s="45"/>
-      <c r="AH8" s="45"/>
-      <c r="AI8" s="45"/>
-      <c r="AJ8" s="45"/>
-      <c r="AK8" s="45"/>
-      <c r="AL8" s="45"/>
-      <c r="AM8" s="45"/>
-      <c r="AN8" s="45"/>
-      <c r="AO8" s="45"/>
-      <c r="AP8" s="45"/>
-      <c r="AQ8" s="45"/>
-      <c r="AR8" s="45"/>
-      <c r="AS8" s="45"/>
-      <c r="AT8" s="45"/>
-      <c r="AU8" s="45"/>
-      <c r="AV8" s="45"/>
+      <c r="AA8" s="45">
+        <v>250</v>
+      </c>
+      <c r="AB8" s="45">
+        <v>200</v>
+      </c>
+      <c r="AC8" s="45">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="45">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="45">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="45">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="45">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="45">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="45">
+        <v>10.25</v>
+      </c>
+      <c r="AJ8" s="45">
+        <v>10.25</v>
+      </c>
+      <c r="AK8" s="45">
+        <v>-0.25</v>
+      </c>
+      <c r="AL8" s="45">
+        <v>1.9</v>
+      </c>
+      <c r="AM8" s="45">
+        <v>0</v>
+      </c>
+      <c r="AN8" s="45">
+        <v>0</v>
+      </c>
+      <c r="AO8" s="45">
+        <v>0</v>
+      </c>
+      <c r="AP8" s="45">
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="45">
+        <v>0</v>
+      </c>
+      <c r="AR8" s="45">
+        <v>0</v>
+      </c>
+      <c r="AS8" s="45">
+        <v>0</v>
+      </c>
+      <c r="AT8" s="45">
+        <v>0</v>
+      </c>
+      <c r="AU8" s="45">
+        <v>10</v>
+      </c>
+      <c r="AV8" s="45">
+        <v>30</v>
+      </c>
       <c r="AW8" s="14"/>
-      <c r="AX8" s="45"/>
-      <c r="AY8" s="45"/>
-      <c r="AZ8" s="45"/>
-      <c r="BA8" s="45"/>
-      <c r="BB8" s="45"/>
-      <c r="BC8" s="50"/>
+      <c r="AX8" s="45">
+        <v>900</v>
+      </c>
+      <c r="AY8" s="45">
+        <v>10.5</v>
+      </c>
+      <c r="AZ8" s="45">
+        <v>0.03</v>
+      </c>
+      <c r="BA8" s="45">
+        <v>120.628</v>
+      </c>
+      <c r="BB8" s="45">
+        <v>70.396699999999996</v>
+      </c>
+      <c r="BC8" s="50">
+        <v>0</v>
+      </c>
       <c r="BD8" s="14"/>
-      <c r="BE8" s="45"/>
-      <c r="BF8" s="45"/>
-      <c r="BG8" s="45"/>
-      <c r="BH8" s="45"/>
-      <c r="BI8" s="45"/>
-      <c r="BJ8" s="45"/>
-      <c r="BK8" s="45"/>
-      <c r="BL8" s="45"/>
-      <c r="BM8" s="45"/>
-      <c r="BN8" s="45"/>
-      <c r="BO8" s="45"/>
-      <c r="BP8" s="45"/>
-      <c r="BQ8" s="45"/>
+      <c r="BE8" s="45">
+        <v>1</v>
+      </c>
+      <c r="BF8" s="45">
+        <v>2.75</v>
+      </c>
+      <c r="BG8" s="45">
+        <v>2</v>
+      </c>
+      <c r="BH8" s="45">
+        <v>1.6659999999999999</v>
+      </c>
+      <c r="BI8" s="45">
+        <v>1.444</v>
+      </c>
+      <c r="BJ8" s="45">
+        <v>1.304</v>
+      </c>
+      <c r="BK8" s="45">
+        <v>2.1110000000000002</v>
+      </c>
+      <c r="BL8" s="45">
+        <v>2.625</v>
+      </c>
+      <c r="BM8" s="45">
+        <v>0.9</v>
+      </c>
+      <c r="BN8" s="45">
+        <v>0</v>
+      </c>
+      <c r="BO8" s="45">
+        <v>0</v>
+      </c>
+      <c r="BP8" s="45">
+        <v>0</v>
+      </c>
+      <c r="BQ8" s="45">
+        <v>20</v>
+      </c>
       <c r="BR8" s="14"/>
-      <c r="BS8" s="45"/>
-      <c r="BT8" s="45"/>
-      <c r="BU8" s="45"/>
-      <c r="BV8" s="45"/>
-      <c r="BW8" s="45"/>
-      <c r="BX8" s="45"/>
+      <c r="BS8" s="45">
+        <v>6762.75</v>
+      </c>
+      <c r="BT8" s="45">
+        <v>3238.5</v>
+      </c>
+      <c r="BU8" s="45">
+        <v>0</v>
+      </c>
+      <c r="BV8" s="45">
+        <v>0</v>
+      </c>
+      <c r="BW8" s="45">
+        <v>0</v>
+      </c>
+      <c r="BX8" s="45">
+        <v>0.96699999999999997</v>
+      </c>
       <c r="BY8" s="14"/>
-      <c r="BZ8" s="45"/>
-      <c r="CA8" s="45"/>
-      <c r="CB8" s="45"/>
-      <c r="CC8" s="45"/>
-      <c r="CD8" s="45"/>
-      <c r="CE8" s="45"/>
-      <c r="CF8" s="45"/>
-      <c r="CG8" s="45"/>
-      <c r="CH8" s="45"/>
-      <c r="CI8" s="45"/>
+      <c r="BZ8" s="45">
+        <v>0</v>
+      </c>
+      <c r="CA8" s="45">
+        <v>0</v>
+      </c>
+      <c r="CB8" s="45">
+        <v>0</v>
+      </c>
+      <c r="CC8" s="45">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="CD8" s="45">
+        <v>-2.9000000000000001E-2</v>
+      </c>
+      <c r="CE8" s="45">
+        <v>2015</v>
+      </c>
+      <c r="CF8" s="45">
+        <v>2.3289999999999999E-3</v>
+      </c>
+      <c r="CG8" s="45">
+        <v>34.25</v>
+      </c>
+      <c r="CH8" s="45">
+        <v>0</v>
+      </c>
+      <c r="CI8" s="45">
+        <v>10</v>
+      </c>
       <c r="CJ8" s="14"/>
-      <c r="CK8" s="45"/>
-      <c r="CL8" s="45"/>
-      <c r="CM8" s="45"/>
-      <c r="CN8" s="45"/>
-      <c r="CO8" s="45"/>
-      <c r="CP8" s="45"/>
-      <c r="CQ8" s="45"/>
+      <c r="CK8" s="45">
+        <v>3.984</v>
+      </c>
+      <c r="CL8" s="45">
+        <v>6.56</v>
+      </c>
+      <c r="CM8" s="45">
+        <v>250</v>
+      </c>
+      <c r="CN8" s="45">
+        <v>8.9789999999999998E-4</v>
+      </c>
+      <c r="CO8" s="45">
+        <v>8.9789999999999998E-4</v>
+      </c>
+      <c r="CP8" s="45">
+        <v>8.9789999999999998E-4</v>
+      </c>
+      <c r="CQ8" s="45">
+        <v>0</v>
+      </c>
       <c r="CR8" s="14"/>
-      <c r="CS8" s="45"/>
-      <c r="CT8" s="45"/>
-      <c r="CU8" s="45"/>
-      <c r="CV8" s="51"/>
+      <c r="CS8" s="45">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="CT8" s="45">
+        <v>9000</v>
+      </c>
+      <c r="CU8" s="45">
+        <v>0</v>
+      </c>
+      <c r="CV8" s="51" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="9" spans="1:100" ht="13" x14ac:dyDescent="0.25">
       <c r="A9" s="47"/>
@@ -6848,19 +7035,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="11267" r:id="rId4" name="SetDateTimeMain">
+        <control shapeId="11265" r:id="rId4" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>12700</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -6868,7 +7055,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="11267" r:id="rId4" name="SetDateTimeMain"/>
+        <control shapeId="11265" r:id="rId4" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -6898,19 +7085,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="11265" r:id="rId8" name="SetDateTimeRef">
+        <control shapeId="11267" r:id="rId8" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" autoPict="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>12700</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -6918,7 +7105,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="11265" r:id="rId8" name="SetDateTimeRef"/>
+        <control shapeId="11267" r:id="rId8" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -10795,19 +10982,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain">
+        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>12700</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -10815,7 +11002,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain"/>
+        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10845,19 +11032,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef">
+        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>12700</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>12700</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -10865,7 +11052,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef"/>
+        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Mostly working...imaginary numbers popping up with high rpm limits.
</commit_message>
<xml_diff>
--- a/SetupSheets.xlsx
+++ b/SetupSheets.xlsx
@@ -2254,248 +2254,248 @@
       <c r="C5" s="30"/>
       <c r="D5" s="21"/>
       <c r="E5" s="43">
-        <f>E3-E4</f>
+        <f t="shared" ref="E5:AE5" si="0">E3-E4</f>
         <v>0</v>
       </c>
       <c r="F5" s="43">
-        <f>F3-F4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G5" s="43">
-        <f>G3-G4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H5" s="43">
-        <f>H3-H4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I5" s="43">
-        <f>I3-I4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J5" s="43">
-        <f>J3-J4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K5" s="43">
-        <f>K3-K4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L5" s="43">
-        <f>L3-L4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M5" s="43">
-        <f>M3-M4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N5" s="43">
-        <f>N3-N4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O5" s="43">
-        <f>O3-O4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P5" s="43">
-        <f>P3-P4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q5" s="43">
-        <f>Q3-Q4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R5" s="43">
-        <f>R3-R4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S5" s="43">
-        <f>S3-S4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T5" s="43">
-        <f>T3-T4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U5" s="43">
-        <f>U3-U4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="V5" s="43">
-        <f>V3-V4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W5" s="43">
-        <f>W3-W4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X5" s="43">
-        <f>X3-X4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Y5" s="43">
-        <f>Y3-Y4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Z5" s="21">
-        <f>Z3-Z4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AA5" s="43">
-        <f>AA3-AA4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AB5" s="43">
-        <f>AB3-AB4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AC5" s="43">
-        <f>AC3-AC4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AD5" s="43">
-        <f>AD3-AD4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AE5" s="43">
-        <f>AE3-AE4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AF5" s="43"/>
       <c r="AG5" s="43">
-        <f>AG3-AG4</f>
+        <f t="shared" ref="AG5:BN5" si="1">AG3-AG4</f>
         <v>0</v>
       </c>
       <c r="AH5" s="43">
-        <f>AH3-AH4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI5" s="43">
-        <f>AI3-AI4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AJ5" s="43">
-        <f>AJ3-AJ4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AK5" s="43">
-        <f>AK3-AK4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AL5" s="43">
-        <f>AL3-AL4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AM5" s="43">
-        <f>AM3-AM4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AN5" s="43">
-        <f>AN3-AN4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AO5" s="43">
-        <f>AO3-AO4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AP5" s="43">
-        <f>AP3-AP4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AQ5" s="43">
-        <f>AQ3-AQ4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AR5" s="43">
-        <f>AR3-AR4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AS5" s="43">
-        <f>AS3-AS4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AT5" s="43">
-        <f>AT3-AT4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AU5" s="43">
-        <f>AU3-AU4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AV5" s="43">
-        <f>AV3-AV4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AW5" s="21">
-        <f>AW3-AW4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AX5" s="43">
-        <f>AX3-AX4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AY5" s="43">
-        <f>AY3-AY4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AZ5" s="43">
-        <f>AZ3-AZ4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BA5" s="43">
-        <f>BA3-BA4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BB5" s="43">
-        <f>BB3-BB4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BC5" s="43">
-        <f>BC3-BC4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BD5" s="21">
-        <f>BD3-BD4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BE5" s="43">
-        <f>BE3-BE4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BF5" s="43">
-        <f>BF3-BF4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BG5" s="43">
-        <f>BG3-BG4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BH5" s="43">
-        <f>BH3-BH4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BI5" s="43">
-        <f>BI3-BI4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BJ5" s="43">
-        <f>BJ3-BJ4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BK5" s="43">
-        <f>BK3-BK4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BL5" s="43">
-        <f>BL3-BL4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BM5" s="43">
-        <f>BM3-BM4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BN5" s="43">
-        <f>BN3-BN4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="BO5" s="43"/>
@@ -2523,27 +2523,27 @@
       <c r="BV5" s="43"/>
       <c r="BW5" s="43"/>
       <c r="BX5" s="43">
-        <f>BX3-BX4</f>
+        <f t="shared" ref="BX5:CC5" si="2">BX3-BX4</f>
         <v>0</v>
       </c>
       <c r="BY5" s="21">
-        <f>BY3-BY4</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BZ5" s="43">
-        <f>BZ3-BZ4</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CA5" s="43">
-        <f>CA3-CA4</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CB5" s="43">
-        <f>CB3-CB4</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CC5" s="43">
-        <f>CC3-CC4</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CD5" s="43"/>
@@ -2556,31 +2556,31 @@
       <c r="CH5" s="43"/>
       <c r="CI5" s="43"/>
       <c r="CJ5" s="21">
-        <f>CJ3-CJ4</f>
+        <f t="shared" ref="CJ5:CP5" si="3">CJ3-CJ4</f>
         <v>0</v>
       </c>
       <c r="CK5" s="43">
-        <f>CK3-CK4</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CL5" s="43">
-        <f>CL3-CL4</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CM5" s="43">
-        <f>CM3-CM4</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CN5" s="43">
-        <f>CN3-CN4</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CO5" s="43">
-        <f>CO3-CO4</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CP5" s="43">
-        <f>CP3-CP4</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CQ5" s="43"/>
@@ -7024,19 +7024,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="11267" r:id="rId4" name="SetDateTimeMain">
+        <control shapeId="11265" r:id="rId4" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -7044,7 +7044,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="11267" r:id="rId4" name="SetDateTimeMain"/>
+        <control shapeId="11265" r:id="rId4" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -7074,19 +7074,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="11265" r:id="rId8" name="SetDateTimeRef">
+        <control shapeId="11267" r:id="rId8" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" autoPict="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -7094,7 +7094,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="11265" r:id="rId8" name="SetDateTimeRef"/>
+        <control shapeId="11267" r:id="rId8" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -7107,10 +7107,10 @@
   <dimension ref="A1:CU50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="CD6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="L6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="CU6" sqref="CU6"/>
+      <selection pane="bottomRight" activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10971,19 +10971,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain">
+        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -10991,7 +10991,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain"/>
+        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11021,19 +11021,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef">
+        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -11041,7 +11041,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef"/>
+        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Ignore commit, only for accessing master
Initially tried to fix RPM histograms with this version thinking Thomas
figured it out. But he actually figured out Battery modeling issues.
</commit_message>
<xml_diff>
--- a/SetupSheets.xlsx
+++ b/SetupSheets.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Code\LapSimCombined\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Journey\Documents\GitHub\LapSimCombined\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1815" yWindow="540" windowWidth="9705" windowHeight="3240" activeTab="1"/>
+    <workbookView xWindow="1820" yWindow="540" windowWidth="9710" windowHeight="3240"/>
   </bookViews>
   <sheets>
     <sheet name="Combustion" sheetId="11" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="117">
   <si>
     <t>Date</t>
   </si>
@@ -368,6 +368,9 @@
   </si>
   <si>
     <t>Wf</t>
+  </si>
+  <si>
+    <t>CalPolySLO</t>
   </si>
 </sst>
 </file>
@@ -751,11 +754,11 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -810,7 +813,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -861,11 +864,11 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -971,11 +974,11 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -1030,7 +1033,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -1081,11 +1084,11 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -1434,41 +1437,41 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:CU50"/>
+  <dimension ref="A1:CV50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="BT6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="CQ6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="CU6" sqref="CU6"/>
+      <selection pane="bottomRight" activeCell="CX10" sqref="CX9:CX10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" style="23" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="33" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="34" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="24" customWidth="1"/>
-    <col min="5" max="25" width="6.85546875" style="23" customWidth="1"/>
-    <col min="26" max="26" width="6.85546875" style="24" customWidth="1"/>
-    <col min="27" max="48" width="6.85546875" style="23" customWidth="1"/>
-    <col min="49" max="49" width="6.85546875" style="24" customWidth="1"/>
-    <col min="50" max="54" width="6.85546875" style="23" customWidth="1"/>
-    <col min="55" max="55" width="10.85546875" style="23" customWidth="1"/>
-    <col min="56" max="56" width="6.85546875" style="24" customWidth="1"/>
-    <col min="57" max="69" width="6.85546875" style="23" customWidth="1"/>
-    <col min="70" max="70" width="6.85546875" style="24" customWidth="1"/>
-    <col min="71" max="76" width="6.85546875" style="23" customWidth="1"/>
-    <col min="77" max="77" width="6.85546875" style="24" customWidth="1"/>
-    <col min="78" max="87" width="6.85546875" style="23" customWidth="1"/>
-    <col min="88" max="88" width="6.85546875" style="24" customWidth="1"/>
-    <col min="89" max="95" width="6.85546875" style="23" customWidth="1"/>
-    <col min="96" max="96" width="6.85546875" style="24" customWidth="1"/>
-    <col min="97" max="99" width="6.85546875" style="23" customWidth="1"/>
-    <col min="100" max="16384" width="9.140625" style="23"/>
+    <col min="2" max="2" width="12.26953125" style="33" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" style="34" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" style="24" customWidth="1"/>
+    <col min="5" max="25" width="6.81640625" style="23" customWidth="1"/>
+    <col min="26" max="26" width="6.81640625" style="24" customWidth="1"/>
+    <col min="27" max="48" width="6.81640625" style="23" customWidth="1"/>
+    <col min="49" max="49" width="6.81640625" style="24" customWidth="1"/>
+    <col min="50" max="54" width="6.81640625" style="23" customWidth="1"/>
+    <col min="55" max="55" width="10.81640625" style="23" customWidth="1"/>
+    <col min="56" max="56" width="6.81640625" style="24" customWidth="1"/>
+    <col min="57" max="69" width="6.81640625" style="23" customWidth="1"/>
+    <col min="70" max="70" width="6.81640625" style="24" customWidth="1"/>
+    <col min="71" max="76" width="6.81640625" style="23" customWidth="1"/>
+    <col min="77" max="77" width="6.81640625" style="24" customWidth="1"/>
+    <col min="78" max="87" width="6.81640625" style="23" customWidth="1"/>
+    <col min="88" max="88" width="6.81640625" style="24" customWidth="1"/>
+    <col min="89" max="95" width="6.81640625" style="23" customWidth="1"/>
+    <col min="96" max="96" width="6.81640625" style="24" customWidth="1"/>
+    <col min="97" max="99" width="6.81640625" style="23" customWidth="1"/>
+    <col min="100" max="16384" width="9.1796875" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" s="25" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:100" s="25" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>35</v>
       </c>
@@ -1763,7 +1766,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:99" s="28" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:100" s="28" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="36"/>
       <c r="B2" s="26" t="s">
         <v>0</v>
@@ -2044,7 +2047,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:99" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:100" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37"/>
       <c r="B3" s="29"/>
       <c r="C3" s="30"/>
@@ -2145,7 +2148,7 @@
       <c r="CT3" s="15"/>
       <c r="CU3" s="15"/>
     </row>
-    <row r="4" spans="1:99" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:100" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="37"/>
       <c r="B4" s="29"/>
       <c r="C4" s="30"/>
@@ -2246,7 +2249,7 @@
       <c r="CT4" s="15"/>
       <c r="CU4" s="15"/>
     </row>
-    <row r="5" spans="1:99" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:100" s="22" customFormat="1" ht="13" x14ac:dyDescent="0.25">
       <c r="A5" s="51" t="s">
         <v>115</v>
       </c>
@@ -2601,7 +2604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:99" s="50" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:100" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="49">
         <v>0</v>
       </c>
@@ -2883,8 +2886,11 @@
       <c r="CU6" s="45">
         <v>0</v>
       </c>
+      <c r="CV6" s="50" t="s">
+        <v>116</v>
+      </c>
     </row>
-    <row r="7" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A7" s="49">
         <v>1</v>
       </c>
@@ -3167,7 +3173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A8" s="49">
         <v>2</v>
       </c>
@@ -3450,7 +3456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A9" s="49"/>
       <c r="B9" s="48"/>
       <c r="C9" s="47"/>
@@ -3551,7 +3557,7 @@
       <c r="CT9" s="45"/>
       <c r="CU9" s="45"/>
     </row>
-    <row r="10" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A10" s="49"/>
       <c r="B10" s="48"/>
       <c r="C10" s="47"/>
@@ -3652,7 +3658,7 @@
       <c r="CT10" s="45"/>
       <c r="CU10" s="45"/>
     </row>
-    <row r="11" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A11" s="49"/>
       <c r="B11" s="48"/>
       <c r="C11" s="47"/>
@@ -3753,7 +3759,7 @@
       <c r="CT11" s="45"/>
       <c r="CU11" s="45"/>
     </row>
-    <row r="12" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A12" s="49"/>
       <c r="B12" s="48"/>
       <c r="C12" s="47"/>
@@ -3854,7 +3860,7 @@
       <c r="CT12" s="45"/>
       <c r="CU12" s="45"/>
     </row>
-    <row r="13" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A13" s="49"/>
       <c r="B13" s="48"/>
       <c r="C13" s="47"/>
@@ -3955,7 +3961,7 @@
       <c r="CT13" s="45"/>
       <c r="CU13" s="45"/>
     </row>
-    <row r="14" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A14" s="49"/>
       <c r="B14" s="48"/>
       <c r="C14" s="47"/>
@@ -4056,7 +4062,7 @@
       <c r="CT14" s="45"/>
       <c r="CU14" s="45"/>
     </row>
-    <row r="15" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A15" s="49"/>
       <c r="B15" s="48"/>
       <c r="C15" s="47"/>
@@ -4157,7 +4163,7 @@
       <c r="CT15" s="45"/>
       <c r="CU15" s="45"/>
     </row>
-    <row r="16" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A16" s="49"/>
       <c r="B16" s="48"/>
       <c r="C16" s="47"/>
@@ -4258,7 +4264,7 @@
       <c r="CT16" s="45"/>
       <c r="CU16" s="45"/>
     </row>
-    <row r="17" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A17" s="49"/>
       <c r="B17" s="48"/>
       <c r="C17" s="47"/>
@@ -4359,7 +4365,7 @@
       <c r="CT17" s="45"/>
       <c r="CU17" s="45"/>
     </row>
-    <row r="18" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A18" s="49"/>
       <c r="B18" s="48"/>
       <c r="C18" s="47"/>
@@ -4460,7 +4466,7 @@
       <c r="CT18" s="45"/>
       <c r="CU18" s="45"/>
     </row>
-    <row r="19" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A19" s="49"/>
       <c r="B19" s="48"/>
       <c r="C19" s="47"/>
@@ -4561,7 +4567,7 @@
       <c r="CT19" s="45"/>
       <c r="CU19" s="45"/>
     </row>
-    <row r="20" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A20" s="49"/>
       <c r="B20" s="48"/>
       <c r="C20" s="47"/>
@@ -4662,7 +4668,7 @@
       <c r="CT20" s="45"/>
       <c r="CU20" s="45"/>
     </row>
-    <row r="21" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A21" s="49"/>
       <c r="B21" s="48"/>
       <c r="C21" s="47"/>
@@ -4763,7 +4769,7 @@
       <c r="CT21" s="45"/>
       <c r="CU21" s="45"/>
     </row>
-    <row r="22" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A22" s="49"/>
       <c r="B22" s="48"/>
       <c r="C22" s="47"/>
@@ -4864,7 +4870,7 @@
       <c r="CT22" s="45"/>
       <c r="CU22" s="45"/>
     </row>
-    <row r="23" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A23" s="49"/>
       <c r="B23" s="48"/>
       <c r="C23" s="47"/>
@@ -4965,7 +4971,7 @@
       <c r="CT23" s="45"/>
       <c r="CU23" s="45"/>
     </row>
-    <row r="24" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A24" s="49"/>
       <c r="B24" s="48"/>
       <c r="C24" s="47"/>
@@ -5066,7 +5072,7 @@
       <c r="CT24" s="45"/>
       <c r="CU24" s="45"/>
     </row>
-    <row r="25" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A25" s="49"/>
       <c r="B25" s="48"/>
       <c r="C25" s="47"/>
@@ -5167,7 +5173,7 @@
       <c r="CT25" s="45"/>
       <c r="CU25" s="45"/>
     </row>
-    <row r="26" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A26" s="49"/>
       <c r="B26" s="48"/>
       <c r="C26" s="47"/>
@@ -5268,7 +5274,7 @@
       <c r="CT26" s="45"/>
       <c r="CU26" s="45"/>
     </row>
-    <row r="27" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A27" s="49"/>
       <c r="B27" s="48"/>
       <c r="C27" s="47"/>
@@ -5369,7 +5375,7 @@
       <c r="CT27" s="45"/>
       <c r="CU27" s="45"/>
     </row>
-    <row r="28" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A28" s="49"/>
       <c r="B28" s="48"/>
       <c r="C28" s="47"/>
@@ -5470,7 +5476,7 @@
       <c r="CT28" s="45"/>
       <c r="CU28" s="45"/>
     </row>
-    <row r="29" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A29" s="49"/>
       <c r="B29" s="48"/>
       <c r="C29" s="47"/>
@@ -5571,7 +5577,7 @@
       <c r="CT29" s="45"/>
       <c r="CU29" s="45"/>
     </row>
-    <row r="30" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A30" s="49"/>
       <c r="B30" s="48"/>
       <c r="C30" s="47"/>
@@ -5672,7 +5678,7 @@
       <c r="CT30" s="45"/>
       <c r="CU30" s="45"/>
     </row>
-    <row r="31" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A31" s="49"/>
       <c r="B31" s="48"/>
       <c r="C31" s="47"/>
@@ -5773,7 +5779,7 @@
       <c r="CT31" s="45"/>
       <c r="CU31" s="45"/>
     </row>
-    <row r="32" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A32" s="49"/>
       <c r="B32" s="48"/>
       <c r="C32" s="47"/>
@@ -5874,7 +5880,7 @@
       <c r="CT32" s="45"/>
       <c r="CU32" s="45"/>
     </row>
-    <row r="33" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A33" s="49"/>
       <c r="B33" s="48"/>
       <c r="C33" s="47"/>
@@ -5975,7 +5981,7 @@
       <c r="CT33" s="45"/>
       <c r="CU33" s="45"/>
     </row>
-    <row r="34" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A34" s="49"/>
       <c r="B34" s="48"/>
       <c r="C34" s="47"/>
@@ -6076,7 +6082,7 @@
       <c r="CT34" s="45"/>
       <c r="CU34" s="45"/>
     </row>
-    <row r="35" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A35" s="49"/>
       <c r="B35" s="48"/>
       <c r="C35" s="47"/>
@@ -6177,7 +6183,7 @@
       <c r="CT35" s="45"/>
       <c r="CU35" s="45"/>
     </row>
-    <row r="36" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A36" s="49"/>
       <c r="B36" s="48"/>
       <c r="C36" s="47"/>
@@ -6278,7 +6284,7 @@
       <c r="CT36" s="45"/>
       <c r="CU36" s="45"/>
     </row>
-    <row r="37" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A37" s="49"/>
       <c r="B37" s="48"/>
       <c r="C37" s="47"/>
@@ -6379,7 +6385,7 @@
       <c r="CT37" s="45"/>
       <c r="CU37" s="45"/>
     </row>
-    <row r="38" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A38" s="49"/>
       <c r="B38" s="48"/>
       <c r="C38" s="47"/>
@@ -6480,7 +6486,7 @@
       <c r="CT38" s="45"/>
       <c r="CU38" s="45"/>
     </row>
-    <row r="39" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A39" s="49"/>
       <c r="B39" s="48"/>
       <c r="C39" s="47"/>
@@ -6581,7 +6587,7 @@
       <c r="CT39" s="45"/>
       <c r="CU39" s="45"/>
     </row>
-    <row r="40" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A40" s="49"/>
       <c r="B40" s="48"/>
       <c r="C40" s="47"/>
@@ -6682,7 +6688,7 @@
       <c r="CT40" s="45"/>
       <c r="CU40" s="45"/>
     </row>
-    <row r="41" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A41" s="49"/>
       <c r="B41" s="48"/>
       <c r="C41" s="47"/>
@@ -6783,7 +6789,7 @@
       <c r="CT41" s="45"/>
       <c r="CU41" s="45"/>
     </row>
-    <row r="42" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A42" s="49"/>
       <c r="B42" s="48"/>
       <c r="C42" s="47"/>
@@ -6884,7 +6890,7 @@
       <c r="CT42" s="45"/>
       <c r="CU42" s="45"/>
     </row>
-    <row r="43" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A43" s="49"/>
       <c r="B43" s="48"/>
       <c r="C43" s="47"/>
@@ -6985,31 +6991,31 @@
       <c r="CT43" s="45"/>
       <c r="CU43" s="45"/>
     </row>
-    <row r="44" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B44" s="31"/>
       <c r="C44" s="32"/>
     </row>
-    <row r="45" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B45" s="31"/>
       <c r="C45" s="32"/>
     </row>
-    <row r="46" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B46" s="31"/>
       <c r="C46" s="32"/>
     </row>
-    <row r="47" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B47" s="31"/>
       <c r="C47" s="32"/>
     </row>
-    <row r="48" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B48" s="31"/>
       <c r="C48" s="32"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="31"/>
       <c r="C49" s="32"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="31"/>
       <c r="C50" s="32"/>
     </row>
@@ -7024,19 +7030,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="11265" r:id="rId4" name="SetDateTimeRef">
+        <control shapeId="11267" r:id="rId4" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>12700</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:colOff>12700</xdr:colOff>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -7044,7 +7050,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="11265" r:id="rId4" name="SetDateTimeRef"/>
+        <control shapeId="11267" r:id="rId4" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -7060,7 +7066,7 @@
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:colOff>12700</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
@@ -7074,19 +7080,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="11267" r:id="rId8" name="SetDateTimeMain">
+        <control shapeId="11265" r:id="rId8" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" autoPict="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>12700</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:colOff>12700</xdr:colOff>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -7094,7 +7100,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="11267" r:id="rId8" name="SetDateTimeMain"/>
+        <control shapeId="11265" r:id="rId8" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -7106,39 +7112,39 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:CU50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="5" topLeftCell="L6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
       <selection pane="bottomRight" activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" style="23" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="33" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="34" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="24" customWidth="1"/>
-    <col min="5" max="25" width="6.85546875" style="23" customWidth="1"/>
-    <col min="26" max="26" width="6.85546875" style="24" customWidth="1"/>
-    <col min="27" max="48" width="6.85546875" style="23" customWidth="1"/>
-    <col min="49" max="49" width="6.85546875" style="24" customWidth="1"/>
-    <col min="50" max="54" width="6.85546875" style="23" customWidth="1"/>
-    <col min="55" max="55" width="10.85546875" style="23" customWidth="1"/>
-    <col min="56" max="56" width="6.85546875" style="24" customWidth="1"/>
-    <col min="57" max="69" width="6.85546875" style="23" customWidth="1"/>
-    <col min="70" max="70" width="6.85546875" style="24" customWidth="1"/>
-    <col min="71" max="76" width="6.85546875" style="23" customWidth="1"/>
-    <col min="77" max="77" width="6.85546875" style="24" customWidth="1"/>
-    <col min="78" max="87" width="6.85546875" style="23" customWidth="1"/>
-    <col min="88" max="88" width="6.85546875" style="24" customWidth="1"/>
-    <col min="89" max="95" width="6.85546875" style="23" customWidth="1"/>
-    <col min="96" max="96" width="6.85546875" style="24" customWidth="1"/>
-    <col min="97" max="99" width="6.85546875" style="23" customWidth="1"/>
-    <col min="100" max="16384" width="9.140625" style="23"/>
+    <col min="2" max="2" width="12.26953125" style="33" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" style="34" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" style="24" customWidth="1"/>
+    <col min="5" max="25" width="6.81640625" style="23" customWidth="1"/>
+    <col min="26" max="26" width="6.81640625" style="24" customWidth="1"/>
+    <col min="27" max="48" width="6.81640625" style="23" customWidth="1"/>
+    <col min="49" max="49" width="6.81640625" style="24" customWidth="1"/>
+    <col min="50" max="54" width="6.81640625" style="23" customWidth="1"/>
+    <col min="55" max="55" width="10.81640625" style="23" customWidth="1"/>
+    <col min="56" max="56" width="6.81640625" style="24" customWidth="1"/>
+    <col min="57" max="69" width="6.81640625" style="23" customWidth="1"/>
+    <col min="70" max="70" width="6.81640625" style="24" customWidth="1"/>
+    <col min="71" max="76" width="6.81640625" style="23" customWidth="1"/>
+    <col min="77" max="77" width="6.81640625" style="24" customWidth="1"/>
+    <col min="78" max="87" width="6.81640625" style="23" customWidth="1"/>
+    <col min="88" max="88" width="6.81640625" style="24" customWidth="1"/>
+    <col min="89" max="95" width="6.81640625" style="23" customWidth="1"/>
+    <col min="96" max="96" width="6.81640625" style="24" customWidth="1"/>
+    <col min="97" max="99" width="6.81640625" style="23" customWidth="1"/>
+    <col min="100" max="16384" width="9.1796875" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" s="25" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:99" s="25" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>35</v>
       </c>
@@ -7433,7 +7439,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:99" s="28" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:99" s="28" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="36"/>
       <c r="B2" s="26" t="s">
         <v>0</v>
@@ -7714,7 +7720,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:99" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:99" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37"/>
       <c r="B3" s="29"/>
       <c r="C3" s="30"/>
@@ -7815,7 +7821,7 @@
       <c r="CT3" s="15"/>
       <c r="CU3" s="15"/>
     </row>
-    <row r="4" spans="1:99" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:99" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="37"/>
       <c r="B4" s="29"/>
       <c r="C4" s="30"/>
@@ -7916,7 +7922,7 @@
       <c r="CT4" s="15"/>
       <c r="CU4" s="15"/>
     </row>
-    <row r="5" spans="1:99" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:99" s="22" customFormat="1" ht="13" x14ac:dyDescent="0.25">
       <c r="A5" s="37" t="s">
         <v>36</v>
       </c>
@@ -8271,7 +8277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:99" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:99" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="1">
         <v>35065</v>
@@ -8554,7 +8560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:99" ht="13" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="1"/>
       <c r="C7" s="8"/>
@@ -8655,7 +8661,7 @@
       <c r="CT7" s="18"/>
       <c r="CU7" s="18"/>
     </row>
-    <row r="8" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
       <c r="B8" s="1"/>
       <c r="C8" s="8"/>
@@ -8755,7 +8761,7 @@
       <c r="CT8" s="18"/>
       <c r="CU8" s="18"/>
     </row>
-    <row r="9" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="B9" s="1"/>
       <c r="C9" s="8"/>
@@ -8856,7 +8862,7 @@
       <c r="CT9" s="18"/>
       <c r="CU9" s="18"/>
     </row>
-    <row r="10" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
       <c r="B10" s="1"/>
       <c r="C10" s="8"/>
@@ -8957,7 +8963,7 @@
       <c r="CT10" s="18"/>
       <c r="CU10" s="18"/>
     </row>
-    <row r="11" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A11" s="19"/>
       <c r="B11" s="1"/>
       <c r="C11" s="8"/>
@@ -9058,7 +9064,7 @@
       <c r="CT11" s="18"/>
       <c r="CU11" s="18"/>
     </row>
-    <row r="12" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A12" s="19"/>
       <c r="B12" s="1"/>
       <c r="C12" s="8"/>
@@ -9159,7 +9165,7 @@
       <c r="CT12" s="18"/>
       <c r="CU12" s="18"/>
     </row>
-    <row r="13" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
       <c r="B13" s="1"/>
       <c r="C13" s="8"/>
@@ -9260,7 +9266,7 @@
       <c r="CT13" s="18"/>
       <c r="CU13" s="18"/>
     </row>
-    <row r="14" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A14" s="19"/>
       <c r="B14" s="1"/>
       <c r="C14" s="8"/>
@@ -9361,7 +9367,7 @@
       <c r="CT14" s="18"/>
       <c r="CU14" s="18"/>
     </row>
-    <row r="15" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
       <c r="B15" s="1"/>
       <c r="C15" s="8"/>
@@ -9462,7 +9468,7 @@
       <c r="CT15" s="18"/>
       <c r="CU15" s="18"/>
     </row>
-    <row r="16" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
       <c r="B16" s="1"/>
       <c r="C16" s="8"/>
@@ -9563,7 +9569,7 @@
       <c r="CT16" s="18"/>
       <c r="CU16" s="18"/>
     </row>
-    <row r="17" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
       <c r="B17" s="1"/>
       <c r="C17" s="8"/>
@@ -9664,7 +9670,7 @@
       <c r="CT17" s="18"/>
       <c r="CU17" s="18"/>
     </row>
-    <row r="18" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18" s="1"/>
       <c r="C18" s="8"/>
@@ -9765,7 +9771,7 @@
       <c r="CT18" s="18"/>
       <c r="CU18" s="18"/>
     </row>
-    <row r="19" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
       <c r="B19" s="1"/>
       <c r="C19" s="8"/>
@@ -9866,7 +9872,7 @@
       <c r="CT19" s="18"/>
       <c r="CU19" s="18"/>
     </row>
-    <row r="20" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
       <c r="B20" s="1"/>
       <c r="C20" s="8"/>
@@ -9967,7 +9973,7 @@
       <c r="CT20" s="18"/>
       <c r="CU20" s="18"/>
     </row>
-    <row r="21" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
       <c r="B21" s="1"/>
       <c r="C21" s="8"/>
@@ -10068,7 +10074,7 @@
       <c r="CT21" s="18"/>
       <c r="CU21" s="18"/>
     </row>
-    <row r="22" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
       <c r="B22" s="1"/>
       <c r="C22" s="8"/>
@@ -10169,7 +10175,7 @@
       <c r="CT22" s="18"/>
       <c r="CU22" s="18"/>
     </row>
-    <row r="23" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
       <c r="B23" s="1"/>
       <c r="C23" s="8"/>
@@ -10270,7 +10276,7 @@
       <c r="CT23" s="18"/>
       <c r="CU23" s="18"/>
     </row>
-    <row r="24" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24" s="1"/>
       <c r="C24" s="8"/>
@@ -10371,7 +10377,7 @@
       <c r="CT24" s="18"/>
       <c r="CU24" s="18"/>
     </row>
-    <row r="25" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
       <c r="B25" s="1"/>
       <c r="C25" s="8"/>
@@ -10472,7 +10478,7 @@
       <c r="CT25" s="18"/>
       <c r="CU25" s="18"/>
     </row>
-    <row r="26" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="B26" s="1"/>
       <c r="C26" s="8"/>
@@ -10573,7 +10579,7 @@
       <c r="CT26" s="18"/>
       <c r="CU26" s="18"/>
     </row>
-    <row r="27" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
       <c r="B27" s="1"/>
       <c r="C27" s="8"/>
@@ -10674,7 +10680,7 @@
       <c r="CT27" s="18"/>
       <c r="CU27" s="18"/>
     </row>
-    <row r="28" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
       <c r="B28" s="1"/>
       <c r="C28" s="8"/>
@@ -10775,7 +10781,7 @@
       <c r="CT28" s="18"/>
       <c r="CU28" s="18"/>
     </row>
-    <row r="29" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
       <c r="B29" s="1"/>
       <c r="C29" s="8"/>
@@ -10876,87 +10882,87 @@
       <c r="CT29" s="18"/>
       <c r="CU29" s="18"/>
     </row>
-    <row r="30" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B30" s="31"/>
       <c r="C30" s="32"/>
     </row>
-    <row r="31" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B31" s="31"/>
       <c r="C31" s="32"/>
     </row>
-    <row r="32" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B32" s="31"/>
       <c r="C32" s="32"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="31"/>
       <c r="C33" s="32"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="31"/>
       <c r="C34" s="32"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="31"/>
       <c r="C35" s="32"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="31"/>
       <c r="C36" s="32"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="31"/>
       <c r="C37" s="32"/>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="31"/>
       <c r="C38" s="32"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="31"/>
       <c r="C39" s="32"/>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="31"/>
       <c r="C40" s="32"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="31"/>
       <c r="C41" s="32"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="31"/>
       <c r="C42" s="32"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" s="31"/>
       <c r="C43" s="32"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" s="31"/>
       <c r="C44" s="32"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" s="31"/>
       <c r="C45" s="32"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" s="31"/>
       <c r="C46" s="32"/>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" s="31"/>
       <c r="C47" s="32"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" s="31"/>
       <c r="C48" s="32"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="31"/>
       <c r="C49" s="32"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="31"/>
       <c r="C50" s="32"/>
     </row>
@@ -10971,19 +10977,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef">
+        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain">
           <controlPr print="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>12700</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:colOff>12700</xdr:colOff>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -10991,7 +10997,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8193" r:id="rId4" name="SetDateTimeRef"/>
+        <control shapeId="8195" r:id="rId4" name="SetDateTimeMain"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11007,7 +11013,7 @@
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:colOff>12700</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
@@ -11021,19 +11027,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain">
+        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef">
           <controlPr print="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>12700</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
+                <xdr:colOff>12700</xdr:colOff>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -11041,7 +11047,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8195" r:id="rId8" name="SetDateTimeMain"/>
+        <control shapeId="8193" r:id="rId8" name="SetDateTimeRef"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>